<commit_message>
Add USs related to cluster domain "Biology & Botanic" [Biology]
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
+++ b/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
   <si>
     <t>Tabella 1</t>
   </si>
@@ -37,12 +37,18 @@
     <t>Biology &amp; Botanic</t>
   </si>
   <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>adversarial learning</t>
+  </si>
+  <si>
+    <t>As a bioinformatics scientist, I want to employ adversarial learning techniques to enhance the robustness of my deep learning models for predicting protein structures, so that I can improve accuracy in drug design applications.</t>
+  </si>
+  <si>
     <t>Plant Science</t>
   </si>
   <si>
-    <t>adversarial learning</t>
-  </si>
-  <si>
     <t>As a botanist, I want to apply adversarial learning techniques to enhance the robustness of my plant disease detection model against adversarial attacks, so that I can deploy it confidently in real-world agricultural settings.</t>
   </si>
   <si>
@@ -52,112 +58,169 @@
     <t>cnn</t>
   </si>
   <si>
+    <t>As a marine biologist, I want to utilize CNNs to classify underwater species based on sonar data, so that I can monitor biodiversity and assess the health of marine ecosystems.</t>
+  </si>
+  <si>
     <t>As a horticulturist, I want to employ CNNs to monitor plant growth in greenhouse environments by analyzing daily images, so that I can optimize growth conditions and predict harvest times more accurately.</t>
   </si>
   <si>
     <t>conversational agent</t>
   </si>
   <si>
+    <t>As a biology educator, I want to build a virtual tutor with NLP capabilities to provide personalized learning experiences for students studying evolutionary biology, so that they can better grasp complex concepts and improve their academic performance.</t>
+  </si>
+  <si>
     <t>As an agricultural consultant, I want to create a conversational agent capable of recommending optimal crop rotation strategies based on soil type, climate conditions, and previous crop history, to help farmers maximize yield and sustainability.</t>
   </si>
   <si>
     <t>decision tree</t>
   </si>
   <si>
+    <t>As a wildlife biologist, I want to employ decision tree models to analyze animal behavior data collected from GPS trackers, so that I can identify factors influencing migration patterns and habitat preferences of endangered species.</t>
+  </si>
+  <si>
     <t>As a plant breeder, I want to use decision trees to predict the genetic traits of hybrid plants based on parental characteristics, to accelerate the development of new plant varieties with desired traits such as disease resistance and yield potential.</t>
   </si>
   <si>
     <t>document classification</t>
   </si>
   <si>
+    <t>As a molecular biologist, I want to apply document classification techniques to classify scientific literature on gene expression studies into different experimental methodologies, so that I can extract relevant data and trends for meta-analysis and hypothesis generation.</t>
+  </si>
+  <si>
     <t>As a plant pathology expert, I want to use document classification to automatically classify and prioritize incoming reports of new plant diseases and outbreaks based on symptoms and geographic location, to expedite response strategies and prevent widespread crop losses.</t>
   </si>
   <si>
     <t>entity extraction</t>
   </si>
   <si>
+    <t>As a molecular biologist, I want to develop an entity extraction system to automatically identify gene names, protein functions, and mutation types from scientific literature, so that I can build comprehensive databases for genetic research and analysis.</t>
+  </si>
+  <si>
     <t>As an agroecologist, I want to build an entity extraction system that can extract agricultural practices and farming techniques mentioned in agricultural manuals and field reports, to analyze the impact of different farming methods on soil health and crop productivity in sustainable agriculture.</t>
   </si>
   <si>
     <t>feature selection</t>
   </si>
   <si>
+    <t>As a bioinformatics scientist, I want to apply feature selection techniques in machine learning to identify the most relevant genetic markers associated with cancer progression, so that I can develop biomarker panels for early detection and prognosis prediction.</t>
+  </si>
+  <si>
     <t>As a botanist, I want to employ feature selection methods to identify key morphological traits that distinguish invasive plant species from native ones, to support effective management strategies for controlling invasive species in natural habitats.</t>
   </si>
   <si>
     <t>imbalanced dataset</t>
   </si>
   <si>
+    <t>As a microbiologist, I want to develop a machine learning model to classify bacterial species from metagenomic data, despite the inherent imbalance in the dataset due to rare species, so that I can improve our ability to study microbial communities in diverse environments.</t>
+  </si>
+  <si>
     <t>As a plant disease researcher, I want to address class imbalance in disease occurrence data to develop a robust model for early detection of rare but devastating plant pathogens, to prevent widespread crop losses.</t>
   </si>
   <si>
     <t>k-nearest neighbor</t>
   </si>
   <si>
+    <t>As a genetics educator, I want to develop a machine learning model for extracting key genetic terms and concepts from educational materials, so that I can create customized learning resources and enhance student understanding of complex genetic principles.</t>
+  </si>
+  <si>
     <t>As a horticulturist, I want to develop a keyword extraction model to extract gardening tips and plant care advice from online forums and gardening blogs, such as soil preparation methods, pruning techniques, and seasonal planting tips, to provide personalized gardening recommendations.</t>
   </si>
   <si>
     <t>keyword extraction</t>
   </si>
   <si>
+    <t>As a bioinformatician, I want to implement k-Nearest Neighbor algorithms to classify gene expression profiles into different disease categories, so that I can identify potential biomarkers and therapeutic targets for precision medicine applications.</t>
+  </si>
+  <si>
     <t>As a plant ecologist, I want to use k-NN to predict plant species composition in new habitats based on similarity to existing vegetation plots, leveraging ecological data to assess biodiversity and habitat suitability for conservation planning.</t>
   </si>
   <si>
     <t>multi-label classification</t>
   </si>
   <si>
+    <t>As a bioinformatics scientist, I want to develop a multi-label classification model to predict the functions of uncharacterized proteins based on their amino acid sequences, so that I can annotate protein databases more comprehensively.</t>
+  </si>
+  <si>
     <t>As a plant biologist, I want to use multi-label classification techniques to categorize plant species based on their medicinal properties and biochemical compositions, facilitating the discovery of new pharmaceutical compounds from natural sources.</t>
   </si>
   <si>
     <t>neural network</t>
   </si>
   <si>
+    <t>As a genomics researcher, I want to train a neural network to predict gene expression levels based on genomic sequences and environmental factors, so that I can uncover regulatory mechanisms underlying gene function and disease susceptibility.</t>
+  </si>
+  <si>
     <t>As a plant physiologist, I want to implement a neural network for forecasting plant responses to climate change, incorporating physiological data on photosynthesis, water use efficiency, and stress tolerance, to guide adaptive agricultural strategies.</t>
   </si>
   <si>
     <t>random forest</t>
   </si>
   <si>
+    <t>As a pharmacologist, I aim to use random forest algorithms to predict drug response variability across patient populations using genomic and clinical data, so that I can tailor pharmacotherapy for better treatment outcomes.</t>
+  </si>
+  <si>
     <t>As a botanist, I want to employ random forest algorithms to classify plant species from leaf images, integrating features such as leaf shape, venation patterns, and texture, to assist in rapid species identification in field surveys.</t>
   </si>
   <si>
     <t>semantic similarity</t>
   </si>
   <si>
+    <t>As a molecular biologist, I want to use semantic similarity methods to compare biomedical ontologies and identify candidate genes associated with complex diseases, so that I can facilitate genetic research and drug development for personalized medicine.</t>
+  </si>
+  <si>
     <t>As a plant genetics researcher, I want to use semantic similarity techniques to analyze gene function annotations and biological pathways in plant genomes, to discover relationships between genetic traits and plant phenotypes.</t>
   </si>
   <si>
     <t>sentiment analysis</t>
   </si>
   <si>
+    <t>As a bioinformatics researcher, I want to apply sentiment analysis to analyze public perception and sentiment towards genetically modified organisms (GMOs) based on social media and survey data, so that I can understand public acceptance and inform policy decisions.</t>
+  </si>
+  <si>
     <t>As a botanist, I want to analyze public sentiment towards conservation efforts and policies related to endangered plant species, using sentiment analysis to gauge public awareness and support for conservation initiatives.</t>
   </si>
   <si>
     <t>speech to text</t>
   </si>
   <si>
+    <t>As a field biologist, I aim to use speech-to-text technology to record and transcribe field observations of animal behaviors and environmental conditions, so that I can create detailed field notes for biodiversity surveys and research publications.</t>
+  </si>
+  <si>
     <t>As a field researcher, I want to use speech to text technology to record observations and data on plant growth and phenology during field surveys, to streamline data collection processes and minimize errors.</t>
   </si>
   <si>
     <t>text categorization</t>
   </si>
   <si>
+    <t>As a bioinformatics researcher, I want to develop a text categorization model to classify scientific articles into categories such as genomics, proteomics, and bioinformatics, so that I can quickly access relevant literature for my research in molecular biology.</t>
+  </si>
+  <si>
     <t>As an agricultural researcher, I want to implement text categorization techniques to classify agricultural extension documents into categories such as crop management, pest control, soil health, and irrigation techniques, to provide targeted advice to farmers.</t>
   </si>
   <si>
     <t>unsupervised clustering</t>
   </si>
   <si>
+    <t>As a botanist, I aim to apply unsupervised clustering techniques to classify plant species based on morphological and genetic data, so that I can identify new species and understand plant biodiversity patterns.</t>
+  </si>
+  <si>
     <t>As a horticulturist, I want to cluster customer feedback and reviews on garden plants and products using unsupervised learning, to identify customer preferences and trends in gardening preferences, guiding product selection and marketing strategies.</t>
   </si>
   <si>
     <t>voice recognition</t>
   </si>
   <si>
+    <t>As a field biologist, I want to develop a voice recognition system to record and transcribe field observations of bird calls and other wildlife vocalizations, so that I can study biodiversity and animal behavior in natural habitats.</t>
+  </si>
+  <si>
     <t>As a field researcher, I want to develop a voice recognition system to verbally record observations on plant phenology and environmental conditions during field surveys, to streamline data collection processes and ensure accurate documentation.</t>
   </si>
   <si>
     <t>word embedding</t>
+  </si>
+  <si>
+    <t>As a molecular biologist, I want to use word embedding techniques to analyze biomedical literature and extract meaningful associations between gene names, protein functions, and disease pathways, so that I can identify novel targets for therapeutic interventions.</t>
   </si>
   <si>
     <t>As a botanist, I want to apply word embedding models to categorize and analyze botanical descriptions and taxonomic classifications of plant species, to improve consistency and accuracy in species identification and classification.</t>
@@ -193,7 +256,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +278,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -323,7 +392,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -355,9 +424,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -366,8 +444,14 @@
     <xf numFmtId="49" fontId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -389,6 +473,7 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ff00a1fe"/>
       <rgbColor rgb="ff56c1fe"/>
       <rgbColor rgb="ffffffff"/>
     </indexedColors>
@@ -1449,7 +1534,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:F22"/>
+  <dimension ref="A2:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1511,28 +1596,26 @@
       <c r="E3" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="F3" t="s" s="11">
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" ht="19" customHeight="1">
+      <c r="A4" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" ht="19" customHeight="1">
-      <c r="A4" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B4" s="7">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s" s="8">
-        <v>8</v>
-      </c>
       <c r="D4" t="s" s="9">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s" s="15">
         <v>12</v>
       </c>
-      <c r="E4" t="s" s="12">
+      <c r="F4" t="s" s="16">
         <v>13</v>
-      </c>
-      <c r="F4" t="s" s="13">
-        <v>11</v>
       </c>
     </row>
     <row r="5" ht="19" customHeight="1">
@@ -1545,34 +1628,32 @@
       <c r="C5" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D5" t="s" s="14">
+      <c r="D5" t="s" s="9">
         <v>14</v>
       </c>
-      <c r="E5" t="s" s="13">
+      <c r="E5" t="s" s="15">
         <v>15</v>
       </c>
-      <c r="F5" t="s" s="13">
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" ht="19" customHeight="1">
+      <c r="A6" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B6" s="13">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" ht="19" customHeight="1">
-      <c r="A6" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B6" s="7">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s" s="14">
+      <c r="D6" t="s" s="9">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s" s="15">
         <v>16</v>
       </c>
-      <c r="E6" t="s" s="13">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s" s="13">
-        <v>11</v>
+      <c r="F6" t="s" s="16">
+        <v>13</v>
       </c>
     </row>
     <row r="7" ht="19" customHeight="1">
@@ -1585,34 +1666,32 @@
       <c r="C7" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D7" t="s" s="14">
+      <c r="D7" t="s" s="18">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="E7" t="s" s="13">
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" ht="19" customHeight="1">
+      <c r="A8" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s" s="18">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s" s="16">
         <v>19</v>
       </c>
-      <c r="F7" t="s" s="13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" ht="19" customHeight="1">
-      <c r="A8" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s" s="14">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s" s="12">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s" s="13">
-        <v>11</v>
+      <c r="F8" t="s" s="16">
+        <v>13</v>
       </c>
     </row>
     <row r="9" ht="19" customHeight="1">
@@ -1625,34 +1704,32 @@
       <c r="C9" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D9" t="s" s="14">
+      <c r="D9" t="s" s="18">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s" s="16">
+        <v>21</v>
+      </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" ht="19" customHeight="1">
+      <c r="A10" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s" s="18">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s" s="16">
         <v>22</v>
       </c>
-      <c r="E9" t="s" s="13">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s" s="13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" ht="19" customHeight="1">
-      <c r="A10" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B10" s="7">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s" s="14">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s" s="13">
-        <v>25</v>
-      </c>
-      <c r="F10" t="s" s="13">
-        <v>11</v>
+      <c r="F10" t="s" s="16">
+        <v>13</v>
       </c>
     </row>
     <row r="11" ht="19" customHeight="1">
@@ -1665,34 +1742,32 @@
       <c r="C11" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D11" t="s" s="14">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s" s="13">
-        <v>27</v>
-      </c>
-      <c r="F11" t="s" s="13">
+      <c r="D11" t="s" s="18">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s" s="16">
+        <v>24</v>
+      </c>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" ht="19" customHeight="1">
+      <c r="A12" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" ht="19" customHeight="1">
-      <c r="A12" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s" s="14">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s" s="13">
-        <v>29</v>
-      </c>
-      <c r="F12" t="s" s="13">
-        <v>11</v>
+      <c r="D12" t="s" s="18">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s" s="16">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s" s="16">
+        <v>13</v>
       </c>
     </row>
     <row r="13" ht="19" customHeight="1">
@@ -1705,34 +1780,32 @@
       <c r="C13" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D13" t="s" s="14">
-        <v>30</v>
-      </c>
-      <c r="E13" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="F13" t="s" s="13">
+      <c r="D13" t="s" s="18">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s" s="16">
+        <v>27</v>
+      </c>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" ht="19" customHeight="1">
+      <c r="A14" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" ht="19" customHeight="1">
-      <c r="A14" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B14" s="7">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s" s="14">
-        <v>32</v>
-      </c>
-      <c r="E14" t="s" s="13">
-        <v>33</v>
-      </c>
-      <c r="F14" t="s" s="13">
-        <v>11</v>
+      <c r="D14" t="s" s="18">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s" s="15">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s" s="16">
+        <v>13</v>
       </c>
     </row>
     <row r="15" ht="19" customHeight="1">
@@ -1745,34 +1818,32 @@
       <c r="C15" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D15" t="s" s="14">
-        <v>34</v>
-      </c>
-      <c r="E15" t="s" s="13">
-        <v>35</v>
-      </c>
-      <c r="F15" t="s" s="13">
+      <c r="D15" t="s" s="18">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s" s="16">
+        <v>30</v>
+      </c>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" ht="19" customHeight="1">
+      <c r="A16" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B16" s="13">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" ht="19" customHeight="1">
-      <c r="A16" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B16" s="7">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s" s="14">
-        <v>36</v>
-      </c>
-      <c r="E16" t="s" s="13">
-        <v>37</v>
-      </c>
-      <c r="F16" t="s" s="13">
-        <v>11</v>
+      <c r="D16" t="s" s="18">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s" s="16">
+        <v>31</v>
+      </c>
+      <c r="F16" t="s" s="16">
+        <v>13</v>
       </c>
     </row>
     <row r="17" ht="19" customHeight="1">
@@ -1785,34 +1856,32 @@
       <c r="C17" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D17" t="s" s="14">
-        <v>38</v>
-      </c>
-      <c r="E17" t="s" s="13">
-        <v>39</v>
-      </c>
-      <c r="F17" t="s" s="13">
+      <c r="D17" t="s" s="18">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s" s="16">
+        <v>33</v>
+      </c>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" ht="19" customHeight="1">
+      <c r="A18" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B18" s="13">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" ht="19" customHeight="1">
-      <c r="A18" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B18" s="7">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s" s="14">
-        <v>40</v>
-      </c>
-      <c r="E18" t="s" s="13">
-        <v>41</v>
-      </c>
-      <c r="F18" t="s" s="13">
-        <v>11</v>
+      <c r="D18" t="s" s="18">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s" s="16">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s" s="16">
+        <v>13</v>
       </c>
     </row>
     <row r="19" ht="19" customHeight="1">
@@ -1825,34 +1894,32 @@
       <c r="C19" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D19" t="s" s="14">
-        <v>42</v>
-      </c>
-      <c r="E19" t="s" s="13">
-        <v>43</v>
-      </c>
-      <c r="F19" t="s" s="13">
+      <c r="D19" t="s" s="18">
+        <v>35</v>
+      </c>
+      <c r="E19" t="s" s="16">
+        <v>36</v>
+      </c>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" ht="19" customHeight="1">
+      <c r="A20" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B20" s="13">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" ht="19" customHeight="1">
-      <c r="A20" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B20" s="7">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s" s="14">
-        <v>44</v>
-      </c>
-      <c r="E20" t="s" s="13">
-        <v>45</v>
-      </c>
-      <c r="F20" t="s" s="13">
-        <v>11</v>
+      <c r="D20" t="s" s="18">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s" s="16">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s" s="16">
+        <v>13</v>
       </c>
     </row>
     <row r="21" ht="19" customHeight="1">
@@ -1865,34 +1932,412 @@
       <c r="C21" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D21" t="s" s="14">
+      <c r="D21" t="s" s="18">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s" s="15">
+        <v>39</v>
+      </c>
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" ht="19" customHeight="1">
+      <c r="A22" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B22" s="13">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s" s="18">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s" s="16">
+        <v>40</v>
+      </c>
+      <c r="F22" t="s" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" ht="19" customHeight="1">
+      <c r="A23" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="B23" s="7">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s" s="18">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s" s="15">
+        <v>42</v>
+      </c>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" ht="19" customHeight="1">
+      <c r="A24" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B24" s="13">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s" s="18">
+        <v>41</v>
+      </c>
+      <c r="E24" t="s" s="16">
+        <v>43</v>
+      </c>
+      <c r="F24" t="s" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" ht="19" customHeight="1">
+      <c r="A25" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="B25" s="7">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s" s="18">
+        <v>44</v>
+      </c>
+      <c r="E25" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="F25" s="17"/>
+    </row>
+    <row r="26" ht="19" customHeight="1">
+      <c r="A26" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B26" s="13">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s" s="18">
+        <v>44</v>
+      </c>
+      <c r="E26" t="s" s="16">
         <v>46</v>
       </c>
-      <c r="E21" t="s" s="13">
+      <c r="F26" t="s" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" ht="19" customHeight="1">
+      <c r="A27" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="B27" s="7">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s" s="18">
         <v>47</v>
       </c>
-      <c r="F21" t="s" s="13">
+      <c r="E27" t="s" s="16">
+        <v>48</v>
+      </c>
+      <c r="F27" s="17"/>
+    </row>
+    <row r="28" ht="19" customHeight="1">
+      <c r="A28" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B28" s="13">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" ht="19" customHeight="1">
-      <c r="A22" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B22" s="7">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s" s="8">
+      <c r="D28" t="s" s="18">
+        <v>47</v>
+      </c>
+      <c r="E28" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="F28" t="s" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" ht="19" customHeight="1">
+      <c r="A29" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D22" t="s" s="14">
-        <v>48</v>
-      </c>
-      <c r="E22" t="s" s="13">
-        <v>49</v>
-      </c>
-      <c r="F22" t="s" s="13">
+      <c r="D29" t="s" s="18">
+        <v>50</v>
+      </c>
+      <c r="E29" t="s" s="19">
+        <v>51</v>
+      </c>
+      <c r="F29" s="17"/>
+    </row>
+    <row r="30" ht="19" customHeight="1">
+      <c r="A30" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B30" s="13">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s" s="14">
         <v>11</v>
+      </c>
+      <c r="D30" t="s" s="18">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="F30" t="s" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" ht="19" customHeight="1">
+      <c r="A31" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s" s="18">
+        <v>53</v>
+      </c>
+      <c r="E31" t="s" s="16">
+        <v>54</v>
+      </c>
+      <c r="F31" s="17"/>
+    </row>
+    <row r="32" ht="19" customHeight="1">
+      <c r="A32" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B32" s="13">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s" s="18">
+        <v>53</v>
+      </c>
+      <c r="E32" t="s" s="16">
+        <v>55</v>
+      </c>
+      <c r="F32" t="s" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" ht="19" customHeight="1">
+      <c r="A33" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="B33" s="7">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s" s="18">
+        <v>56</v>
+      </c>
+      <c r="E33" t="s" s="16">
+        <v>57</v>
+      </c>
+      <c r="F33" s="17"/>
+    </row>
+    <row r="34" ht="19" customHeight="1">
+      <c r="A34" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B34" s="13">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s" s="18">
+        <v>56</v>
+      </c>
+      <c r="E34" t="s" s="16">
+        <v>58</v>
+      </c>
+      <c r="F34" t="s" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" ht="19" customHeight="1">
+      <c r="A35" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="B35" s="7">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s" s="18">
+        <v>59</v>
+      </c>
+      <c r="E35" t="s" s="16">
+        <v>60</v>
+      </c>
+      <c r="F35" s="17"/>
+    </row>
+    <row r="36" ht="19" customHeight="1">
+      <c r="A36" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B36" s="13">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s" s="18">
+        <v>59</v>
+      </c>
+      <c r="E36" t="s" s="16">
+        <v>61</v>
+      </c>
+      <c r="F36" t="s" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" ht="19" customHeight="1">
+      <c r="A37" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="B37" s="7">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s" s="18">
+        <v>62</v>
+      </c>
+      <c r="E37" t="s" s="16">
+        <v>63</v>
+      </c>
+      <c r="F37" s="17"/>
+    </row>
+    <row r="38" ht="19" customHeight="1">
+      <c r="A38" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B38" s="13">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s" s="18">
+        <v>62</v>
+      </c>
+      <c r="E38" t="s" s="16">
+        <v>64</v>
+      </c>
+      <c r="F38" t="s" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" ht="19" customHeight="1">
+      <c r="A39" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="B39" s="7">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s" s="18">
+        <v>65</v>
+      </c>
+      <c r="E39" t="s" s="16">
+        <v>66</v>
+      </c>
+      <c r="F39" s="17"/>
+    </row>
+    <row r="40" ht="19" customHeight="1">
+      <c r="A40" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B40" s="13">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s" s="18">
+        <v>65</v>
+      </c>
+      <c r="E40" t="s" s="16">
+        <v>67</v>
+      </c>
+      <c r="F40" t="s" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" ht="19" customHeight="1">
+      <c r="A41" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="B41" s="7">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s" s="18">
+        <v>68</v>
+      </c>
+      <c r="E41" t="s" s="16">
+        <v>69</v>
+      </c>
+      <c r="F41" s="17"/>
+    </row>
+    <row r="42" ht="19" customHeight="1">
+      <c r="A42" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B42" s="13">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s" s="18">
+        <v>68</v>
+      </c>
+      <c r="E42" t="s" s="16">
+        <v>70</v>
+      </c>
+      <c r="F42" t="s" s="16">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add USs related to cluster domain "Social and Urban Studies" [Demography]
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
+++ b/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
   <si>
     <t>Tabella 1</t>
   </si>
@@ -46,15 +46,15 @@
     <t>As a bioinformatics scientist, I want to employ adversarial learning techniques to enhance the robustness of my deep learning models for predicting protein structures, so that I can improve accuracy in drug design applications.</t>
   </si>
   <si>
+    <t>Domain_CoTPrompt</t>
+  </si>
+  <si>
     <t>Plant Science</t>
   </si>
   <si>
     <t>As a botanist, I want to apply adversarial learning techniques to enhance the robustness of my plant disease detection model against adversarial attacks, so that I can deploy it confidently in real-world agricultural settings.</t>
   </si>
   <si>
-    <t>Domain_CoTPrompt</t>
-  </si>
-  <si>
     <t>cnn</t>
   </si>
   <si>
@@ -224,6 +224,69 @@
   </si>
   <si>
     <t>As a botanist, I want to apply word embedding models to categorize and analyze botanical descriptions and taxonomic classifications of plant species, to improve consistency and accuracy in species identification and classification.</t>
+  </si>
+  <si>
+    <t>Social and Urban Studies</t>
+  </si>
+  <si>
+    <t>Demography</t>
+  </si>
+  <si>
+    <t>As a demographer, I want to apply adversarial learning techniques to detect and mitigate biases in census data, so that population statistics are more accurate and representative across diverse demographic groups.</t>
+  </si>
+  <si>
+    <t>As a demographer, I need to apply CNN models to analyze satellite imagery and identify changes in urban sprawl over time, helping me understand how demographic shifts affect city planning and development.</t>
+  </si>
+  <si>
+    <t>As a government official, I want to deploy a conversational agent that can interactively guide citizens through demographic surveys, ensuring accurate data collection and enhancing public engagement in demographic studies.</t>
+  </si>
+  <si>
+    <t>As a demography data analyst, I want to employ a decision tree algorithm to evaluate the impact of educational attainment levels on population growth rates across various regions, providing insights into educational policies and workforce planning initiatives.</t>
+  </si>
+  <si>
+    <t>As a demography researcher, I need a document classification model to automatically categorize research papers and reports into topics such as fertility rates, aging population trends, and migration patterns, facilitating literature review and data synthesis.</t>
+  </si>
+  <si>
+    <t>As a demography consultant, I need an entity extraction tool to extract key demographic indicators such as birth rates, mortality rates, and migration flows from international demographic databases and reports, facilitating comparative analysis across countries.</t>
+  </si>
+  <si>
+    <t>As a demography researcher, I need a feature selection algorithm to identify the most influential demographic variables affecting population density changes in urban areas, helping me prioritize factors for detailed analysis and policy recommendations.</t>
+  </si>
+  <si>
+    <t>As a demographer, I need to address class imbalance in demographic datasets when analyzing rare population characteristics such as extreme age groups or minority ethnicities, ensuring accurate representation and interpretation of demographic trends.</t>
+  </si>
+  <si>
+    <t>As a demographer, I need to apply k-Nearest Neighbor (k-NN) algorithm to identify similar demographic clusters across different regions based on socio-economic indicators, facilitating comparative demographic analysis and regional policy recommendations.</t>
+  </si>
+  <si>
+    <t>As a demography researcher, I need a keyword extraction algorithm to automatically identify and extract key demographic terms from large volumes of census data and demographic surveys, enabling efficient data summarization and trend analysis.</t>
+  </si>
+  <si>
+    <t>As a demography researcher, I need a multi-label classification model to classify demographic surveys into multiple categories such as age groups, income brackets, and educational levels simultaneously, enabling comprehensive analysis of socio-economic profiles within populations.</t>
+  </si>
+  <si>
+    <t>As a demographer, I aim to use a neural network to analyze complex demographic datasets and predict future population trends based on historical census data, enabling accurate forecasting for urban planning and policy-making.</t>
+  </si>
+  <si>
+    <t>As a demography researcher, I need to apply random forest algorithms to analyze demographic survey data and predict household income levels based on demographic variables such as age, education, and employment status, aiding in socio-economic research and policy planning.</t>
+  </si>
+  <si>
+    <t>As a demography educator, I want to create a semantic similarity tool to compare demographic theories and methodologies from different historical periods and cultural contexts, facilitating comparative demographic studies and theoretical analysis.</t>
+  </si>
+  <si>
+    <t>As a demography researcher, I need to perform sentiment analysis on social media data to understand public sentiment towards demographic policies and changes, helping to gauge public perception and support for policy initiatives.</t>
+  </si>
+  <si>
+    <t>As a demographer, I need a speech-to-text system to transcribe interviews and focus group discussions on demographic trends and population behaviors, facilitating qualitative data analysis and research insights.</t>
+  </si>
+  <si>
+    <t>As a demographer, I need to apply unsupervised clustering algorithms to analyze demographic survey data and identify distinct demographic segments within a population based on socio-economic characteristics, enabling targeted policy interventions and resource allocation strategies.</t>
+  </si>
+  <si>
+    <t>As a demography educator, I want to utilize voice recognition capabilities to transcribe lectures and seminars on demographic theories and methodologies, providing accessible resources for students and researchers in demography.</t>
+  </si>
+  <si>
+    <t>As a demography researcher, I need to apply word embedding techniques to analyze text data from demographic surveys and reports, identifying semantic relationships between demographic terms and concepts, enhancing data interpretation and insight generation.</t>
   </si>
 </sst>
 </file>
@@ -256,7 +319,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +347,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -392,7 +461,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -426,9 +495,6 @@
     <xf numFmtId="49" fontId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -444,14 +510,23 @@
     <xf numFmtId="49" fontId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,6 +551,7 @@
       <rgbColor rgb="ff00a1fe"/>
       <rgbColor rgb="ff56c1fe"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff72fce9"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1534,7 +1610,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:F42"/>
+  <dimension ref="A2:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1596,26 +1672,28 @@
       <c r="E3" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" t="s" s="10">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" ht="19" customHeight="1">
-      <c r="A4" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B4" s="13">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s" s="14">
-        <v>11</v>
+      <c r="A4" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="13">
+        <v>12</v>
       </c>
       <c r="D4" t="s" s="9">
         <v>9</v>
       </c>
-      <c r="E4" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s" s="16">
+      <c r="E4" t="s" s="14">
         <v>13</v>
+      </c>
+      <c r="F4" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="5" ht="19" customHeight="1">
@@ -1631,29 +1709,31 @@
       <c r="D5" t="s" s="9">
         <v>14</v>
       </c>
-      <c r="E5" t="s" s="15">
+      <c r="E5" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" ht="19" customHeight="1">
-      <c r="A6" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B6" s="13">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s" s="14">
-        <v>11</v>
+      <c r="A6" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s" s="13">
+        <v>12</v>
       </c>
       <c r="D6" t="s" s="9">
         <v>14</v>
       </c>
-      <c r="E6" t="s" s="15">
+      <c r="E6" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="F6" t="s" s="16">
-        <v>13</v>
+      <c r="F6" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="7" ht="19" customHeight="1">
@@ -1666,32 +1746,34 @@
       <c r="C7" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D7" t="s" s="18">
+      <c r="D7" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="E7" t="s" s="15">
+      <c r="E7" t="s" s="14">
         <v>18</v>
       </c>
-      <c r="F7" s="17"/>
+      <c r="F7" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" ht="19" customHeight="1">
-      <c r="A8" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B8" s="13">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s" s="18">
+      <c r="A8" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="E8" t="s" s="16">
+      <c r="E8" t="s" s="15">
         <v>19</v>
       </c>
-      <c r="F8" t="s" s="16">
-        <v>13</v>
+      <c r="F8" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="9" ht="19" customHeight="1">
@@ -1704,32 +1786,34 @@
       <c r="C9" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D9" t="s" s="18">
+      <c r="D9" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="E9" t="s" s="16">
+      <c r="E9" t="s" s="15">
         <v>21</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" ht="19" customHeight="1">
-      <c r="A10" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B10" s="13">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s" s="18">
+      <c r="A10" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="E10" t="s" s="16">
+      <c r="E10" t="s" s="15">
         <v>22</v>
       </c>
-      <c r="F10" t="s" s="16">
-        <v>13</v>
+      <c r="F10" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="11" ht="19" customHeight="1">
@@ -1742,32 +1826,34 @@
       <c r="C11" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D11" t="s" s="18">
+      <c r="D11" t="s" s="16">
         <v>23</v>
       </c>
-      <c r="E11" t="s" s="16">
+      <c r="E11" t="s" s="15">
         <v>24</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" ht="19" customHeight="1">
-      <c r="A12" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B12" s="13">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s" s="18">
+      <c r="A12" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s" s="16">
         <v>23</v>
       </c>
-      <c r="E12" t="s" s="16">
+      <c r="E12" t="s" s="15">
         <v>25</v>
       </c>
-      <c r="F12" t="s" s="16">
-        <v>13</v>
+      <c r="F12" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="13" ht="19" customHeight="1">
@@ -1780,32 +1866,34 @@
       <c r="C13" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D13" t="s" s="18">
+      <c r="D13" t="s" s="16">
         <v>26</v>
       </c>
-      <c r="E13" t="s" s="16">
+      <c r="E13" t="s" s="15">
         <v>27</v>
       </c>
-      <c r="F13" s="17"/>
+      <c r="F13" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" ht="19" customHeight="1">
-      <c r="A14" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B14" s="13">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s" s="18">
+      <c r="A14" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B14" s="12">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s" s="16">
         <v>26</v>
       </c>
-      <c r="E14" t="s" s="15">
+      <c r="E14" t="s" s="14">
         <v>28</v>
       </c>
-      <c r="F14" t="s" s="16">
-        <v>13</v>
+      <c r="F14" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="15" ht="19" customHeight="1">
@@ -1818,32 +1906,34 @@
       <c r="C15" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D15" t="s" s="18">
+      <c r="D15" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="E15" t="s" s="16">
+      <c r="E15" t="s" s="15">
         <v>30</v>
       </c>
-      <c r="F15" s="17"/>
+      <c r="F15" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" ht="19" customHeight="1">
-      <c r="A16" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B16" s="13">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D16" t="s" s="18">
+      <c r="A16" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B16" s="12">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="E16" t="s" s="16">
+      <c r="E16" t="s" s="15">
         <v>31</v>
       </c>
-      <c r="F16" t="s" s="16">
-        <v>13</v>
+      <c r="F16" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="17" ht="19" customHeight="1">
@@ -1856,32 +1946,34 @@
       <c r="C17" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D17" t="s" s="18">
+      <c r="D17" t="s" s="16">
         <v>32</v>
       </c>
-      <c r="E17" t="s" s="16">
+      <c r="E17" t="s" s="15">
         <v>33</v>
       </c>
-      <c r="F17" s="17"/>
+      <c r="F17" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="18" ht="19" customHeight="1">
-      <c r="A18" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B18" s="13">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D18" t="s" s="18">
+      <c r="A18" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B18" s="12">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s" s="16">
         <v>32</v>
       </c>
-      <c r="E18" t="s" s="16">
+      <c r="E18" t="s" s="15">
         <v>34</v>
       </c>
-      <c r="F18" t="s" s="16">
-        <v>13</v>
+      <c r="F18" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="19" ht="19" customHeight="1">
@@ -1894,32 +1986,34 @@
       <c r="C19" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D19" t="s" s="18">
+      <c r="D19" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E19" t="s" s="16">
+      <c r="E19" t="s" s="15">
         <v>36</v>
       </c>
-      <c r="F19" s="17"/>
+      <c r="F19" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="20" ht="19" customHeight="1">
-      <c r="A20" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B20" s="13">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s" s="18">
+      <c r="A20" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B20" s="12">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E20" t="s" s="16">
+      <c r="E20" t="s" s="15">
         <v>37</v>
       </c>
-      <c r="F20" t="s" s="16">
-        <v>13</v>
+      <c r="F20" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="21" ht="19" customHeight="1">
@@ -1932,32 +2026,34 @@
       <c r="C21" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D21" t="s" s="18">
+      <c r="D21" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E21" t="s" s="15">
+      <c r="E21" t="s" s="14">
         <v>39</v>
       </c>
-      <c r="F21" s="17"/>
+      <c r="F21" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="22" ht="19" customHeight="1">
-      <c r="A22" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B22" s="13">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D22" t="s" s="18">
+      <c r="A22" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B22" s="12">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E22" t="s" s="16">
+      <c r="E22" t="s" s="15">
         <v>40</v>
       </c>
-      <c r="F22" t="s" s="16">
-        <v>13</v>
+      <c r="F22" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="23" ht="19" customHeight="1">
@@ -1970,32 +2066,34 @@
       <c r="C23" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D23" t="s" s="18">
+      <c r="D23" t="s" s="16">
         <v>41</v>
       </c>
-      <c r="E23" t="s" s="15">
+      <c r="E23" t="s" s="14">
         <v>42</v>
       </c>
-      <c r="F23" s="17"/>
+      <c r="F23" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="24" ht="19" customHeight="1">
-      <c r="A24" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B24" s="13">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D24" t="s" s="18">
+      <c r="A24" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B24" s="12">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s" s="16">
         <v>41</v>
       </c>
-      <c r="E24" t="s" s="16">
+      <c r="E24" t="s" s="15">
         <v>43</v>
       </c>
-      <c r="F24" t="s" s="16">
-        <v>13</v>
+      <c r="F24" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="25" ht="19" customHeight="1">
@@ -2008,32 +2106,34 @@
       <c r="C25" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D25" t="s" s="18">
+      <c r="D25" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E25" t="s" s="16">
+      <c r="E25" t="s" s="15">
         <v>45</v>
       </c>
-      <c r="F25" s="17"/>
+      <c r="F25" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="26" ht="19" customHeight="1">
-      <c r="A26" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B26" s="13">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D26" t="s" s="18">
+      <c r="A26" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B26" s="12">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E26" t="s" s="16">
+      <c r="E26" t="s" s="15">
         <v>46</v>
       </c>
-      <c r="F26" t="s" s="16">
-        <v>13</v>
+      <c r="F26" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="27" ht="19" customHeight="1">
@@ -2046,32 +2146,34 @@
       <c r="C27" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D27" t="s" s="18">
+      <c r="D27" t="s" s="16">
         <v>47</v>
       </c>
-      <c r="E27" t="s" s="16">
+      <c r="E27" t="s" s="15">
         <v>48</v>
       </c>
-      <c r="F27" s="17"/>
+      <c r="F27" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="28" ht="19" customHeight="1">
-      <c r="A28" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B28" s="13">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D28" t="s" s="18">
+      <c r="A28" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B28" s="12">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s" s="16">
         <v>47</v>
       </c>
-      <c r="E28" t="s" s="16">
+      <c r="E28" t="s" s="15">
         <v>49</v>
       </c>
-      <c r="F28" t="s" s="16">
-        <v>13</v>
+      <c r="F28" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="29" ht="19" customHeight="1">
@@ -2084,32 +2186,34 @@
       <c r="C29" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D29" t="s" s="18">
+      <c r="D29" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="E29" t="s" s="19">
+      <c r="E29" t="s" s="17">
         <v>51</v>
       </c>
-      <c r="F29" s="17"/>
+      <c r="F29" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="30" ht="19" customHeight="1">
-      <c r="A30" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B30" s="13">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D30" t="s" s="18">
+      <c r="A30" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B30" s="12">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="E30" t="s" s="16">
+      <c r="E30" t="s" s="15">
         <v>52</v>
       </c>
-      <c r="F30" t="s" s="16">
-        <v>13</v>
+      <c r="F30" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="31" ht="19" customHeight="1">
@@ -2122,32 +2226,34 @@
       <c r="C31" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D31" t="s" s="18">
+      <c r="D31" t="s" s="16">
         <v>53</v>
       </c>
-      <c r="E31" t="s" s="16">
+      <c r="E31" t="s" s="15">
         <v>54</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" ht="19" customHeight="1">
-      <c r="A32" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B32" s="13">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D32" t="s" s="18">
+      <c r="A32" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B32" s="12">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s" s="16">
         <v>53</v>
       </c>
-      <c r="E32" t="s" s="16">
+      <c r="E32" t="s" s="15">
         <v>55</v>
       </c>
-      <c r="F32" t="s" s="16">
-        <v>13</v>
+      <c r="F32" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="33" ht="19" customHeight="1">
@@ -2160,32 +2266,34 @@
       <c r="C33" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D33" t="s" s="18">
+      <c r="D33" t="s" s="16">
         <v>56</v>
       </c>
-      <c r="E33" t="s" s="16">
+      <c r="E33" t="s" s="15">
         <v>57</v>
       </c>
-      <c r="F33" s="17"/>
+      <c r="F33" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="34" ht="19" customHeight="1">
-      <c r="A34" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B34" s="13">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D34" t="s" s="18">
+      <c r="A34" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B34" s="12">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s" s="16">
         <v>56</v>
       </c>
-      <c r="E34" t="s" s="16">
+      <c r="E34" t="s" s="15">
         <v>58</v>
       </c>
-      <c r="F34" t="s" s="16">
-        <v>13</v>
+      <c r="F34" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="35" ht="19" customHeight="1">
@@ -2198,32 +2306,34 @@
       <c r="C35" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D35" t="s" s="18">
+      <c r="D35" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E35" t="s" s="16">
+      <c r="E35" t="s" s="15">
         <v>60</v>
       </c>
-      <c r="F35" s="17"/>
+      <c r="F35" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="36" ht="19" customHeight="1">
-      <c r="A36" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B36" s="13">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D36" t="s" s="18">
+      <c r="A36" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B36" s="12">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E36" t="s" s="16">
+      <c r="E36" t="s" s="15">
         <v>61</v>
       </c>
-      <c r="F36" t="s" s="16">
-        <v>13</v>
+      <c r="F36" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="37" ht="19" customHeight="1">
@@ -2236,32 +2346,34 @@
       <c r="C37" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D37" t="s" s="18">
+      <c r="D37" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E37" t="s" s="16">
+      <c r="E37" t="s" s="15">
         <v>63</v>
       </c>
-      <c r="F37" s="17"/>
+      <c r="F37" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="38" ht="19" customHeight="1">
-      <c r="A38" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B38" s="13">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D38" t="s" s="18">
+      <c r="A38" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B38" s="12">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E38" t="s" s="16">
+      <c r="E38" t="s" s="15">
         <v>64</v>
       </c>
-      <c r="F38" t="s" s="16">
-        <v>13</v>
+      <c r="F38" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="39" ht="19" customHeight="1">
@@ -2274,32 +2386,34 @@
       <c r="C39" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D39" t="s" s="18">
+      <c r="D39" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E39" t="s" s="16">
+      <c r="E39" t="s" s="15">
         <v>66</v>
       </c>
-      <c r="F39" s="17"/>
+      <c r="F39" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="40" ht="19" customHeight="1">
-      <c r="A40" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B40" s="13">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D40" t="s" s="18">
+      <c r="A40" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B40" s="12">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E40" t="s" s="16">
+      <c r="E40" t="s" s="15">
         <v>67</v>
       </c>
-      <c r="F40" t="s" s="16">
-        <v>13</v>
+      <c r="F40" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="41" ht="19" customHeight="1">
@@ -2312,32 +2426,432 @@
       <c r="C41" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D41" t="s" s="18">
+      <c r="D41" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E41" t="s" s="16">
+      <c r="E41" t="s" s="15">
         <v>69</v>
       </c>
-      <c r="F41" s="17"/>
+      <c r="F41" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="42" ht="19" customHeight="1">
-      <c r="A42" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B42" s="13">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="D42" t="s" s="18">
+      <c r="A42" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="B42" s="12">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E42" t="s" s="16">
+      <c r="E42" t="s" s="15">
         <v>70</v>
       </c>
-      <c r="F42" t="s" s="16">
-        <v>13</v>
+      <c r="F42" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" ht="19" customHeight="1">
+      <c r="A43" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B43" s="19">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D43" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s" s="15">
+        <v>73</v>
+      </c>
+      <c r="F43" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" ht="19" customHeight="1">
+      <c r="A44" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B44" s="19">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D44" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E44" t="s" s="15">
+        <v>74</v>
+      </c>
+      <c r="F44" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" ht="19" customHeight="1">
+      <c r="A45" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B45" s="19">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D45" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E45" t="s" s="15">
+        <v>75</v>
+      </c>
+      <c r="F45" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" ht="19" customHeight="1">
+      <c r="A46" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B46" s="19">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D46" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="E46" t="s" s="17">
+        <v>76</v>
+      </c>
+      <c r="F46" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" ht="19" customHeight="1">
+      <c r="A47" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B47" s="19">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D47" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="E47" t="s" s="14">
+        <v>77</v>
+      </c>
+      <c r="F47" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" ht="19" customHeight="1">
+      <c r="A48" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B48" s="19">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D48" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E48" t="s" s="14">
+        <v>78</v>
+      </c>
+      <c r="F48" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" ht="19" customHeight="1">
+      <c r="A49" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B49" s="19">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D49" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E49" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="F49" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" ht="19" customHeight="1">
+      <c r="A50" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B50" s="19">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D50" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E50" t="s" s="15">
+        <v>80</v>
+      </c>
+      <c r="F50" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" ht="19" customHeight="1">
+      <c r="A51" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B51" s="19">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D51" t="s" s="16">
+        <v>35</v>
+      </c>
+      <c r="E51" t="s" s="14">
+        <v>81</v>
+      </c>
+      <c r="F51" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" ht="19" customHeight="1">
+      <c r="A52" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B52" s="19">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D52" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="E52" t="s" s="15">
+        <v>82</v>
+      </c>
+      <c r="F52" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" ht="19" customHeight="1">
+      <c r="A53" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B53" s="19">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D53" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E53" t="s" s="15">
+        <v>83</v>
+      </c>
+      <c r="F53" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" ht="19" customHeight="1">
+      <c r="A54" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B54" s="19">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D54" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="E54" t="s" s="15">
+        <v>84</v>
+      </c>
+      <c r="F54" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" ht="19" customHeight="1">
+      <c r="A55" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B55" s="19">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D55" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E55" t="s" s="15">
+        <v>85</v>
+      </c>
+      <c r="F55" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" ht="19" customHeight="1">
+      <c r="A56" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B56" s="19">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D56" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E56" t="s" s="17">
+        <v>86</v>
+      </c>
+      <c r="F56" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" ht="19" customHeight="1">
+      <c r="A57" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B57" s="19">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D57" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E57" t="s" s="14">
+        <v>87</v>
+      </c>
+      <c r="F57" s="21"/>
+    </row>
+    <row r="58" ht="19" customHeight="1">
+      <c r="A58" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B58" s="19">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D58" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E58" t="s" s="15">
+        <v>87</v>
+      </c>
+      <c r="F58" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" ht="19" customHeight="1">
+      <c r="A59" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B59" s="19">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D59" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E59" t="s" s="15">
+        <v>88</v>
+      </c>
+      <c r="F59" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" ht="19" customHeight="1">
+      <c r="A60" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B60" s="19">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D60" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E60" t="s" s="15">
+        <v>89</v>
+      </c>
+      <c r="F60" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" ht="19" customHeight="1">
+      <c r="A61" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B61" s="19">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D61" t="s" s="16">
+        <v>65</v>
+      </c>
+      <c r="E61" t="s" s="15">
+        <v>90</v>
+      </c>
+      <c r="F61" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" ht="19" customHeight="1">
+      <c r="A62" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B62" s="19">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D62" t="s" s="16">
+        <v>68</v>
+      </c>
+      <c r="E62" t="s" s="15">
+        <v>91</v>
+      </c>
+      <c r="F62" t="s" s="15">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add USs related to cluster domain "Social and Urban Studies" [Education]
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
+++ b/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
   <si>
     <t>Tabella 1</t>
   </si>
@@ -235,58 +235,121 @@
     <t>As a demographer, I want to apply adversarial learning techniques to detect and mitigate biases in census data, so that population statistics are more accurate and representative across diverse demographic groups.</t>
   </si>
   <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>As an AI engineer working with educational chatbots, I want to implement adversarial examples to improve the resilience of natural language understanding models, so that I can enhance the quality of student interactions.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply CNN models to analyze satellite imagery and identify changes in urban sprawl over time, helping me understand how demographic shifts affect city planning and development.</t>
   </si>
   <si>
+    <t>As a teacher, I want to employ CNNs to detect facial expressions of students during lessons, so that I can gauge their engagement and adjust my teaching approach accordingly.</t>
+  </si>
+  <si>
     <t>As a government official, I want to deploy a conversational agent that can interactively guide citizens through demographic surveys, ensuring accurate data collection and enhancing public engagement in demographic studies.</t>
   </si>
   <si>
+    <t>As a language instructor, I want to develop a conversational agent powered by natural language processing to provide real-time feedback and personalized language practice for students, so that I can enhance their language learning experience.</t>
+  </si>
+  <si>
     <t>As a demography data analyst, I want to employ a decision tree algorithm to evaluate the impact of educational attainment levels on population growth rates across various regions, providing insights into educational policies and workforce planning initiatives.</t>
   </si>
   <si>
+    <t>As a school principal, I want to implement a decision tree model to predict student dropout risk factors based on attendance, behavior, and academic performance data, so that I can intervene early and prevent dropouts.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a document classification model to automatically categorize research papers and reports into topics such as fertility rates, aging population trends, and migration patterns, facilitating literature review and data synthesis.</t>
   </si>
   <si>
+    <t>As a student counselor, I want to develop a document classification model to automatically tag and categorize student essays and reports based on academic performance indicators, so that I can provide targeted guidance and support.</t>
+  </si>
+  <si>
     <t>As a demography consultant, I need an entity extraction tool to extract key demographic indicators such as birth rates, mortality rates, and migration flows from international demographic databases and reports, facilitating comparative analysis across countries.</t>
   </si>
   <si>
+    <t>As a language teacher, I want to implement entity extraction algorithms to automatically extract and classify vocabulary terms and grammatical structures from student texts and exercises, so that I can provide personalized feedback and targeted language learning support.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a feature selection algorithm to identify the most influential demographic variables affecting population density changes in urban areas, helping me prioritize factors for detailed analysis and policy recommendations.</t>
   </si>
   <si>
+    <t>As a data analyst in education, I want to perform feature selection on student performance data to identify the most influential factors affecting academic outcomes, so that I can create targeted intervention strategies.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to address class imbalance in demographic datasets when analyzing rare population characteristics such as extreme age groups or minority ethnicities, ensuring accurate representation and interpretation of demographic trends.</t>
   </si>
   <si>
+    <t>As an educational researcher, I want to develop a predictive model for identifying gifted students in underrepresented populations using machine learning methods suitable for imbalanced datasets, so that I can support inclusive educational practices and talent development.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply k-Nearest Neighbor (k-NN) algorithm to identify similar demographic clusters across different regions based on socio-economic indicators, facilitating comparative demographic analysis and regional policy recommendations.</t>
   </si>
   <si>
+    <t>As a teacher, I want to integrate a keyword extraction algorithm into classroom discussion forums to automatically highlight and categorize student-generated ideas and discussions based on relevant educational topics, so that I can facilitate meaningful class discussions.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a keyword extraction algorithm to automatically identify and extract key demographic terms from large volumes of census data and demographic surveys, enabling efficient data summarization and trend analysis.</t>
   </si>
   <si>
+    <t>As a special education teacher, I want to employ a k-NN model to identify similarities in learning profiles among students with disabilities, so that I can group them effectively for personalized educational interventions and support.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a multi-label classification model to classify demographic surveys into multiple categories such as age groups, income brackets, and educational levels simultaneously, enabling comprehensive analysis of socio-economic profiles within populations.</t>
   </si>
   <si>
+    <t>As a school counselor, I want to develop a multi-label classification model to predict various behavioral and academic outcomes for students based on their historical data, so that I can implement targeted intervention plans.</t>
+  </si>
+  <si>
     <t>As a demographer, I aim to use a neural network to analyze complex demographic datasets and predict future population trends based on historical census data, enabling accurate forecasting for urban planning and policy-making.</t>
   </si>
   <si>
+    <t>As a teacher, I want to leverage neural networks to create predictive models that forecast student engagement levels and academic performance trends over time, so that I can proactively adjust my teaching strategies and classroom activities.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to apply random forest algorithms to analyze demographic survey data and predict household income levels based on demographic variables such as age, education, and employment status, aiding in socio-economic research and policy planning.</t>
   </si>
   <si>
+    <t>As a school administrator, I want to implement a random forest model to analyze student attendance records, academic performance metrics, and behavioral data to identify patterns that predict student dropout risk, so that I can intervene early and improve retention rates.</t>
+  </si>
+  <si>
     <t>As a demography educator, I want to create a semantic similarity tool to compare demographic theories and methodologies from different historical periods and cultural contexts, facilitating comparative demographic studies and theoretical analysis.</t>
   </si>
   <si>
+    <t>As a language teacher, I want to develop a semantic similarity model using natural language processing to assess the similarity of student essays and provide feedback on content and language usage, so that I can support their writing development effectively.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to perform sentiment analysis on social media data to understand public sentiment towards demographic policies and changes, helping to gauge public perception and support for policy initiatives.</t>
   </si>
   <si>
+    <t>As a teacher, I want to use sentiment analysis to analyze student responses in classroom discussion forums and assignments to understand their emotional responses to learning topics and identify areas of confusion or interest, so that I can adjust my teaching approach accordingly.</t>
+  </si>
+  <si>
+    <t>As a special education teacher, I want to utilize speech-to-text tools to convert spoken responses from students with speech disabilities into written text, so that I can facilitate their participation in classroom discussions and assessments.</t>
+  </si>
+  <si>
     <t>As a demographer, I need a speech-to-text system to transcribe interviews and focus group discussions on demographic trends and population behaviors, facilitating qualitative data analysis and research insights.</t>
   </si>
   <si>
+    <t>As an educational researcher, I want to apply text categorization models to analyze student essays and assignments based on content themes and learning outcomes, so that I can gain insights into student performance and learning patterns.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply unsupervised clustering algorithms to analyze demographic survey data and identify distinct demographic segments within a population based on socio-economic characteristics, enabling targeted policy interventions and resource allocation strategies.</t>
   </si>
   <si>
+    <t>As a teacher, I want to use unsupervised clustering algorithms to group student collaboration data in group projects and assignments to identify effective team dynamics and collaboration patterns, so that I can provide feedback and support for collaborative learning.</t>
+  </si>
+  <si>
     <t>As a demography educator, I want to utilize voice recognition capabilities to transcribe lectures and seminars on demographic theories and methodologies, providing accessible resources for students and researchers in demography.</t>
   </si>
   <si>
+    <t>As an educational researcher, I want to develop a voice recognition model to analyze teacher-student interactions in classrooms to measure engagement levels and identify effective teaching strategies, so that I can improve classroom dynamics and learning outcomes.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to apply word embedding techniques to analyze text data from demographic surveys and reports, identifying semantic relationships between demographic terms and concepts, enhancing data interpretation and insight generation.</t>
+  </si>
+  <si>
+    <t>As a language instructor, I want to utilize word embedding algorithms to create semantic maps of vocabulary and grammar structures to visualize language acquisition progress among students, so that I can tailor language lessons more effectively.</t>
   </si>
 </sst>
 </file>
@@ -319,7 +382,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +416,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -461,7 +530,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -525,6 +594,15 @@
     <xf numFmtId="49" fontId="3" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -552,6 +630,7 @@
       <rgbColor rgb="ff56c1fe"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff72fce9"/>
+      <rgbColor rgb="ff16e6cf"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1610,7 +1689,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:F62"/>
+  <dimension ref="A2:F82"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2477,24 +2556,22 @@
       </c>
     </row>
     <row r="44" ht="19" customHeight="1">
-      <c r="A44" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B44" s="19">
-        <v>7</v>
-      </c>
-      <c r="C44" t="s" s="20">
-        <v>72</v>
+      <c r="A44" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B44" s="22">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D44" t="s" s="16">
-        <v>14</v>
-      </c>
-      <c r="E44" t="s" s="15">
-        <v>74</v>
-      </c>
-      <c r="F44" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E44" t="s" s="14">
+        <v>75</v>
+      </c>
+      <c r="F44" s="24"/>
     </row>
     <row r="45" ht="19" customHeight="1">
       <c r="A45" t="s" s="18">
@@ -2507,34 +2584,32 @@
         <v>72</v>
       </c>
       <c r="D45" t="s" s="16">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E45" t="s" s="15">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F45" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="46" ht="19" customHeight="1">
-      <c r="A46" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B46" s="19">
-        <v>7</v>
-      </c>
-      <c r="C46" t="s" s="20">
-        <v>72</v>
+      <c r="A46" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B46" s="22">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D46" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E46" t="s" s="17">
-        <v>76</v>
-      </c>
-      <c r="F46" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E46" t="s" s="15">
+        <v>77</v>
+      </c>
+      <c r="F46" s="24"/>
     </row>
     <row r="47" ht="19" customHeight="1">
       <c r="A47" t="s" s="18">
@@ -2547,34 +2622,32 @@
         <v>72</v>
       </c>
       <c r="D47" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E47" t="s" s="14">
-        <v>77</v>
+        <v>17</v>
+      </c>
+      <c r="E47" t="s" s="15">
+        <v>78</v>
       </c>
       <c r="F47" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="48" ht="19" customHeight="1">
-      <c r="A48" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B48" s="19">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s" s="20">
-        <v>72</v>
+      <c r="A48" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B48" s="22">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D48" t="s" s="16">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E48" t="s" s="14">
-        <v>78</v>
-      </c>
-      <c r="F48" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="F48" s="24"/>
     </row>
     <row r="49" ht="19" customHeight="1">
       <c r="A49" t="s" s="18">
@@ -2587,34 +2660,32 @@
         <v>72</v>
       </c>
       <c r="D49" t="s" s="16">
-        <v>29</v>
-      </c>
-      <c r="E49" t="s" s="15">
-        <v>79</v>
+        <v>20</v>
+      </c>
+      <c r="E49" t="s" s="17">
+        <v>80</v>
       </c>
       <c r="F49" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="50" ht="19" customHeight="1">
-      <c r="A50" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B50" s="19">
-        <v>7</v>
-      </c>
-      <c r="C50" t="s" s="20">
-        <v>72</v>
+      <c r="A50" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B50" s="22">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D50" t="s" s="16">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E50" t="s" s="15">
-        <v>80</v>
-      </c>
-      <c r="F50" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="F50" s="24"/>
     </row>
     <row r="51" ht="19" customHeight="1">
       <c r="A51" t="s" s="18">
@@ -2627,34 +2698,32 @@
         <v>72</v>
       </c>
       <c r="D51" t="s" s="16">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E51" t="s" s="14">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F51" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="52" ht="19" customHeight="1">
-      <c r="A52" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B52" s="19">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s" s="20">
-        <v>72</v>
+      <c r="A52" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B52" s="22">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D52" t="s" s="16">
-        <v>38</v>
-      </c>
-      <c r="E52" t="s" s="15">
-        <v>82</v>
-      </c>
-      <c r="F52" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E52" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="F52" s="24"/>
     </row>
     <row r="53" ht="19" customHeight="1">
       <c r="A53" t="s" s="18">
@@ -2667,34 +2736,32 @@
         <v>72</v>
       </c>
       <c r="D53" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="E53" t="s" s="15">
-        <v>83</v>
+        <v>26</v>
+      </c>
+      <c r="E53" t="s" s="14">
+        <v>84</v>
       </c>
       <c r="F53" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="54" ht="19" customHeight="1">
-      <c r="A54" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B54" s="19">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s" s="20">
-        <v>72</v>
+      <c r="A54" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B54" s="22">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D54" t="s" s="16">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E54" t="s" s="15">
-        <v>84</v>
-      </c>
-      <c r="F54" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="F54" s="24"/>
     </row>
     <row r="55" ht="19" customHeight="1">
       <c r="A55" t="s" s="18">
@@ -2707,34 +2774,32 @@
         <v>72</v>
       </c>
       <c r="D55" t="s" s="16">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E55" t="s" s="15">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F55" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="56" ht="19" customHeight="1">
-      <c r="A56" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B56" s="19">
-        <v>7</v>
-      </c>
-      <c r="C56" t="s" s="20">
-        <v>72</v>
+      <c r="A56" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B56" s="22">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D56" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E56" t="s" s="17">
-        <v>86</v>
-      </c>
-      <c r="F56" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E56" t="s" s="14">
+        <v>87</v>
+      </c>
+      <c r="F56" s="24"/>
     </row>
     <row r="57" ht="19" customHeight="1">
       <c r="A57" t="s" s="18">
@@ -2747,32 +2812,32 @@
         <v>72</v>
       </c>
       <c r="D57" t="s" s="16">
-        <v>53</v>
-      </c>
-      <c r="E57" t="s" s="14">
-        <v>87</v>
-      </c>
-      <c r="F57" s="21"/>
+        <v>32</v>
+      </c>
+      <c r="E57" t="s" s="15">
+        <v>88</v>
+      </c>
+      <c r="F57" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="58" ht="19" customHeight="1">
-      <c r="A58" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B58" s="19">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s" s="20">
-        <v>72</v>
+      <c r="A58" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B58" s="22">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D58" t="s" s="16">
-        <v>56</v>
-      </c>
-      <c r="E58" t="s" s="15">
-        <v>87</v>
-      </c>
-      <c r="F58" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E58" t="s" s="17">
+        <v>89</v>
+      </c>
+      <c r="F58" s="24"/>
     </row>
     <row r="59" ht="19" customHeight="1">
       <c r="A59" t="s" s="18">
@@ -2785,34 +2850,32 @@
         <v>72</v>
       </c>
       <c r="D59" t="s" s="16">
-        <v>59</v>
-      </c>
-      <c r="E59" t="s" s="15">
-        <v>88</v>
+        <v>35</v>
+      </c>
+      <c r="E59" t="s" s="14">
+        <v>90</v>
       </c>
       <c r="F59" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="60" ht="19" customHeight="1">
-      <c r="A60" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B60" s="19">
-        <v>7</v>
-      </c>
-      <c r="C60" t="s" s="20">
-        <v>72</v>
+      <c r="A60" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B60" s="22">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D60" t="s" s="16">
-        <v>62</v>
-      </c>
-      <c r="E60" t="s" s="15">
-        <v>89</v>
-      </c>
-      <c r="F60" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E60" t="s" s="14">
+        <v>91</v>
+      </c>
+      <c r="F60" s="24"/>
     </row>
     <row r="61" ht="19" customHeight="1">
       <c r="A61" t="s" s="18">
@@ -2825,34 +2888,410 @@
         <v>72</v>
       </c>
       <c r="D61" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="E61" t="s" s="15">
+        <v>92</v>
+      </c>
+      <c r="F61" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" ht="19" customHeight="1">
+      <c r="A62" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B62" s="22">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D62" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="E62" t="s" s="15">
+        <v>93</v>
+      </c>
+      <c r="F62" s="24"/>
+    </row>
+    <row r="63" ht="19" customHeight="1">
+      <c r="A63" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B63" s="19">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D63" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E63" t="s" s="15">
+        <v>94</v>
+      </c>
+      <c r="F63" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" ht="19" customHeight="1">
+      <c r="A64" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B64" s="22">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D64" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E64" t="s" s="14">
+        <v>95</v>
+      </c>
+      <c r="F64" s="24"/>
+    </row>
+    <row r="65" ht="19" customHeight="1">
+      <c r="A65" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B65" s="19">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D65" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="E65" t="s" s="15">
+        <v>96</v>
+      </c>
+      <c r="F65" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" ht="19" customHeight="1">
+      <c r="A66" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B66" s="22">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D66" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="E66" t="s" s="14">
+        <v>97</v>
+      </c>
+      <c r="F66" s="24"/>
+    </row>
+    <row r="67" ht="19" customHeight="1">
+      <c r="A67" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B67" s="19">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D67" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E67" t="s" s="15">
+        <v>98</v>
+      </c>
+      <c r="F67" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" ht="19" customHeight="1">
+      <c r="A68" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B68" s="22">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D68" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E68" t="s" s="14">
+        <v>99</v>
+      </c>
+      <c r="F68" s="24"/>
+    </row>
+    <row r="69" ht="19" customHeight="1">
+      <c r="A69" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B69" s="19">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D69" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E69" t="s" s="17">
+        <v>100</v>
+      </c>
+      <c r="F69" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" ht="19" customHeight="1">
+      <c r="A70" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B70" s="22">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D70" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E70" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="F70" s="24"/>
+    </row>
+    <row r="71" ht="19" customHeight="1">
+      <c r="A71" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B71" s="19">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D71" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E71" t="s" s="14">
+        <v>102</v>
+      </c>
+      <c r="F71" s="24"/>
+    </row>
+    <row r="72" ht="19" customHeight="1">
+      <c r="A72" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B72" s="22">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D72" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E72" t="s" s="14">
+        <v>103</v>
+      </c>
+      <c r="F72" s="24"/>
+    </row>
+    <row r="73" ht="19" customHeight="1">
+      <c r="A73" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B73" s="19">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D73" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E73" t="s" s="15">
+        <v>102</v>
+      </c>
+      <c r="F73" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" ht="19" customHeight="1">
+      <c r="A74" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B74" s="22">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D74" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E74" t="s" s="14">
+        <v>104</v>
+      </c>
+      <c r="F74" s="24"/>
+    </row>
+    <row r="75" ht="19" customHeight="1">
+      <c r="A75" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B75" s="19">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D75" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E75" t="s" s="15">
+        <v>105</v>
+      </c>
+      <c r="F75" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" ht="19" customHeight="1">
+      <c r="A76" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B76" s="22">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D76" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E76" t="s" s="14">
+        <v>106</v>
+      </c>
+      <c r="F76" s="24"/>
+    </row>
+    <row r="77" ht="19" customHeight="1">
+      <c r="A77" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B77" s="19">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D77" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E77" t="s" s="15">
+        <v>107</v>
+      </c>
+      <c r="F77" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" ht="19" customHeight="1">
+      <c r="A78" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B78" s="22">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D78" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E78" t="s" s="14">
+        <v>108</v>
+      </c>
+      <c r="F78" s="24"/>
+    </row>
+    <row r="79" ht="19" customHeight="1">
+      <c r="A79" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B79" s="19">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D79" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E61" t="s" s="15">
-        <v>90</v>
-      </c>
-      <c r="F61" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" ht="19" customHeight="1">
-      <c r="A62" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B62" s="19">
-        <v>7</v>
-      </c>
-      <c r="C62" t="s" s="20">
+      <c r="E79" t="s" s="15">
+        <v>109</v>
+      </c>
+      <c r="F79" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" ht="19" customHeight="1">
+      <c r="A80" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B80" s="22">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D80" t="s" s="16">
+        <v>65</v>
+      </c>
+      <c r="E80" t="s" s="14">
+        <v>110</v>
+      </c>
+      <c r="F80" s="24"/>
+    </row>
+    <row r="81" ht="19" customHeight="1">
+      <c r="A81" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B81" s="19">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D62" t="s" s="16">
+      <c r="D81" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E62" t="s" s="15">
-        <v>91</v>
-      </c>
-      <c r="F62" t="s" s="15">
-        <v>11</v>
-      </c>
+      <c r="E81" t="s" s="15">
+        <v>111</v>
+      </c>
+      <c r="F81" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" ht="19" customHeight="1">
+      <c r="A82" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B82" s="22">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D82" t="s" s="16">
+        <v>68</v>
+      </c>
+      <c r="E82" t="s" s="14">
+        <v>112</v>
+      </c>
+      <c r="F82" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add USs related to cluster domain "Social and Urban Studies" [Social Media]
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
+++ b/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
   <si>
     <t>Tabella 1</t>
   </si>
@@ -241,115 +241,178 @@
     <t>As an AI engineer working with educational chatbots, I want to implement adversarial examples to improve the resilience of natural language understanding models, so that I can enhance the quality of student interactions.</t>
   </si>
   <si>
+    <t>Social Media</t>
+  </si>
+  <si>
+    <t>As a social media content moderator, I want to employ adversarial learning techniques to automatically detect and filter out hate speech in user comments, in order to create a safer and more inclusive online community.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply CNN models to analyze satellite imagery and identify changes in urban sprawl over time, helping me understand how demographic shifts affect city planning and development.</t>
   </si>
   <si>
     <t>As a teacher, I want to employ CNNs to detect facial expressions of students during lessons, so that I can gauge their engagement and adjust my teaching approach accordingly.</t>
   </si>
   <si>
+    <t>As a social media trend analyst, I want to use CNN models to analyze image content across posts and identify emerging trends or viral content early, so that I can advise brands on timely marketing strategies.</t>
+  </si>
+  <si>
     <t>As a government official, I want to deploy a conversational agent that can interactively guide citizens through demographic surveys, ensuring accurate data collection and enhancing public engagement in demographic studies.</t>
   </si>
   <si>
     <t>As a language instructor, I want to develop a conversational agent powered by natural language processing to provide real-time feedback and personalized language practice for students, so that I can enhance their language learning experience.</t>
   </si>
   <si>
+    <t>As a social media marketer, I want to develop a chatbot using NLP techniques to conduct surveys and gather feedback from followers about their preferences and opinions on our brand's content, to inform future marketing strategies.</t>
+  </si>
+  <si>
     <t>As a demography data analyst, I want to employ a decision tree algorithm to evaluate the impact of educational attainment levels on population growth rates across various regions, providing insights into educational policies and workforce planning initiatives.</t>
   </si>
   <si>
     <t>As a school principal, I want to implement a decision tree model to predict student dropout risk factors based on attendance, behavior, and academic performance data, so that I can intervene early and prevent dropouts.</t>
   </si>
   <si>
+    <t>As a social media analytics company, I want to build decision tree classifiers to detect and categorize user sentiment expressed in comments and posts, to provide clients with insights into public opinion and brand perception.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a document classification model to automatically categorize research papers and reports into topics such as fertility rates, aging population trends, and migration patterns, facilitating literature review and data synthesis.</t>
   </si>
   <si>
     <t>As a student counselor, I want to develop a document classification model to automatically tag and categorize student essays and reports based on academic performance indicators, so that I can provide targeted guidance and support.</t>
   </si>
   <si>
+    <t>As a social media influencer, I want to leverage document classification models to automatically filter and prioritize incoming messages and collaboration opportunities based on relevance and topic alignment with my personal brand, to optimize time management and focus on strategic partnerships.</t>
+  </si>
+  <si>
     <t>As a demography consultant, I need an entity extraction tool to extract key demographic indicators such as birth rates, mortality rates, and migration flows from international demographic databases and reports, facilitating comparative analysis across countries.</t>
   </si>
   <si>
     <t>As a language teacher, I want to implement entity extraction algorithms to automatically extract and classify vocabulary terms and grammatical structures from student texts and exercises, so that I can provide personalized feedback and targeted language learning support.</t>
   </si>
   <si>
+    <t>As a social media trend analyst, I want to use entity extraction techniques to identify and track mentions of emerging influencers and viral content across social media platforms, to predict trends and advise brands on influencer marketing strategies.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a feature selection algorithm to identify the most influential demographic variables affecting population density changes in urban areas, helping me prioritize factors for detailed analysis and policy recommendations.</t>
   </si>
   <si>
     <t>As a data analyst in education, I want to perform feature selection on student performance data to identify the most influential factors affecting academic outcomes, so that I can create targeted intervention strategies.</t>
   </si>
   <si>
+    <t>As a social media marketer, I want to use feature selection algorithms to identify influential features (such as hashtags, keywords) that correlate with high engagement rates on social media, to optimize content strategy and increase audience interaction.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to address class imbalance in demographic datasets when analyzing rare population characteristics such as extreme age groups or minority ethnicities, ensuring accurate representation and interpretation of demographic trends.</t>
   </si>
   <si>
     <t>As an educational researcher, I want to develop a predictive model for identifying gifted students in underrepresented populations using machine learning methods suitable for imbalanced datasets, so that I can support inclusive educational practices and talent development.</t>
   </si>
   <si>
+    <t>As a social media analytics company, I want to refine sentiment analysis models to accurately classify user opinions across diverse products and services, despite varying levels of sentiment class imbalance, to provide reliable insights to client brands.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply k-Nearest Neighbor (k-NN) algorithm to identify similar demographic clusters across different regions based on socio-economic indicators, facilitating comparative demographic analysis and regional policy recommendations.</t>
   </si>
   <si>
     <t>As a teacher, I want to integrate a keyword extraction algorithm into classroom discussion forums to automatically highlight and categorize student-generated ideas and discussions based on relevant educational topics, so that I can facilitate meaningful class discussions.</t>
   </si>
   <si>
+    <t>As a social media influencer, I want to apply KNN techniques to identify and connect with other influencers who have similar audience demographics and interests, to explore collaboration opportunities and expand my reach.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a keyword extraction algorithm to automatically identify and extract key demographic terms from large volumes of census data and demographic surveys, enabling efficient data summarization and trend analysis.</t>
   </si>
   <si>
     <t>As a special education teacher, I want to employ a k-NN model to identify similarities in learning profiles among students with disabilities, so that I can group them effectively for personalized educational interventions and support.</t>
   </si>
   <si>
+    <t>As a social media analytics company, I want to develop keyword extraction models to extract key terms related to product features and customer preferences from user conversations, to provide actionable insights for product development and marketing strategies.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a multi-label classification model to classify demographic surveys into multiple categories such as age groups, income brackets, and educational levels simultaneously, enabling comprehensive analysis of socio-economic profiles within populations.</t>
   </si>
   <si>
     <t>As a school counselor, I want to develop a multi-label classification model to predict various behavioral and academic outcomes for students based on their historical data, so that I can implement targeted intervention plans.</t>
   </si>
   <si>
+    <t>As a social media influencer, I want to use multi-label classification algorithms to categorize my content into multiple relevant topics or themes (e.g., beauty, fitness, travel), to attract a diverse audience and enhance engagement across different interest groups.</t>
+  </si>
+  <si>
     <t>As a demographer, I aim to use a neural network to analyze complex demographic datasets and predict future population trends based on historical census data, enabling accurate forecasting for urban planning and policy-making.</t>
   </si>
   <si>
     <t>As a teacher, I want to leverage neural networks to create predictive models that forecast student engagement levels and academic performance trends over time, so that I can proactively adjust my teaching strategies and classroom activities.</t>
   </si>
   <si>
+    <t>As a social media marketer, I want to develop neural network models for sentiment analysis of user-generated content (posts, comments) across multiple platforms, to gauge public opinion and adapt marketing strategies in real-time.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to apply random forest algorithms to analyze demographic survey data and predict household income levels based on demographic variables such as age, education, and employment status, aiding in socio-economic research and policy planning.</t>
   </si>
   <si>
     <t>As a school administrator, I want to implement a random forest model to analyze student attendance records, academic performance metrics, and behavioral data to identify patterns that predict student dropout risk, so that I can intervene early and improve retention rates.</t>
   </si>
   <si>
+    <t>As a social media content moderator, I want to use Random Forest algorithms to classify and filter inappropriate or harmful comments from user posts, to maintain a safe and respectful online community.</t>
+  </si>
+  <si>
     <t>As a demography educator, I want to create a semantic similarity tool to compare demographic theories and methodologies from different historical periods and cultural contexts, facilitating comparative demographic studies and theoretical analysis.</t>
   </si>
   <si>
     <t>As a language teacher, I want to develop a semantic similarity model using natural language processing to assess the similarity of student essays and provide feedback on content and language usage, so that I can support their writing development effectively.</t>
   </si>
   <si>
+    <t>As a social media analytics company, I want to implement semantic similarity analysis to detect duplicate or highly similar content across different social media channels, to ensure content uniqueness and avoid penalties from platform algorithms.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to perform sentiment analysis on social media data to understand public sentiment towards demographic policies and changes, helping to gauge public perception and support for policy initiatives.</t>
   </si>
   <si>
     <t>As a teacher, I want to use sentiment analysis to analyze student responses in classroom discussion forums and assignments to understand their emotional responses to learning topics and identify areas of confusion or interest, so that I can adjust my teaching approach accordingly.</t>
   </si>
   <si>
+    <t>As a social media marketer, I want to utilize sentiment analysis algorithms to track and analyze customer sentiment towards our brand across various social media platforms, to gauge public perception and inform brand strategies.</t>
+  </si>
+  <si>
     <t>As a special education teacher, I want to utilize speech-to-text tools to convert spoken responses from students with speech disabilities into written text, so that I can facilitate their participation in classroom discussions and assessments.</t>
   </si>
   <si>
+    <t>As a social media analytics company, I want to develop speech to text algorithms to transcribe user-generated video content on social media platforms, to extract valuable insights and sentiment from spoken content for client analysis and reporting.</t>
+  </si>
+  <si>
     <t>As a demographer, I need a speech-to-text system to transcribe interviews and focus group discussions on demographic trends and population behaviors, facilitating qualitative data analysis and research insights.</t>
   </si>
   <si>
     <t>As an educational researcher, I want to apply text categorization models to analyze student essays and assignments based on content themes and learning outcomes, so that I can gain insights into student performance and learning patterns.</t>
   </si>
   <si>
+    <t>As a social media marketer, I want to use text categorization algorithms to categorize customer inquiries and support tickets on social media platforms, to streamline response times and improve customer service efficiency.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply unsupervised clustering algorithms to analyze demographic survey data and identify distinct demographic segments within a population based on socio-economic characteristics, enabling targeted policy interventions and resource allocation strategies.</t>
   </si>
   <si>
     <t>As a teacher, I want to use unsupervised clustering algorithms to group student collaboration data in group projects and assignments to identify effective team dynamics and collaboration patterns, so that I can provide feedback and support for collaborative learning.</t>
   </si>
   <si>
+    <t>As a social media trend analyst, I want to use unsupervised clustering techniques to identify and categorize trending hashtags and topics across different social media platforms, to uncover emerging trends and viral content.</t>
+  </si>
+  <si>
     <t>As a demography educator, I want to utilize voice recognition capabilities to transcribe lectures and seminars on demographic theories and methodologies, providing accessible resources for students and researchers in demography.</t>
   </si>
   <si>
     <t>As an educational researcher, I want to develop a voice recognition model to analyze teacher-student interactions in classrooms to measure engagement levels and identify effective teaching strategies, so that I can improve classroom dynamics and learning outcomes.</t>
   </si>
   <si>
+    <t>As a social media content creator, I want to use voice recognition software to transcribe spoken content from videos or live streams into text for captions and SEO optimization on social media platforms.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to apply word embedding techniques to analyze text data from demographic surveys and reports, identifying semantic relationships between demographic terms and concepts, enhancing data interpretation and insight generation.</t>
   </si>
   <si>
     <t>As a language instructor, I want to utilize word embedding algorithms to create semantic maps of vocabulary and grammar structures to visualize language acquisition progress among students, so that I can tailor language lessons more effectively.</t>
+  </si>
+  <si>
+    <t>As a social media influencer, I want to apply word embedding algorithms to analyze and compare the engagement levels of different content types (e.g., images, videos, text) based on semantic similarities and user preferences, to optimize content strategy.</t>
   </si>
 </sst>
 </file>
@@ -382,7 +445,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,6 +485,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -530,7 +599,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -606,6 +675,15 @@
     <xf numFmtId="0" fontId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,6 +709,7 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff72fce9"/>
       <rgbColor rgb="ff16e6cf"/>
+      <rgbColor rgb="ff00ab8e"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1689,7 +1768,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:F82"/>
+  <dimension ref="A2:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2574,78 +2653,76 @@
       <c r="F44" s="24"/>
     </row>
     <row r="45" ht="19" customHeight="1">
-      <c r="A45" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B45" s="19">
-        <v>7</v>
-      </c>
-      <c r="C45" t="s" s="20">
+      <c r="A45" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B45" s="26">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D45" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s" s="14">
+        <v>77</v>
+      </c>
+      <c r="F45" s="24"/>
+    </row>
+    <row r="46" ht="19" customHeight="1">
+      <c r="A46" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B46" s="19">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D45" t="s" s="16">
-        <v>14</v>
-      </c>
-      <c r="E45" t="s" s="15">
-        <v>76</v>
-      </c>
-      <c r="F45" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" ht="19" customHeight="1">
-      <c r="A46" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B46" s="22">
-        <v>7</v>
-      </c>
-      <c r="C46" t="s" s="23">
-        <v>74</v>
       </c>
       <c r="D46" t="s" s="16">
         <v>14</v>
       </c>
       <c r="E46" t="s" s="15">
-        <v>77</v>
-      </c>
-      <c r="F46" s="24"/>
+        <v>78</v>
+      </c>
+      <c r="F46" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="47" ht="19" customHeight="1">
-      <c r="A47" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B47" s="19">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s" s="20">
-        <v>72</v>
+      <c r="A47" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B47" s="22">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D47" t="s" s="16">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E47" t="s" s="15">
-        <v>78</v>
-      </c>
-      <c r="F47" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="F47" s="24"/>
     </row>
     <row r="48" ht="19" customHeight="1">
-      <c r="A48" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B48" s="22">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s" s="23">
-        <v>74</v>
+      <c r="A48" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B48" s="26">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s" s="27">
+        <v>76</v>
       </c>
       <c r="D48" t="s" s="16">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E48" t="s" s="14">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F48" s="24"/>
     </row>
@@ -2660,10 +2737,10 @@
         <v>72</v>
       </c>
       <c r="D49" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E49" t="s" s="17">
-        <v>80</v>
+        <v>17</v>
+      </c>
+      <c r="E49" t="s" s="15">
+        <v>81</v>
       </c>
       <c r="F49" t="s" s="15">
         <v>11</v>
@@ -2680,86 +2757,84 @@
         <v>74</v>
       </c>
       <c r="D50" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E50" t="s" s="14">
+        <v>82</v>
+      </c>
+      <c r="F50" s="24"/>
+    </row>
+    <row r="51" ht="19" customHeight="1">
+      <c r="A51" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B51" s="26">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D51" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E51" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="F51" s="24"/>
+    </row>
+    <row r="52" ht="19" customHeight="1">
+      <c r="A52" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B52" s="19">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D52" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="E50" t="s" s="15">
-        <v>81</v>
-      </c>
-      <c r="F50" s="24"/>
-    </row>
-    <row r="51" ht="19" customHeight="1">
-      <c r="A51" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B51" s="19">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D51" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E51" t="s" s="14">
-        <v>82</v>
-      </c>
-      <c r="F51" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" ht="19" customHeight="1">
-      <c r="A52" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B52" s="22">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s" s="23">
+      <c r="E52" t="s" s="17">
+        <v>84</v>
+      </c>
+      <c r="F52" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" ht="19" customHeight="1">
+      <c r="A53" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B53" s="22">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D52" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E52" t="s" s="14">
-        <v>83</v>
-      </c>
-      <c r="F52" s="24"/>
-    </row>
-    <row r="53" ht="19" customHeight="1">
-      <c r="A53" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B53" s="19">
-        <v>7</v>
-      </c>
-      <c r="C53" t="s" s="20">
-        <v>72</v>
-      </c>
       <c r="D53" t="s" s="16">
-        <v>26</v>
-      </c>
-      <c r="E53" t="s" s="14">
-        <v>84</v>
-      </c>
-      <c r="F53" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E53" t="s" s="15">
+        <v>85</v>
+      </c>
+      <c r="F53" s="24"/>
     </row>
     <row r="54" ht="19" customHeight="1">
-      <c r="A54" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B54" s="22">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s" s="23">
-        <v>74</v>
+      <c r="A54" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B54" s="26">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s" s="27">
+        <v>76</v>
       </c>
       <c r="D54" t="s" s="16">
-        <v>26</v>
-      </c>
-      <c r="E54" t="s" s="15">
-        <v>85</v>
+        <v>20</v>
+      </c>
+      <c r="E54" t="s" s="17">
+        <v>86</v>
       </c>
       <c r="F54" s="24"/>
     </row>
@@ -2774,10 +2849,10 @@
         <v>72</v>
       </c>
       <c r="D55" t="s" s="16">
-        <v>29</v>
-      </c>
-      <c r="E55" t="s" s="15">
-        <v>86</v>
+        <v>23</v>
+      </c>
+      <c r="E55" t="s" s="14">
+        <v>87</v>
       </c>
       <c r="F55" t="s" s="15">
         <v>11</v>
@@ -2794,86 +2869,84 @@
         <v>74</v>
       </c>
       <c r="D56" t="s" s="16">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E56" t="s" s="14">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F56" s="24"/>
     </row>
     <row r="57" ht="19" customHeight="1">
-      <c r="A57" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B57" s="19">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s" s="20">
+      <c r="A57" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B57" s="26">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D57" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="E57" t="s" s="17">
+        <v>89</v>
+      </c>
+      <c r="F57" s="24"/>
+    </row>
+    <row r="58" ht="19" customHeight="1">
+      <c r="A58" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B58" s="19">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D57" t="s" s="16">
-        <v>32</v>
-      </c>
-      <c r="E57" t="s" s="15">
-        <v>88</v>
-      </c>
-      <c r="F57" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" ht="19" customHeight="1">
-      <c r="A58" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B58" s="22">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s" s="23">
+      <c r="D58" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E58" t="s" s="14">
+        <v>90</v>
+      </c>
+      <c r="F58" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" ht="19" customHeight="1">
+      <c r="A59" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B59" s="22">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D58" t="s" s="16">
-        <v>32</v>
-      </c>
-      <c r="E58" t="s" s="17">
-        <v>89</v>
-      </c>
-      <c r="F58" s="24"/>
-    </row>
-    <row r="59" ht="19" customHeight="1">
-      <c r="A59" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B59" s="19">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s" s="20">
-        <v>72</v>
-      </c>
       <c r="D59" t="s" s="16">
-        <v>35</v>
-      </c>
-      <c r="E59" t="s" s="14">
-        <v>90</v>
-      </c>
-      <c r="F59" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E59" t="s" s="15">
+        <v>91</v>
+      </c>
+      <c r="F59" s="24"/>
     </row>
     <row r="60" ht="19" customHeight="1">
-      <c r="A60" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B60" s="22">
-        <v>7</v>
-      </c>
-      <c r="C60" t="s" s="23">
-        <v>74</v>
+      <c r="A60" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B60" s="26">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s" s="27">
+        <v>76</v>
       </c>
       <c r="D60" t="s" s="16">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E60" t="s" s="14">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F60" s="24"/>
     </row>
@@ -2888,10 +2961,10 @@
         <v>72</v>
       </c>
       <c r="D61" t="s" s="16">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E61" t="s" s="15">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F61" t="s" s="15">
         <v>11</v>
@@ -2908,86 +2981,84 @@
         <v>74</v>
       </c>
       <c r="D62" t="s" s="16">
-        <v>38</v>
-      </c>
-      <c r="E62" t="s" s="15">
-        <v>93</v>
+        <v>29</v>
+      </c>
+      <c r="E62" t="s" s="14">
+        <v>94</v>
       </c>
       <c r="F62" s="24"/>
     </row>
     <row r="63" ht="19" customHeight="1">
-      <c r="A63" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B63" s="19">
-        <v>7</v>
-      </c>
-      <c r="C63" t="s" s="20">
+      <c r="A63" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B63" s="26">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D63" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E63" t="s" s="14">
+        <v>95</v>
+      </c>
+      <c r="F63" s="24"/>
+    </row>
+    <row r="64" ht="19" customHeight="1">
+      <c r="A64" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B64" s="19">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D63" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="E63" t="s" s="15">
-        <v>94</v>
-      </c>
-      <c r="F63" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" ht="19" customHeight="1">
-      <c r="A64" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B64" s="22">
-        <v>7</v>
-      </c>
-      <c r="C64" t="s" s="23">
+      <c r="D64" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E64" t="s" s="15">
+        <v>96</v>
+      </c>
+      <c r="F64" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" ht="19" customHeight="1">
+      <c r="A65" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B65" s="22">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D64" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="E64" t="s" s="14">
-        <v>95</v>
-      </c>
-      <c r="F64" s="24"/>
-    </row>
-    <row r="65" ht="19" customHeight="1">
-      <c r="A65" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B65" s="19">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s" s="20">
-        <v>72</v>
-      </c>
       <c r="D65" t="s" s="16">
-        <v>44</v>
-      </c>
-      <c r="E65" t="s" s="15">
-        <v>96</v>
-      </c>
-      <c r="F65" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E65" t="s" s="17">
+        <v>97</v>
+      </c>
+      <c r="F65" s="24"/>
     </row>
     <row r="66" ht="19" customHeight="1">
-      <c r="A66" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B66" s="22">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s" s="23">
-        <v>74</v>
+      <c r="A66" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B66" s="26">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s" s="27">
+        <v>76</v>
       </c>
       <c r="D66" t="s" s="16">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E66" t="s" s="14">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F66" s="24"/>
     </row>
@@ -3002,10 +3073,10 @@
         <v>72</v>
       </c>
       <c r="D67" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E67" t="s" s="15">
-        <v>98</v>
+        <v>35</v>
+      </c>
+      <c r="E67" t="s" s="14">
+        <v>99</v>
       </c>
       <c r="F67" t="s" s="15">
         <v>11</v>
@@ -3022,84 +3093,84 @@
         <v>74</v>
       </c>
       <c r="D68" t="s" s="16">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E68" t="s" s="14">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F68" s="24"/>
     </row>
     <row r="69" ht="19" customHeight="1">
-      <c r="A69" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B69" s="19">
-        <v>7</v>
-      </c>
-      <c r="C69" t="s" s="20">
+      <c r="A69" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B69" s="26">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D69" t="s" s="16">
+        <v>35</v>
+      </c>
+      <c r="E69" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="F69" s="24"/>
+    </row>
+    <row r="70" ht="19" customHeight="1">
+      <c r="A70" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B70" s="19">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D69" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E69" t="s" s="17">
-        <v>100</v>
-      </c>
-      <c r="F69" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="70" ht="19" customHeight="1">
-      <c r="A70" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B70" s="22">
-        <v>7</v>
-      </c>
-      <c r="C70" t="s" s="23">
+      <c r="D70" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="E70" t="s" s="15">
+        <v>102</v>
+      </c>
+      <c r="F70" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" ht="19" customHeight="1">
+      <c r="A71" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B71" s="22">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D70" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E70" t="s" s="14">
-        <v>101</v>
-      </c>
-      <c r="F70" s="24"/>
-    </row>
-    <row r="71" ht="19" customHeight="1">
-      <c r="A71" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B71" s="19">
-        <v>7</v>
-      </c>
-      <c r="C71" t="s" s="20">
-        <v>72</v>
-      </c>
       <c r="D71" t="s" s="16">
-        <v>53</v>
-      </c>
-      <c r="E71" t="s" s="14">
-        <v>102</v>
+        <v>38</v>
+      </c>
+      <c r="E71" t="s" s="15">
+        <v>103</v>
       </c>
       <c r="F71" s="24"/>
     </row>
     <row r="72" ht="19" customHeight="1">
-      <c r="A72" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B72" s="22">
-        <v>7</v>
-      </c>
-      <c r="C72" t="s" s="23">
-        <v>74</v>
+      <c r="A72" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B72" s="26">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s" s="27">
+        <v>76</v>
       </c>
       <c r="D72" t="s" s="16">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="E72" t="s" s="14">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F72" s="24"/>
     </row>
@@ -3114,10 +3185,10 @@
         <v>72</v>
       </c>
       <c r="D73" t="s" s="16">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E73" t="s" s="15">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F73" t="s" s="15">
         <v>11</v>
@@ -3134,86 +3205,84 @@
         <v>74</v>
       </c>
       <c r="D74" t="s" s="16">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E74" t="s" s="14">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F74" s="24"/>
     </row>
     <row r="75" ht="19" customHeight="1">
-      <c r="A75" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B75" s="19">
-        <v>7</v>
-      </c>
-      <c r="C75" t="s" s="20">
+      <c r="A75" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B75" s="26">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D75" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E75" t="s" s="14">
+        <v>107</v>
+      </c>
+      <c r="F75" s="24"/>
+    </row>
+    <row r="76" ht="19" customHeight="1">
+      <c r="A76" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B76" s="19">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D75" t="s" s="16">
-        <v>59</v>
-      </c>
-      <c r="E75" t="s" s="15">
-        <v>105</v>
-      </c>
-      <c r="F75" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="76" ht="19" customHeight="1">
-      <c r="A76" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B76" s="22">
-        <v>7</v>
-      </c>
-      <c r="C76" t="s" s="23">
+      <c r="D76" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="E76" t="s" s="15">
+        <v>108</v>
+      </c>
+      <c r="F76" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" ht="19" customHeight="1">
+      <c r="A77" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B77" s="22">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D76" t="s" s="16">
-        <v>59</v>
-      </c>
-      <c r="E76" t="s" s="14">
-        <v>106</v>
-      </c>
-      <c r="F76" s="24"/>
-    </row>
-    <row r="77" ht="19" customHeight="1">
-      <c r="A77" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B77" s="19">
-        <v>7</v>
-      </c>
-      <c r="C77" t="s" s="20">
-        <v>72</v>
-      </c>
       <c r="D77" t="s" s="16">
-        <v>62</v>
-      </c>
-      <c r="E77" t="s" s="15">
-        <v>107</v>
-      </c>
-      <c r="F77" t="s" s="15">
-        <v>11</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E77" t="s" s="14">
+        <v>109</v>
+      </c>
+      <c r="F77" s="24"/>
     </row>
     <row r="78" ht="19" customHeight="1">
-      <c r="A78" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B78" s="22">
-        <v>7</v>
-      </c>
-      <c r="C78" t="s" s="23">
-        <v>74</v>
+      <c r="A78" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B78" s="26">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s" s="27">
+        <v>76</v>
       </c>
       <c r="D78" t="s" s="16">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E78" t="s" s="14">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F78" s="24"/>
     </row>
@@ -3228,10 +3297,10 @@
         <v>72</v>
       </c>
       <c r="D79" t="s" s="16">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="E79" t="s" s="15">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F79" t="s" s="15">
         <v>11</v>
@@ -3248,50 +3317,420 @@
         <v>74</v>
       </c>
       <c r="D80" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E80" t="s" s="14">
+        <v>112</v>
+      </c>
+      <c r="F80" s="24"/>
+    </row>
+    <row r="81" ht="19" customHeight="1">
+      <c r="A81" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B81" s="26">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D81" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E81" t="s" s="14">
+        <v>113</v>
+      </c>
+      <c r="F81" s="24"/>
+    </row>
+    <row r="82" ht="19" customHeight="1">
+      <c r="A82" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B82" s="19">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D82" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E82" t="s" s="17">
+        <v>114</v>
+      </c>
+      <c r="F82" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" ht="19" customHeight="1">
+      <c r="A83" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B83" s="22">
+        <v>7</v>
+      </c>
+      <c r="C83" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D83" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E83" t="s" s="14">
+        <v>115</v>
+      </c>
+      <c r="F83" s="24"/>
+    </row>
+    <row r="84" ht="19" customHeight="1">
+      <c r="A84" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B84" s="26">
+        <v>7</v>
+      </c>
+      <c r="C84" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D84" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E84" t="s" s="17">
+        <v>116</v>
+      </c>
+      <c r="F84" s="24"/>
+    </row>
+    <row r="85" ht="19" customHeight="1">
+      <c r="A85" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B85" s="19">
+        <v>7</v>
+      </c>
+      <c r="C85" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D85" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E85" t="s" s="14">
+        <v>117</v>
+      </c>
+      <c r="F85" s="24"/>
+    </row>
+    <row r="86" ht="19" customHeight="1">
+      <c r="A86" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B86" s="22">
+        <v>7</v>
+      </c>
+      <c r="C86" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D86" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E86" t="s" s="14">
+        <v>118</v>
+      </c>
+      <c r="F86" s="24"/>
+    </row>
+    <row r="87" ht="19" customHeight="1">
+      <c r="A87" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B87" s="26">
+        <v>7</v>
+      </c>
+      <c r="C87" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D87" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E87" t="s" s="14">
+        <v>119</v>
+      </c>
+      <c r="F87" s="24"/>
+    </row>
+    <row r="88" ht="19" customHeight="1">
+      <c r="A88" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B88" s="19">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D88" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E88" t="s" s="15">
+        <v>117</v>
+      </c>
+      <c r="F88" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" ht="19" customHeight="1">
+      <c r="A89" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B89" s="22">
+        <v>7</v>
+      </c>
+      <c r="C89" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D89" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E89" t="s" s="14">
+        <v>120</v>
+      </c>
+      <c r="F89" s="24"/>
+    </row>
+    <row r="90" ht="19" customHeight="1">
+      <c r="A90" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B90" s="26">
+        <v>7</v>
+      </c>
+      <c r="C90" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D90" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E90" t="s" s="17">
+        <v>121</v>
+      </c>
+      <c r="F90" s="24"/>
+    </row>
+    <row r="91" ht="19" customHeight="1">
+      <c r="A91" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B91" s="19">
+        <v>7</v>
+      </c>
+      <c r="C91" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D91" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E91" t="s" s="15">
+        <v>122</v>
+      </c>
+      <c r="F91" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" ht="19" customHeight="1">
+      <c r="A92" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B92" s="22">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D92" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E92" t="s" s="14">
+        <v>123</v>
+      </c>
+      <c r="F92" s="24"/>
+    </row>
+    <row r="93" ht="19" customHeight="1">
+      <c r="A93" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B93" s="26">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D93" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E93" t="s" s="14">
+        <v>124</v>
+      </c>
+      <c r="F93" s="24"/>
+    </row>
+    <row r="94" ht="19" customHeight="1">
+      <c r="A94" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B94" s="19">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D94" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E94" t="s" s="15">
+        <v>125</v>
+      </c>
+      <c r="F94" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" ht="19" customHeight="1">
+      <c r="A95" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B95" s="22">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D95" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E95" t="s" s="14">
+        <v>126</v>
+      </c>
+      <c r="F95" s="24"/>
+    </row>
+    <row r="96" ht="19" customHeight="1">
+      <c r="A96" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B96" s="26">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D96" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E96" t="s" s="14">
+        <v>127</v>
+      </c>
+      <c r="F96" s="24"/>
+    </row>
+    <row r="97" ht="19" customHeight="1">
+      <c r="A97" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B97" s="19">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D97" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E80" t="s" s="14">
-        <v>110</v>
-      </c>
-      <c r="F80" s="24"/>
-    </row>
-    <row r="81" ht="19" customHeight="1">
-      <c r="A81" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B81" s="19">
-        <v>7</v>
-      </c>
-      <c r="C81" t="s" s="20">
+      <c r="E97" t="s" s="15">
+        <v>128</v>
+      </c>
+      <c r="F97" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" ht="19" customHeight="1">
+      <c r="A98" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B98" s="22">
+        <v>7</v>
+      </c>
+      <c r="C98" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D98" t="s" s="16">
+        <v>65</v>
+      </c>
+      <c r="E98" t="s" s="14">
+        <v>129</v>
+      </c>
+      <c r="F98" s="24"/>
+    </row>
+    <row r="99" ht="19" customHeight="1">
+      <c r="A99" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B99" s="26">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D99" t="s" s="16">
+        <v>65</v>
+      </c>
+      <c r="E99" t="s" s="14">
+        <v>130</v>
+      </c>
+      <c r="F99" s="24"/>
+    </row>
+    <row r="100" ht="19" customHeight="1">
+      <c r="A100" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B100" s="19">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D81" t="s" s="16">
+      <c r="D100" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E81" t="s" s="15">
-        <v>111</v>
-      </c>
-      <c r="F81" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="82" ht="19" customHeight="1">
-      <c r="A82" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B82" s="22">
-        <v>7</v>
-      </c>
-      <c r="C82" t="s" s="23">
+      <c r="E100" t="s" s="15">
+        <v>131</v>
+      </c>
+      <c r="F100" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" ht="19" customHeight="1">
+      <c r="A101" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B101" s="22">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D82" t="s" s="16">
+      <c r="D101" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E82" t="s" s="14">
-        <v>112</v>
-      </c>
-      <c r="F82" s="24"/>
+      <c r="E101" t="s" s="14">
+        <v>132</v>
+      </c>
+      <c r="F101" s="24"/>
+    </row>
+    <row r="102" ht="19" customHeight="1">
+      <c r="A102" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="B102" s="26">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s" s="27">
+        <v>76</v>
+      </c>
+      <c r="D102" t="s" s="16">
+        <v>68</v>
+      </c>
+      <c r="E102" t="s" s="14">
+        <v>133</v>
+      </c>
+      <c r="F102" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add USs related to cluster domain "Social and Urban Studies" [Social Networks]
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
+++ b/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="155">
   <si>
     <t>Tabella 1</t>
   </si>
@@ -247,6 +247,12 @@
     <t>As a social media content moderator, I want to employ adversarial learning techniques to automatically detect and filter out hate speech in user comments, in order to create a safer and more inclusive online community.</t>
   </si>
   <si>
+    <t>Social Networks</t>
+  </si>
+  <si>
+    <t>As a social media analyst, I want to employ adversarial learning techniques to detect and mitigate fake accounts and bot activity on our social media platform, in order to maintain a trustworthy user community.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply CNN models to analyze satellite imagery and identify changes in urban sprawl over time, helping me understand how demographic shifts affect city planning and development.</t>
   </si>
   <si>
@@ -256,6 +262,9 @@
     <t>As a social media trend analyst, I want to use CNN models to analyze image content across posts and identify emerging trends or viral content early, so that I can advise brands on timely marketing strategies.</t>
   </si>
   <si>
+    <t>As a social media analyst, I want to deploy CNN models for image recognition to automatically detect and classify inappropriate or offensive content in user-uploaded images, ensuring a safe and positive user experience.</t>
+  </si>
+  <si>
     <t>As a government official, I want to deploy a conversational agent that can interactively guide citizens through demographic surveys, ensuring accurate data collection and enhancing public engagement in demographic studies.</t>
   </si>
   <si>
@@ -265,6 +274,9 @@
     <t>As a social media marketer, I want to develop a chatbot using NLP techniques to conduct surveys and gather feedback from followers about their preferences and opinions on our brand's content, to inform future marketing strategies.</t>
   </si>
   <si>
+    <t>As a social media manager, I want to develop a conversational agent powered by NLP to automate customer support interactions on our social media platform, improving response times and user satisfaction.</t>
+  </si>
+  <si>
     <t>As a demography data analyst, I want to employ a decision tree algorithm to evaluate the impact of educational attainment levels on population growth rates across various regions, providing insights into educational policies and workforce planning initiatives.</t>
   </si>
   <si>
@@ -274,6 +286,9 @@
     <t>As a social media analytics company, I want to build decision tree classifiers to detect and categorize user sentiment expressed in comments and posts, to provide clients with insights into public opinion and brand perception.</t>
   </si>
   <si>
+    <t>As a social network data scientist, I want to employ decision tree algorithms to segment our user base based on demographic and behavioral data extracted from social media profiles, enabling targeted marketing campaigns.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a document classification model to automatically categorize research papers and reports into topics such as fertility rates, aging population trends, and migration patterns, facilitating literature review and data synthesis.</t>
   </si>
   <si>
@@ -283,6 +298,9 @@
     <t>As a social media influencer, I want to leverage document classification models to automatically filter and prioritize incoming messages and collaboration opportunities based on relevance and topic alignment with my personal brand, to optimize time management and focus on strategic partnerships.</t>
   </si>
   <si>
+    <t>As a community moderator, I want to deploy document classification techniques to detect and filter out inappropriate or offensive content shared within our social network community, ensuring a safe and positive user experience.</t>
+  </si>
+  <si>
     <t>As a demography consultant, I need an entity extraction tool to extract key demographic indicators such as birth rates, mortality rates, and migration flows from international demographic databases and reports, facilitating comparative analysis across countries.</t>
   </si>
   <si>
@@ -292,6 +310,9 @@
     <t>As a social media trend analyst, I want to use entity extraction techniques to identify and track mentions of emerging influencers and viral content across social media platforms, to predict trends and advise brands on influencer marketing strategies.</t>
   </si>
   <si>
+    <t>As a social network data scientist, I want to implement entity extraction techniques to extract key information such as dates, locations, and event details from event announcements and user-generated posts on our social network, facilitating event planning and coordination.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a feature selection algorithm to identify the most influential demographic variables affecting population density changes in urban areas, helping me prioritize factors for detailed analysis and policy recommendations.</t>
   </si>
   <si>
@@ -301,6 +322,9 @@
     <t>As a social media marketer, I want to use feature selection algorithms to identify influential features (such as hashtags, keywords) that correlate with high engagement rates on social media, to optimize content strategy and increase audience interaction.</t>
   </si>
   <si>
+    <t>As a social media analyst, I want to implement feature selection algorithms to identify important linguistic features (such as emojis, hashtags, and linguistic patterns) in user tweets and posts, helping us tailor our marketing messages to resonate better with our audience.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to address class imbalance in demographic datasets when analyzing rare population characteristics such as extreme age groups or minority ethnicities, ensuring accurate representation and interpretation of demographic trends.</t>
   </si>
   <si>
@@ -310,6 +334,9 @@
     <t>As a social media analytics company, I want to refine sentiment analysis models to accurately classify user opinions across diverse products and services, despite varying levels of sentiment class imbalance, to provide reliable insights to client brands.</t>
   </si>
   <si>
+    <t>As a community moderator, I want to use strategies for handling imbalanced data in detecting abusive or harmful content on our social media platform, enabling us to promptly identify and remove such content to protect our user community.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply k-Nearest Neighbor (k-NN) algorithm to identify similar demographic clusters across different regions based on socio-economic indicators, facilitating comparative demographic analysis and regional policy recommendations.</t>
   </si>
   <si>
@@ -319,6 +346,9 @@
     <t>As a social media influencer, I want to apply KNN techniques to identify and connect with other influencers who have similar audience demographics and interests, to explore collaboration opportunities and expand my reach.</t>
   </si>
   <si>
+    <t>As a social media manager, I want to develop a keyword extraction system to automatically identify trending topics and hashtags from user posts on our social media platform, facilitating timely content creation and engagement.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a keyword extraction algorithm to automatically identify and extract key demographic terms from large volumes of census data and demographic surveys, enabling efficient data summarization and trend analysis.</t>
   </si>
   <si>
@@ -328,6 +358,9 @@
     <t>As a social media analytics company, I want to develop keyword extraction models to extract key terms related to product features and customer preferences from user conversations, to provide actionable insights for product development and marketing strategies.</t>
   </si>
   <si>
+    <t>As a social media analyst, I want to implement a k-Nearest Neighbor (k-NN) algorithm to recommend relevant users or accounts for collaboration based on similar interests and engagement patterns on our social media platform.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a multi-label classification model to classify demographic surveys into multiple categories such as age groups, income brackets, and educational levels simultaneously, enabling comprehensive analysis of socio-economic profiles within populations.</t>
   </si>
   <si>
@@ -337,6 +370,9 @@
     <t>As a social media influencer, I want to use multi-label classification algorithms to categorize my content into multiple relevant topics or themes (e.g., beauty, fitness, travel), to attract a diverse audience and enhance engagement across different interest groups.</t>
   </si>
   <si>
+    <t>As a social network researcher, I want to apply multi-label classification techniques to analyze user interactions and classify user interests across various topics (e.g., technology, fashion, sports) on our social network, enabling targeted content recommendation and personalized user experiences.</t>
+  </si>
+  <si>
     <t>As a demographer, I aim to use a neural network to analyze complex demographic datasets and predict future population trends based on historical census data, enabling accurate forecasting for urban planning and policy-making.</t>
   </si>
   <si>
@@ -346,6 +382,9 @@
     <t>As a social media marketer, I want to develop neural network models for sentiment analysis of user-generated content (posts, comments) across multiple platforms, to gauge public opinion and adapt marketing strategies in real-time.</t>
   </si>
   <si>
+    <t>As a social media analyst, I want to train a neural network model to predict user engagement levels with different types of content (e.g., videos, images, text posts) on our social media platform, helping us optimize our content strategy for maximum reach and interaction.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to apply random forest algorithms to analyze demographic survey data and predict household income levels based on demographic variables such as age, education, and employment status, aiding in socio-economic research and policy planning.</t>
   </si>
   <si>
@@ -355,6 +394,9 @@
     <t>As a social media content moderator, I want to use Random Forest algorithms to classify and filter inappropriate or harmful comments from user posts, to maintain a safe and respectful online community.</t>
   </si>
   <si>
+    <t>As a social media manager, I want to develop a random forest model to analyze user engagement metrics (likes, shares, comments) across different types of content on our social media platform, identifying factors that contribute most to user interaction and content virality.</t>
+  </si>
+  <si>
     <t>As a demography educator, I want to create a semantic similarity tool to compare demographic theories and methodologies from different historical periods and cultural contexts, facilitating comparative demographic studies and theoretical analysis.</t>
   </si>
   <si>
@@ -364,6 +406,9 @@
     <t>As a social media analytics company, I want to implement semantic similarity analysis to detect duplicate or highly similar content across different social media channels, to ensure content uniqueness and avoid penalties from platform algorithms.</t>
   </si>
   <si>
+    <t>As a social media analyst, I want to implement semantic similarity algorithms to recommend relevant content and connections to users based on their past interactions and interests on our social media platform, enhancing personalized user experiences.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to perform sentiment analysis on social media data to understand public sentiment towards demographic policies and changes, helping to gauge public perception and support for policy initiatives.</t>
   </si>
   <si>
@@ -373,12 +418,18 @@
     <t>As a social media marketer, I want to utilize sentiment analysis algorithms to track and analyze customer sentiment towards our brand across various social media platforms, to gauge public perception and inform brand strategies.</t>
   </si>
   <si>
+    <t>As a social media manager, I want to develop a sentiment analysis model to automatically classify user comments and reviews on our social media platform into positive, negative, or neutral sentiment categories, enabling us to gauge customer satisfaction and sentiment trends.</t>
+  </si>
+  <si>
     <t>As a special education teacher, I want to utilize speech-to-text tools to convert spoken responses from students with speech disabilities into written text, so that I can facilitate their participation in classroom discussions and assessments.</t>
   </si>
   <si>
     <t>As a social media analytics company, I want to develop speech to text algorithms to transcribe user-generated video content on social media platforms, to extract valuable insights and sentiment from spoken content for client analysis and reporting.</t>
   </si>
   <si>
+    <t>As a social media analyst, I want to implement speech to text algorithms to automatically transcribe live video content shared by users during events and broadcasts on our social media platform, improving content indexing and searchability.</t>
+  </si>
+  <si>
     <t>As a demographer, I need a speech-to-text system to transcribe interviews and focus group discussions on demographic trends and population behaviors, facilitating qualitative data analysis and research insights.</t>
   </si>
   <si>
@@ -388,6 +439,9 @@
     <t>As a social media marketer, I want to use text categorization algorithms to categorize customer inquiries and support tickets on social media platforms, to streamline response times and improve customer service efficiency.</t>
   </si>
   <si>
+    <t>As a social media manager, I want to develop a text categorization system to automatically classify user comments and posts into predefined categories (e.g., feedback, inquiries, complaints) on our social media platform, improving response time and customer service efficiency.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply unsupervised clustering algorithms to analyze demographic survey data and identify distinct demographic segments within a population based on socio-economic characteristics, enabling targeted policy interventions and resource allocation strategies.</t>
   </si>
   <si>
@@ -397,6 +451,9 @@
     <t>As a social media trend analyst, I want to use unsupervised clustering techniques to identify and categorize trending hashtags and topics across different social media platforms, to uncover emerging trends and viral content.</t>
   </si>
   <si>
+    <t>As a social network researcher, I want to use unsupervised clustering techniques to analyze user interactions and group users into communities or segments based on shared interests and connections within our social network, facilitating community engagement strategies.</t>
+  </si>
+  <si>
     <t>As a demography educator, I want to utilize voice recognition capabilities to transcribe lectures and seminars on demographic theories and methodologies, providing accessible resources for students and researchers in demography.</t>
   </si>
   <si>
@@ -406,6 +463,9 @@
     <t>As a social media content creator, I want to use voice recognition software to transcribe spoken content from videos or live streams into text for captions and SEO optimization on social media platforms.</t>
   </si>
   <si>
+    <t>As a community moderator, I want to deploy voice recognition models to monitor and analyze audio content shared by users for compliance with community guidelines and policies on our social media platform, ensuring a safe and respectful online environment.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to apply word embedding techniques to analyze text data from demographic surveys and reports, identifying semantic relationships between demographic terms and concepts, enhancing data interpretation and insight generation.</t>
   </si>
   <si>
@@ -413,6 +473,9 @@
   </si>
   <si>
     <t>As a social media influencer, I want to apply word embedding algorithms to analyze and compare the engagement levels of different content types (e.g., images, videos, text) based on semantic similarities and user preferences, to optimize content strategy.</t>
+  </si>
+  <si>
+    <t>As a social media analyst, I want to use word embedding algorithms to measure the similarity between user queries and product descriptions on our social media platform, improving search relevance and user experience.</t>
   </si>
 </sst>
 </file>
@@ -445,7 +508,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,6 +554,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -599,7 +668,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -672,9 +741,6 @@
     <xf numFmtId="49" fontId="3" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -682,6 +748,15 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="8" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -710,6 +785,7 @@
       <rgbColor rgb="ff72fce9"/>
       <rgbColor rgb="ff16e6cf"/>
       <rgbColor rgb="ff00ab8e"/>
+      <rgbColor rgb="ff006b65"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1768,7 +1844,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:F102"/>
+  <dimension ref="A2:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2650,16 +2726,18 @@
       <c r="E44" t="s" s="14">
         <v>75</v>
       </c>
-      <c r="F44" s="24"/>
+      <c r="F44" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="45" ht="19" customHeight="1">
-      <c r="A45" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B45" s="26">
-        <v>7</v>
-      </c>
-      <c r="C45" t="s" s="27">
+      <c r="A45" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B45" s="25">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s" s="26">
         <v>76</v>
       </c>
       <c r="D45" t="s" s="16">
@@ -2668,175 +2746,189 @@
       <c r="E45" t="s" s="14">
         <v>77</v>
       </c>
-      <c r="F45" s="24"/>
+      <c r="F45" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="46" ht="19" customHeight="1">
-      <c r="A46" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B46" s="19">
-        <v>7</v>
-      </c>
-      <c r="C46" t="s" s="20">
+      <c r="A46" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B46" s="28">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D46" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s" s="14">
+        <v>79</v>
+      </c>
+      <c r="F46" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" ht="19" customHeight="1">
+      <c r="A47" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B47" s="19">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D46" t="s" s="16">
-        <v>14</v>
-      </c>
-      <c r="E46" t="s" s="15">
-        <v>78</v>
-      </c>
-      <c r="F46" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" ht="19" customHeight="1">
-      <c r="A47" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B47" s="22">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s" s="23">
-        <v>74</v>
       </c>
       <c r="D47" t="s" s="16">
         <v>14</v>
       </c>
       <c r="E47" t="s" s="15">
-        <v>79</v>
-      </c>
-      <c r="F47" s="24"/>
+        <v>80</v>
+      </c>
+      <c r="F47" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="48" ht="19" customHeight="1">
-      <c r="A48" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B48" s="26">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s" s="27">
-        <v>76</v>
+      <c r="A48" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B48" s="22">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D48" t="s" s="16">
         <v>14</v>
       </c>
-      <c r="E48" t="s" s="14">
-        <v>80</v>
-      </c>
-      <c r="F48" s="24"/>
+      <c r="E48" t="s" s="15">
+        <v>81</v>
+      </c>
+      <c r="F48" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="49" ht="19" customHeight="1">
-      <c r="A49" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B49" s="19">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s" s="20">
+      <c r="A49" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B49" s="25">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D49" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E49" t="s" s="14">
+        <v>82</v>
+      </c>
+      <c r="F49" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" ht="19" customHeight="1">
+      <c r="A50" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B50" s="28">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D50" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E50" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="F50" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" ht="19" customHeight="1">
+      <c r="A51" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B51" s="19">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D49" t="s" s="16">
-        <v>17</v>
-      </c>
-      <c r="E49" t="s" s="15">
-        <v>81</v>
-      </c>
-      <c r="F49" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" ht="19" customHeight="1">
-      <c r="A50" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B50" s="22">
-        <v>7</v>
-      </c>
-      <c r="C50" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D50" t="s" s="16">
-        <v>17</v>
-      </c>
-      <c r="E50" t="s" s="14">
-        <v>82</v>
-      </c>
-      <c r="F50" s="24"/>
-    </row>
-    <row r="51" ht="19" customHeight="1">
-      <c r="A51" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B51" s="26">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s" s="27">
-        <v>76</v>
       </c>
       <c r="D51" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="E51" t="s" s="14">
-        <v>83</v>
-      </c>
-      <c r="F51" s="24"/>
+      <c r="E51" t="s" s="15">
+        <v>84</v>
+      </c>
+      <c r="F51" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="52" ht="19" customHeight="1">
-      <c r="A52" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B52" s="19">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s" s="20">
-        <v>72</v>
+      <c r="A52" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B52" s="22">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D52" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E52" t="s" s="17">
-        <v>84</v>
+        <v>17</v>
+      </c>
+      <c r="E52" t="s" s="14">
+        <v>85</v>
       </c>
       <c r="F52" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="53" ht="19" customHeight="1">
-      <c r="A53" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B53" s="22">
-        <v>7</v>
-      </c>
-      <c r="C53" t="s" s="23">
-        <v>74</v>
+      <c r="A53" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B53" s="25">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s" s="26">
+        <v>76</v>
       </c>
       <c r="D53" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E53" t="s" s="15">
-        <v>85</v>
-      </c>
-      <c r="F53" s="24"/>
+        <v>17</v>
+      </c>
+      <c r="E53" t="s" s="14">
+        <v>86</v>
+      </c>
+      <c r="F53" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="54" ht="19" customHeight="1">
-      <c r="A54" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B54" s="26">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s" s="27">
-        <v>76</v>
+      <c r="A54" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B54" s="28">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s" s="29">
+        <v>78</v>
       </c>
       <c r="D54" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E54" t="s" s="17">
-        <v>86</v>
-      </c>
-      <c r="F54" s="24"/>
+        <v>17</v>
+      </c>
+      <c r="E54" t="s" s="14">
+        <v>87</v>
+      </c>
+      <c r="F54" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="55" ht="19" customHeight="1">
       <c r="A55" t="s" s="18">
@@ -2849,10 +2941,10 @@
         <v>72</v>
       </c>
       <c r="D55" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E55" t="s" s="14">
-        <v>87</v>
+        <v>20</v>
+      </c>
+      <c r="E55" t="s" s="17">
+        <v>88</v>
       </c>
       <c r="F55" t="s" s="15">
         <v>11</v>
@@ -2869,198 +2961,214 @@
         <v>74</v>
       </c>
       <c r="D56" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="E56" t="s" s="15">
+        <v>89</v>
+      </c>
+      <c r="F56" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" ht="19" customHeight="1">
+      <c r="A57" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B57" s="25">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D57" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="E57" t="s" s="17">
+        <v>90</v>
+      </c>
+      <c r="F57" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" ht="19" customHeight="1">
+      <c r="A58" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B58" s="28">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D58" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="E58" t="s" s="14">
+        <v>91</v>
+      </c>
+      <c r="F58" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" ht="19" customHeight="1">
+      <c r="A59" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B59" s="19">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D59" t="s" s="16">
         <v>23</v>
       </c>
-      <c r="E56" t="s" s="14">
-        <v>88</v>
-      </c>
-      <c r="F56" s="24"/>
-    </row>
-    <row r="57" ht="19" customHeight="1">
-      <c r="A57" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B57" s="26">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s" s="27">
+      <c r="E59" t="s" s="14">
+        <v>92</v>
+      </c>
+      <c r="F59" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" ht="19" customHeight="1">
+      <c r="A60" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B60" s="22">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D60" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="E60" t="s" s="14">
+        <v>93</v>
+      </c>
+      <c r="F60" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" ht="19" customHeight="1">
+      <c r="A61" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B61" s="25">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D57" t="s" s="16">
+      <c r="D61" t="s" s="16">
         <v>23</v>
       </c>
-      <c r="E57" t="s" s="17">
-        <v>89</v>
-      </c>
-      <c r="F57" s="24"/>
-    </row>
-    <row r="58" ht="19" customHeight="1">
-      <c r="A58" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B58" s="19">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s" s="20">
+      <c r="E61" t="s" s="17">
+        <v>94</v>
+      </c>
+      <c r="F61" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" ht="19" customHeight="1">
+      <c r="A62" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B62" s="28">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D62" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="E62" t="s" s="14">
+        <v>95</v>
+      </c>
+      <c r="F62" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" ht="19" customHeight="1">
+      <c r="A63" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B63" s="19">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D58" t="s" s="16">
+      <c r="D63" t="s" s="16">
         <v>26</v>
       </c>
-      <c r="E58" t="s" s="14">
-        <v>90</v>
-      </c>
-      <c r="F58" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" ht="19" customHeight="1">
-      <c r="A59" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B59" s="22">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s" s="23">
+      <c r="E63" t="s" s="14">
+        <v>96</v>
+      </c>
+      <c r="F63" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" ht="19" customHeight="1">
+      <c r="A64" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B64" s="22">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D59" t="s" s="16">
+      <c r="D64" t="s" s="16">
         <v>26</v>
       </c>
-      <c r="E59" t="s" s="15">
-        <v>91</v>
-      </c>
-      <c r="F59" s="24"/>
-    </row>
-    <row r="60" ht="19" customHeight="1">
-      <c r="A60" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B60" s="26">
-        <v>7</v>
-      </c>
-      <c r="C60" t="s" s="27">
+      <c r="E64" t="s" s="15">
+        <v>97</v>
+      </c>
+      <c r="F64" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" ht="19" customHeight="1">
+      <c r="A65" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B65" s="25">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D60" t="s" s="16">
+      <c r="D65" t="s" s="16">
         <v>26</v>
       </c>
-      <c r="E60" t="s" s="14">
-        <v>92</v>
-      </c>
-      <c r="F60" s="24"/>
-    </row>
-    <row r="61" ht="19" customHeight="1">
-      <c r="A61" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B61" s="19">
-        <v>7</v>
-      </c>
-      <c r="C61" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D61" t="s" s="16">
-        <v>29</v>
-      </c>
-      <c r="E61" t="s" s="15">
-        <v>93</v>
-      </c>
-      <c r="F61" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" ht="19" customHeight="1">
-      <c r="A62" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B62" s="22">
-        <v>7</v>
-      </c>
-      <c r="C62" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D62" t="s" s="16">
-        <v>29</v>
-      </c>
-      <c r="E62" t="s" s="14">
-        <v>94</v>
-      </c>
-      <c r="F62" s="24"/>
-    </row>
-    <row r="63" ht="19" customHeight="1">
-      <c r="A63" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B63" s="26">
-        <v>7</v>
-      </c>
-      <c r="C63" t="s" s="27">
-        <v>76</v>
-      </c>
-      <c r="D63" t="s" s="16">
-        <v>29</v>
-      </c>
-      <c r="E63" t="s" s="14">
-        <v>95</v>
-      </c>
-      <c r="F63" s="24"/>
-    </row>
-    <row r="64" ht="19" customHeight="1">
-      <c r="A64" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B64" s="19">
-        <v>7</v>
-      </c>
-      <c r="C64" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D64" t="s" s="16">
-        <v>32</v>
-      </c>
-      <c r="E64" t="s" s="15">
-        <v>96</v>
-      </c>
-      <c r="F64" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" ht="19" customHeight="1">
-      <c r="A65" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B65" s="22">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D65" t="s" s="16">
-        <v>32</v>
-      </c>
-      <c r="E65" t="s" s="17">
-        <v>97</v>
-      </c>
-      <c r="F65" s="24"/>
+      <c r="E65" t="s" s="14">
+        <v>98</v>
+      </c>
+      <c r="F65" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="66" ht="19" customHeight="1">
-      <c r="A66" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B66" s="26">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s" s="27">
-        <v>76</v>
+      <c r="A66" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B66" s="28">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s" s="29">
+        <v>78</v>
       </c>
       <c r="D66" t="s" s="16">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E66" t="s" s="14">
-        <v>98</v>
-      </c>
-      <c r="F66" s="24"/>
+        <v>99</v>
+      </c>
+      <c r="F66" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="67" ht="19" customHeight="1">
       <c r="A67" t="s" s="18">
@@ -3073,10 +3181,10 @@
         <v>72</v>
       </c>
       <c r="D67" t="s" s="16">
-        <v>35</v>
-      </c>
-      <c r="E67" t="s" s="14">
-        <v>99</v>
+        <v>29</v>
+      </c>
+      <c r="E67" t="s" s="15">
+        <v>100</v>
       </c>
       <c r="F67" t="s" s="15">
         <v>11</v>
@@ -3093,198 +3201,214 @@
         <v>74</v>
       </c>
       <c r="D68" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E68" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="F68" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" ht="19" customHeight="1">
+      <c r="A69" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B69" s="25">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D69" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E69" t="s" s="14">
+        <v>102</v>
+      </c>
+      <c r="F69" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" ht="19" customHeight="1">
+      <c r="A70" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B70" s="28">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D70" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E70" t="s" s="14">
+        <v>103</v>
+      </c>
+      <c r="F70" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" ht="19" customHeight="1">
+      <c r="A71" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B71" s="19">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D71" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E71" t="s" s="15">
+        <v>104</v>
+      </c>
+      <c r="F71" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" ht="19" customHeight="1">
+      <c r="A72" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B72" s="22">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D72" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E72" t="s" s="17">
+        <v>105</v>
+      </c>
+      <c r="F72" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" ht="19" customHeight="1">
+      <c r="A73" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B73" s="25">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D73" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E73" t="s" s="14">
+        <v>106</v>
+      </c>
+      <c r="F73" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" ht="19" customHeight="1">
+      <c r="A74" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B74" s="28">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D74" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E74" t="s" s="14">
+        <v>107</v>
+      </c>
+      <c r="F74" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" ht="19" customHeight="1">
+      <c r="A75" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B75" s="19">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D75" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E68" t="s" s="14">
-        <v>100</v>
-      </c>
-      <c r="F68" s="24"/>
-    </row>
-    <row r="69" ht="19" customHeight="1">
-      <c r="A69" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B69" s="26">
-        <v>7</v>
-      </c>
-      <c r="C69" t="s" s="27">
+      <c r="E75" t="s" s="14">
+        <v>108</v>
+      </c>
+      <c r="F75" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" ht="19" customHeight="1">
+      <c r="A76" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B76" s="22">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D76" t="s" s="16">
+        <v>35</v>
+      </c>
+      <c r="E76" t="s" s="14">
+        <v>109</v>
+      </c>
+      <c r="F76" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" ht="19" customHeight="1">
+      <c r="A77" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B77" s="25">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D69" t="s" s="16">
+      <c r="D77" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E69" t="s" s="14">
-        <v>101</v>
-      </c>
-      <c r="F69" s="24"/>
-    </row>
-    <row r="70" ht="19" customHeight="1">
-      <c r="A70" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B70" s="19">
-        <v>7</v>
-      </c>
-      <c r="C70" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D70" t="s" s="16">
-        <v>38</v>
-      </c>
-      <c r="E70" t="s" s="15">
-        <v>102</v>
-      </c>
-      <c r="F70" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="71" ht="19" customHeight="1">
-      <c r="A71" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B71" s="22">
-        <v>7</v>
-      </c>
-      <c r="C71" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D71" t="s" s="16">
-        <v>38</v>
-      </c>
-      <c r="E71" t="s" s="15">
-        <v>103</v>
-      </c>
-      <c r="F71" s="24"/>
-    </row>
-    <row r="72" ht="19" customHeight="1">
-      <c r="A72" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B72" s="26">
-        <v>7</v>
-      </c>
-      <c r="C72" t="s" s="27">
-        <v>76</v>
-      </c>
-      <c r="D72" t="s" s="16">
-        <v>38</v>
-      </c>
-      <c r="E72" t="s" s="14">
-        <v>104</v>
-      </c>
-      <c r="F72" s="24"/>
-    </row>
-    <row r="73" ht="19" customHeight="1">
-      <c r="A73" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B73" s="19">
-        <v>7</v>
-      </c>
-      <c r="C73" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D73" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="E73" t="s" s="15">
-        <v>105</v>
-      </c>
-      <c r="F73" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="74" ht="19" customHeight="1">
-      <c r="A74" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B74" s="22">
-        <v>7</v>
-      </c>
-      <c r="C74" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D74" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="E74" t="s" s="14">
-        <v>106</v>
-      </c>
-      <c r="F74" s="24"/>
-    </row>
-    <row r="75" ht="19" customHeight="1">
-      <c r="A75" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B75" s="26">
-        <v>7</v>
-      </c>
-      <c r="C75" t="s" s="27">
-        <v>76</v>
-      </c>
-      <c r="D75" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="E75" t="s" s="14">
-        <v>107</v>
-      </c>
-      <c r="F75" s="24"/>
-    </row>
-    <row r="76" ht="19" customHeight="1">
-      <c r="A76" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B76" s="19">
-        <v>7</v>
-      </c>
-      <c r="C76" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D76" t="s" s="16">
-        <v>44</v>
-      </c>
-      <c r="E76" t="s" s="15">
-        <v>108</v>
-      </c>
-      <c r="F76" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="77" ht="19" customHeight="1">
-      <c r="A77" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B77" s="22">
-        <v>7</v>
-      </c>
-      <c r="C77" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D77" t="s" s="16">
-        <v>44</v>
-      </c>
       <c r="E77" t="s" s="14">
-        <v>109</v>
-      </c>
-      <c r="F77" s="24"/>
+        <v>110</v>
+      </c>
+      <c r="F77" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="78" ht="19" customHeight="1">
-      <c r="A78" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B78" s="26">
-        <v>7</v>
-      </c>
-      <c r="C78" t="s" s="27">
-        <v>76</v>
+      <c r="A78" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B78" s="28">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s" s="29">
+        <v>78</v>
       </c>
       <c r="D78" t="s" s="16">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E78" t="s" s="14">
-        <v>110</v>
-      </c>
-      <c r="F78" s="24"/>
+        <v>111</v>
+      </c>
+      <c r="F78" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="79" ht="19" customHeight="1">
       <c r="A79" t="s" s="18">
@@ -3297,10 +3421,10 @@
         <v>72</v>
       </c>
       <c r="D79" t="s" s="16">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E79" t="s" s="15">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F79" t="s" s="15">
         <v>11</v>
@@ -3317,196 +3441,214 @@
         <v>74</v>
       </c>
       <c r="D80" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E80" t="s" s="14">
-        <v>112</v>
-      </c>
-      <c r="F80" s="24"/>
+        <v>38</v>
+      </c>
+      <c r="E80" t="s" s="15">
+        <v>113</v>
+      </c>
+      <c r="F80" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="81" ht="19" customHeight="1">
-      <c r="A81" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B81" s="26">
-        <v>7</v>
-      </c>
-      <c r="C81" t="s" s="27">
+      <c r="A81" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B81" s="25">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s" s="26">
         <v>76</v>
       </c>
       <c r="D81" t="s" s="16">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E81" t="s" s="14">
-        <v>113</v>
-      </c>
-      <c r="F81" s="24"/>
+        <v>114</v>
+      </c>
+      <c r="F81" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="82" ht="19" customHeight="1">
-      <c r="A82" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B82" s="19">
-        <v>7</v>
-      </c>
-      <c r="C82" t="s" s="20">
+      <c r="A82" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B82" s="28">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D82" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="E82" t="s" s="14">
+        <v>115</v>
+      </c>
+      <c r="F82" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" ht="19" customHeight="1">
+      <c r="A83" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B83" s="19">
+        <v>7</v>
+      </c>
+      <c r="C83" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D82" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E82" t="s" s="17">
-        <v>114</v>
-      </c>
-      <c r="F82" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="83" ht="19" customHeight="1">
-      <c r="A83" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B83" s="22">
-        <v>7</v>
-      </c>
-      <c r="C83" t="s" s="23">
+      <c r="D83" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E83" t="s" s="15">
+        <v>116</v>
+      </c>
+      <c r="F83" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" ht="19" customHeight="1">
+      <c r="A84" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B84" s="22">
+        <v>7</v>
+      </c>
+      <c r="C84" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D83" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E83" t="s" s="14">
-        <v>115</v>
-      </c>
-      <c r="F83" s="24"/>
-    </row>
-    <row r="84" ht="19" customHeight="1">
-      <c r="A84" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B84" s="26">
-        <v>7</v>
-      </c>
-      <c r="C84" t="s" s="27">
+      <c r="D84" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E84" t="s" s="14">
+        <v>117</v>
+      </c>
+      <c r="F84" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" ht="19" customHeight="1">
+      <c r="A85" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B85" s="25">
+        <v>7</v>
+      </c>
+      <c r="C85" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D84" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E84" t="s" s="17">
-        <v>116</v>
-      </c>
-      <c r="F84" s="24"/>
-    </row>
-    <row r="85" ht="19" customHeight="1">
-      <c r="A85" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B85" s="19">
-        <v>7</v>
-      </c>
-      <c r="C85" t="s" s="20">
+      <c r="D85" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E85" t="s" s="14">
+        <v>118</v>
+      </c>
+      <c r="F85" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" ht="19" customHeight="1">
+      <c r="A86" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B86" s="28">
+        <v>7</v>
+      </c>
+      <c r="C86" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D86" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E86" t="s" s="14">
+        <v>119</v>
+      </c>
+      <c r="F86" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" ht="19" customHeight="1">
+      <c r="A87" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B87" s="19">
+        <v>7</v>
+      </c>
+      <c r="C87" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D85" t="s" s="16">
-        <v>53</v>
-      </c>
-      <c r="E85" t="s" s="14">
-        <v>117</v>
-      </c>
-      <c r="F85" s="24"/>
-    </row>
-    <row r="86" ht="19" customHeight="1">
-      <c r="A86" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B86" s="22">
-        <v>7</v>
-      </c>
-      <c r="C86" t="s" s="23">
+      <c r="D87" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="E87" t="s" s="15">
+        <v>120</v>
+      </c>
+      <c r="F87" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" ht="19" customHeight="1">
+      <c r="A88" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B88" s="22">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D86" t="s" s="16">
-        <v>53</v>
-      </c>
-      <c r="E86" t="s" s="14">
-        <v>118</v>
-      </c>
-      <c r="F86" s="24"/>
-    </row>
-    <row r="87" ht="19" customHeight="1">
-      <c r="A87" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B87" s="26">
-        <v>7</v>
-      </c>
-      <c r="C87" t="s" s="27">
+      <c r="D88" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="E88" t="s" s="14">
+        <v>121</v>
+      </c>
+      <c r="F88" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" ht="19" customHeight="1">
+      <c r="A89" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B89" s="25">
+        <v>7</v>
+      </c>
+      <c r="C89" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D87" t="s" s="16">
-        <v>53</v>
-      </c>
-      <c r="E87" t="s" s="14">
-        <v>119</v>
-      </c>
-      <c r="F87" s="24"/>
-    </row>
-    <row r="88" ht="19" customHeight="1">
-      <c r="A88" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B88" s="19">
-        <v>7</v>
-      </c>
-      <c r="C88" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D88" t="s" s="16">
-        <v>56</v>
-      </c>
-      <c r="E88" t="s" s="15">
-        <v>117</v>
-      </c>
-      <c r="F88" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="89" ht="19" customHeight="1">
-      <c r="A89" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B89" s="22">
-        <v>7</v>
-      </c>
-      <c r="C89" t="s" s="23">
-        <v>74</v>
-      </c>
       <c r="D89" t="s" s="16">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E89" t="s" s="14">
-        <v>120</v>
-      </c>
-      <c r="F89" s="24"/>
+        <v>122</v>
+      </c>
+      <c r="F89" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="90" ht="19" customHeight="1">
-      <c r="A90" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B90" s="26">
-        <v>7</v>
-      </c>
-      <c r="C90" t="s" s="27">
-        <v>76</v>
+      <c r="A90" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B90" s="28">
+        <v>7</v>
+      </c>
+      <c r="C90" t="s" s="29">
+        <v>78</v>
       </c>
       <c r="D90" t="s" s="16">
-        <v>56</v>
-      </c>
-      <c r="E90" t="s" s="17">
-        <v>121</v>
-      </c>
-      <c r="F90" s="24"/>
+        <v>44</v>
+      </c>
+      <c r="E90" t="s" s="14">
+        <v>123</v>
+      </c>
+      <c r="F90" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
     <row r="91" ht="19" customHeight="1">
       <c r="A91" t="s" s="18">
@@ -3519,10 +3661,10 @@
         <v>72</v>
       </c>
       <c r="D91" t="s" s="16">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E91" t="s" s="15">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F91" t="s" s="15">
         <v>11</v>
@@ -3539,198 +3681,614 @@
         <v>74</v>
       </c>
       <c r="D92" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E92" t="s" s="14">
+        <v>125</v>
+      </c>
+      <c r="F92" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" ht="19" customHeight="1">
+      <c r="A93" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B93" s="25">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D93" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E93" t="s" s="14">
+        <v>126</v>
+      </c>
+      <c r="F93" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" ht="19" customHeight="1">
+      <c r="A94" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B94" s="28">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D94" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E94" t="s" s="14">
+        <v>127</v>
+      </c>
+      <c r="F94" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" ht="19" customHeight="1">
+      <c r="A95" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B95" s="19">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D95" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E95" t="s" s="17">
+        <v>128</v>
+      </c>
+      <c r="F95" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" ht="19" customHeight="1">
+      <c r="A96" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B96" s="22">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D96" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E96" t="s" s="14">
+        <v>129</v>
+      </c>
+      <c r="F96" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" ht="19" customHeight="1">
+      <c r="A97" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B97" s="25">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D97" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E97" t="s" s="17">
+        <v>130</v>
+      </c>
+      <c r="F97" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" ht="19" customHeight="1">
+      <c r="A98" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B98" s="28">
+        <v>7</v>
+      </c>
+      <c r="C98" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D98" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E98" t="s" s="14">
+        <v>131</v>
+      </c>
+      <c r="F98" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" ht="19" customHeight="1">
+      <c r="A99" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B99" s="19">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D99" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E99" t="s" s="14">
+        <v>132</v>
+      </c>
+      <c r="F99" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" ht="19" customHeight="1">
+      <c r="A100" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B100" s="22">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D100" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E100" t="s" s="14">
+        <v>133</v>
+      </c>
+      <c r="F100" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" ht="19" customHeight="1">
+      <c r="A101" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B101" s="25">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D101" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E101" t="s" s="14">
+        <v>134</v>
+      </c>
+      <c r="F101" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" ht="19" customHeight="1">
+      <c r="A102" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B102" s="28">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D102" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E102" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="F102" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" ht="19" customHeight="1">
+      <c r="A103" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B103" s="19">
+        <v>7</v>
+      </c>
+      <c r="C103" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D103" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E103" t="s" s="15">
+        <v>132</v>
+      </c>
+      <c r="F103" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104" ht="19" customHeight="1">
+      <c r="A104" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B104" s="22">
+        <v>7</v>
+      </c>
+      <c r="C104" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D104" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E104" t="s" s="14">
+        <v>136</v>
+      </c>
+      <c r="F104" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" ht="19" customHeight="1">
+      <c r="A105" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B105" s="25">
+        <v>7</v>
+      </c>
+      <c r="C105" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D105" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E105" t="s" s="17">
+        <v>137</v>
+      </c>
+      <c r="F105" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" ht="19" customHeight="1">
+      <c r="A106" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B106" s="28">
+        <v>7</v>
+      </c>
+      <c r="C106" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D106" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E106" t="s" s="14">
+        <v>138</v>
+      </c>
+      <c r="F106" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" ht="19" customHeight="1">
+      <c r="A107" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B107" s="19">
+        <v>7</v>
+      </c>
+      <c r="C107" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D107" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E92" t="s" s="14">
-        <v>123</v>
-      </c>
-      <c r="F92" s="24"/>
-    </row>
-    <row r="93" ht="19" customHeight="1">
-      <c r="A93" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B93" s="26">
-        <v>7</v>
-      </c>
-      <c r="C93" t="s" s="27">
+      <c r="E107" t="s" s="15">
+        <v>139</v>
+      </c>
+      <c r="F107" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" ht="19" customHeight="1">
+      <c r="A108" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B108" s="22">
+        <v>7</v>
+      </c>
+      <c r="C108" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D108" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E108" t="s" s="14">
+        <v>140</v>
+      </c>
+      <c r="F108" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" ht="19" customHeight="1">
+      <c r="A109" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B109" s="25">
+        <v>7</v>
+      </c>
+      <c r="C109" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D93" t="s" s="16">
+      <c r="D109" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E93" t="s" s="14">
-        <v>124</v>
-      </c>
-      <c r="F93" s="24"/>
-    </row>
-    <row r="94" ht="19" customHeight="1">
-      <c r="A94" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B94" s="19">
-        <v>7</v>
-      </c>
-      <c r="C94" t="s" s="20">
+      <c r="E109" t="s" s="14">
+        <v>141</v>
+      </c>
+      <c r="F109" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" ht="19" customHeight="1">
+      <c r="A110" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B110" s="28">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D110" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E110" t="s" s="14">
+        <v>142</v>
+      </c>
+      <c r="F110" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="111" ht="19" customHeight="1">
+      <c r="A111" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B111" s="19">
+        <v>7</v>
+      </c>
+      <c r="C111" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D94" t="s" s="16">
+      <c r="D111" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E94" t="s" s="15">
-        <v>125</v>
-      </c>
-      <c r="F94" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="95" ht="19" customHeight="1">
-      <c r="A95" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B95" s="22">
-        <v>7</v>
-      </c>
-      <c r="C95" t="s" s="23">
+      <c r="E111" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="F111" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" ht="19" customHeight="1">
+      <c r="A112" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B112" s="22">
+        <v>7</v>
+      </c>
+      <c r="C112" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D95" t="s" s="16">
+      <c r="D112" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E95" t="s" s="14">
-        <v>126</v>
-      </c>
-      <c r="F95" s="24"/>
-    </row>
-    <row r="96" ht="19" customHeight="1">
-      <c r="A96" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B96" s="26">
-        <v>7</v>
-      </c>
-      <c r="C96" t="s" s="27">
+      <c r="E112" t="s" s="14">
+        <v>144</v>
+      </c>
+      <c r="F112" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" ht="19" customHeight="1">
+      <c r="A113" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B113" s="25">
+        <v>7</v>
+      </c>
+      <c r="C113" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D96" t="s" s="16">
+      <c r="D113" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E96" t="s" s="14">
-        <v>127</v>
-      </c>
-      <c r="F96" s="24"/>
-    </row>
-    <row r="97" ht="19" customHeight="1">
-      <c r="A97" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B97" s="19">
-        <v>7</v>
-      </c>
-      <c r="C97" t="s" s="20">
+      <c r="E113" t="s" s="14">
+        <v>145</v>
+      </c>
+      <c r="F113" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" ht="19" customHeight="1">
+      <c r="A114" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B114" s="28">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D114" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E114" t="s" s="14">
+        <v>146</v>
+      </c>
+      <c r="F114" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" ht="19" customHeight="1">
+      <c r="A115" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B115" s="19">
+        <v>7</v>
+      </c>
+      <c r="C115" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D97" t="s" s="16">
+      <c r="D115" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E97" t="s" s="15">
-        <v>128</v>
-      </c>
-      <c r="F97" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="98" ht="19" customHeight="1">
-      <c r="A98" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B98" s="22">
-        <v>7</v>
-      </c>
-      <c r="C98" t="s" s="23">
+      <c r="E115" t="s" s="15">
+        <v>147</v>
+      </c>
+      <c r="F115" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" ht="19" customHeight="1">
+      <c r="A116" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B116" s="22">
+        <v>7</v>
+      </c>
+      <c r="C116" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D98" t="s" s="16">
+      <c r="D116" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E98" t="s" s="14">
-        <v>129</v>
-      </c>
-      <c r="F98" s="24"/>
-    </row>
-    <row r="99" ht="19" customHeight="1">
-      <c r="A99" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B99" s="26">
-        <v>7</v>
-      </c>
-      <c r="C99" t="s" s="27">
+      <c r="E116" t="s" s="14">
+        <v>148</v>
+      </c>
+      <c r="F116" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" ht="19" customHeight="1">
+      <c r="A117" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B117" s="25">
+        <v>7</v>
+      </c>
+      <c r="C117" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D99" t="s" s="16">
+      <c r="D117" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E99" t="s" s="14">
-        <v>130</v>
-      </c>
-      <c r="F99" s="24"/>
-    </row>
-    <row r="100" ht="19" customHeight="1">
-      <c r="A100" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B100" s="19">
-        <v>7</v>
-      </c>
-      <c r="C100" t="s" s="20">
+      <c r="E117" t="s" s="14">
+        <v>149</v>
+      </c>
+      <c r="F117" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" ht="19" customHeight="1">
+      <c r="A118" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B118" s="28">
+        <v>7</v>
+      </c>
+      <c r="C118" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D118" t="s" s="16">
+        <v>65</v>
+      </c>
+      <c r="E118" t="s" s="14">
+        <v>150</v>
+      </c>
+      <c r="F118" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" ht="19" customHeight="1">
+      <c r="A119" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B119" s="19">
+        <v>7</v>
+      </c>
+      <c r="C119" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D100" t="s" s="16">
+      <c r="D119" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E100" t="s" s="15">
-        <v>131</v>
-      </c>
-      <c r="F100" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="101" ht="19" customHeight="1">
-      <c r="A101" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B101" s="22">
-        <v>7</v>
-      </c>
-      <c r="C101" t="s" s="23">
+      <c r="E119" t="s" s="15">
+        <v>151</v>
+      </c>
+      <c r="F119" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120" ht="19" customHeight="1">
+      <c r="A120" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B120" s="22">
+        <v>7</v>
+      </c>
+      <c r="C120" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D101" t="s" s="16">
+      <c r="D120" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E101" t="s" s="14">
-        <v>132</v>
-      </c>
-      <c r="F101" s="24"/>
-    </row>
-    <row r="102" ht="19" customHeight="1">
-      <c r="A102" t="s" s="25">
-        <v>71</v>
-      </c>
-      <c r="B102" s="26">
-        <v>7</v>
-      </c>
-      <c r="C102" t="s" s="27">
+      <c r="E120" t="s" s="14">
+        <v>152</v>
+      </c>
+      <c r="F120" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" ht="19" customHeight="1">
+      <c r="A121" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B121" s="25">
+        <v>7</v>
+      </c>
+      <c r="C121" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D102" t="s" s="16">
+      <c r="D121" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E102" t="s" s="14">
-        <v>133</v>
-      </c>
-      <c r="F102" s="24"/>
+      <c r="E121" t="s" s="14">
+        <v>153</v>
+      </c>
+      <c r="F121" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" ht="19" customHeight="1">
+      <c r="A122" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B122" s="28">
+        <v>7</v>
+      </c>
+      <c r="C122" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D122" t="s" s="16">
+        <v>68</v>
+      </c>
+      <c r="E122" t="s" s="14">
+        <v>154</v>
+      </c>
+      <c r="F122" t="s" s="15">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add USs related to cluster domain "Social and Urban Studies" [Social Work]
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
+++ b/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="176">
   <si>
     <t>Tabella 1</t>
   </si>
@@ -253,6 +253,12 @@
     <t>As a social media analyst, I want to employ adversarial learning techniques to detect and mitigate fake accounts and bot activity on our social media platform, in order to maintain a trustworthy user community.</t>
   </si>
   <si>
+    <t>Social Work</t>
+  </si>
+  <si>
+    <t>As a social worker, I want to apply adversarial learning techniques to improve the privacy and security of confidential client data, ensuring that sensitive information remains protected while still allowing for effective analysis and decision-making.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply CNN models to analyze satellite imagery and identify changes in urban sprawl over time, helping me understand how demographic shifts affect city planning and development.</t>
   </si>
   <si>
@@ -265,6 +271,9 @@
     <t>As a social media analyst, I want to deploy CNN models for image recognition to automatically detect and classify inappropriate or offensive content in user-uploaded images, ensuring a safe and positive user experience.</t>
   </si>
   <si>
+    <t>As a child welfare advocate, I want to implement CNNs to analyze patterns in child behavior and environmental factors to predict the likelihood of neglect or abuse, facilitating early intervention and protection measures.</t>
+  </si>
+  <si>
     <t>As a government official, I want to deploy a conversational agent that can interactively guide citizens through demographic surveys, ensuring accurate data collection and enhancing public engagement in demographic studies.</t>
   </si>
   <si>
@@ -277,6 +286,9 @@
     <t>As a social media manager, I want to develop a conversational agent powered by NLP to automate customer support interactions on our social media platform, improving response times and user satisfaction.</t>
   </si>
   <si>
+    <t>As a social worker, I want to develop a conversational agent powered by NLP to provide immediate crisis intervention and emotional support to individuals experiencing domestic violence, ensuring they have access to help 24/7.</t>
+  </si>
+  <si>
     <t>As a demography data analyst, I want to employ a decision tree algorithm to evaluate the impact of educational attainment levels on population growth rates across various regions, providing insights into educational policies and workforce planning initiatives.</t>
   </si>
   <si>
@@ -289,6 +301,9 @@
     <t>As a social network data scientist, I want to employ decision tree algorithms to segment our user base based on demographic and behavioral data extracted from social media profiles, enabling targeted marketing campaigns.</t>
   </si>
   <si>
+    <t>As a child protection specialist, I want to utilize decision trees to prioritize cases of child neglect for investigation, ensuring that limited resources are allocated to the most critical situations where early intervention is crucial.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a document classification model to automatically categorize research papers and reports into topics such as fertility rates, aging population trends, and migration patterns, facilitating literature review and data synthesis.</t>
   </si>
   <si>
@@ -301,6 +316,9 @@
     <t>As a community moderator, I want to deploy document classification techniques to detect and filter out inappropriate or offensive content shared within our social network community, ensuring a safe and positive user experience.</t>
   </si>
   <si>
+    <t>As a social worker, I want to develop a document classification model to automatically categorize incoming client reports into different risk levels, facilitating prioritization of cases requiring urgent intervention.</t>
+  </si>
+  <si>
     <t>As a demography consultant, I need an entity extraction tool to extract key demographic indicators such as birth rates, mortality rates, and migration flows from international demographic databases and reports, facilitating comparative analysis across countries.</t>
   </si>
   <si>
@@ -313,6 +331,9 @@
     <t>As a social network data scientist, I want to implement entity extraction techniques to extract key information such as dates, locations, and event details from event announcements and user-generated posts on our social network, facilitating event planning and coordination.</t>
   </si>
   <si>
+    <t>As a social worker, I want to develop an entity extraction system to automatically identify and extract key information from intake forms, such as names, addresses, and contact details, to streamline case management processes.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a feature selection algorithm to identify the most influential demographic variables affecting population density changes in urban areas, helping me prioritize factors for detailed analysis and policy recommendations.</t>
   </si>
   <si>
@@ -325,6 +346,9 @@
     <t>As a social media analyst, I want to implement feature selection algorithms to identify important linguistic features (such as emojis, hashtags, and linguistic patterns) in user tweets and posts, helping us tailor our marketing messages to resonate better with our audience.</t>
   </si>
   <si>
+    <t>As a social worker, I want to perform feature selection on demographic and socioeconomic variables to identify the most influential factors contributing to homelessness, enabling targeted interventions and resource allocation strategies.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to address class imbalance in demographic datasets when analyzing rare population characteristics such as extreme age groups or minority ethnicities, ensuring accurate representation and interpretation of demographic trends.</t>
   </si>
   <si>
@@ -337,6 +361,9 @@
     <t>As a community moderator, I want to use strategies for handling imbalanced data in detecting abusive or harmful content on our social media platform, enabling us to promptly identify and remove such content to protect our user community.</t>
   </si>
   <si>
+    <t>As a domestic violence advocate, I want to apply techniques for managing imbalanced datasets when analyzing police reports and victim statements, improving the accuracy of risk assessments and enhancing safety planning for survivors.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply k-Nearest Neighbor (k-NN) algorithm to identify similar demographic clusters across different regions based on socio-economic indicators, facilitating comparative demographic analysis and regional policy recommendations.</t>
   </si>
   <si>
@@ -349,6 +376,9 @@
     <t>As a social media manager, I want to develop a keyword extraction system to automatically identify trending topics and hashtags from user posts on our social media platform, facilitating timely content creation and engagement.</t>
   </si>
   <si>
+    <t>As a social worker, I want to use KNN to identify similarities in case histories and demographic profiles among clients to better understand common needs and tailor support services accordingly.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a keyword extraction algorithm to automatically identify and extract key demographic terms from large volumes of census data and demographic surveys, enabling efficient data summarization and trend analysis.</t>
   </si>
   <si>
@@ -361,6 +391,9 @@
     <t>As a social media analyst, I want to implement a k-Nearest Neighbor (k-NN) algorithm to recommend relevant users or accounts for collaboration based on similar interests and engagement patterns on our social media platform.</t>
   </si>
   <si>
+    <t>As a social worker, I want to develop a keyword extraction model to automatically identify key phrases related to domestic violence in client narratives, aiding in the identification of high-risk cases for immediate intervention.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a multi-label classification model to classify demographic surveys into multiple categories such as age groups, income brackets, and educational levels simultaneously, enabling comprehensive analysis of socio-economic profiles within populations.</t>
   </si>
   <si>
@@ -373,6 +406,9 @@
     <t>As a social network researcher, I want to apply multi-label classification techniques to analyze user interactions and classify user interests across various topics (e.g., technology, fashion, sports) on our social network, enabling targeted content recommendation and personalized user experiences.</t>
   </si>
   <si>
+    <t>As a healthcare coordinator in social work, I want to implement multi-label classification to categorize patient health records into different chronic conditions and mental health disorders, facilitating personalized care plans and treatment strategies.</t>
+  </si>
+  <si>
     <t>As a demographer, I aim to use a neural network to analyze complex demographic datasets and predict future population trends based on historical census data, enabling accurate forecasting for urban planning and policy-making.</t>
   </si>
   <si>
@@ -385,6 +421,9 @@
     <t>As a social media analyst, I want to train a neural network model to predict user engagement levels with different types of content (e.g., videos, images, text posts) on our social media platform, helping us optimize our content strategy for maximum reach and interaction.</t>
   </si>
   <si>
+    <t>As a social worker, I want to develop a neural network model to analyze patterns in client behavior and demographic data to predict the likelihood of recidivism among individuals in correctional facilities, informing rehabilitation programs and support services.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to apply random forest algorithms to analyze demographic survey data and predict household income levels based on demographic variables such as age, education, and employment status, aiding in socio-economic research and policy planning.</t>
   </si>
   <si>
@@ -397,6 +436,9 @@
     <t>As a social media manager, I want to develop a random forest model to analyze user engagement metrics (likes, shares, comments) across different types of content on our social media platform, identifying factors that contribute most to user interaction and content virality.</t>
   </si>
   <si>
+    <t>As a social worker, I want to develop a random forest model to predict the risk of elderly isolation based on demographic data and living conditions, enabling targeted outreach and support services.</t>
+  </si>
+  <si>
     <t>As a demography educator, I want to create a semantic similarity tool to compare demographic theories and methodologies from different historical periods and cultural contexts, facilitating comparative demographic studies and theoretical analysis.</t>
   </si>
   <si>
@@ -409,6 +451,9 @@
     <t>As a social media analyst, I want to implement semantic similarity algorithms to recommend relevant content and connections to users based on their past interactions and interests on our social media platform, enhancing personalized user experiences.</t>
   </si>
   <si>
+    <t>As a social worker, I want to develop a semantic similarity model to analyze client case notes and identify similarities in reported symptoms and behavior patterns, facilitating more accurate diagnosis and treatment planning.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to perform sentiment analysis on social media data to understand public sentiment towards demographic policies and changes, helping to gauge public perception and support for policy initiatives.</t>
   </si>
   <si>
@@ -421,6 +466,9 @@
     <t>As a social media manager, I want to develop a sentiment analysis model to automatically classify user comments and reviews on our social media platform into positive, negative, or neutral sentiment categories, enabling us to gauge customer satisfaction and sentiment trends.</t>
   </si>
   <si>
+    <t>As a crisis counselor, I want to implement sentiment analysis on text messages and chat transcripts from crisis interventions to assess the emotional state of clients and tailor responses accordingly.</t>
+  </si>
+  <si>
     <t>As a special education teacher, I want to utilize speech-to-text tools to convert spoken responses from students with speech disabilities into written text, so that I can facilitate their participation in classroom discussions and assessments.</t>
   </si>
   <si>
@@ -430,6 +478,9 @@
     <t>As a social media analyst, I want to implement speech to text algorithms to automatically transcribe live video content shared by users during events and broadcasts on our social media platform, improving content indexing and searchability.</t>
   </si>
   <si>
+    <t>As a counselor, I want to implement speech to text for transcribing group therapy sessions to capture discussions and insights shared by participants, facilitating comprehensive session reviews and progress tracking.</t>
+  </si>
+  <si>
     <t>As a demographer, I need a speech-to-text system to transcribe interviews and focus group discussions on demographic trends and population behaviors, facilitating qualitative data analysis and research insights.</t>
   </si>
   <si>
@@ -442,6 +493,9 @@
     <t>As a social media manager, I want to develop a text categorization system to automatically classify user comments and posts into predefined categories (e.g., feedback, inquiries, complaints) on our social media platform, improving response time and customer service efficiency.</t>
   </si>
   <si>
+    <t>As a social worker, I want to develop a text categorization model to classify incoming client emails into different service categories (e.g., counseling, financial assistance, housing support), ensuring timely and efficient response to client needs.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply unsupervised clustering algorithms to analyze demographic survey data and identify distinct demographic segments within a population based on socio-economic characteristics, enabling targeted policy interventions and resource allocation strategies.</t>
   </si>
   <si>
@@ -454,6 +508,9 @@
     <t>As a social network researcher, I want to use unsupervised clustering techniques to analyze user interactions and group users into communities or segments based on shared interests and connections within our social network, facilitating community engagement strategies.</t>
   </si>
   <si>
+    <t>As a social worker, I want to use unsupervised clustering to group client case notes based on similar behavioral patterns and risk factors, identifying common needs and informing personalized intervention plans.</t>
+  </si>
+  <si>
     <t>As a demography educator, I want to utilize voice recognition capabilities to transcribe lectures and seminars on demographic theories and methodologies, providing accessible resources for students and researchers in demography.</t>
   </si>
   <si>
@@ -466,6 +523,9 @@
     <t>As a community moderator, I want to deploy voice recognition models to monitor and analyze audio content shared by users for compliance with community guidelines and policies on our social media platform, ensuring a safe and respectful online environment.</t>
   </si>
   <si>
+    <t>As a counselor, I want to develop a voice recognition system to detect emotional cues and distress signals in client speech during counseling sessions, aiding in real-time assessment and intervention.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to apply word embedding techniques to analyze text data from demographic surveys and reports, identifying semantic relationships between demographic terms and concepts, enhancing data interpretation and insight generation.</t>
   </si>
   <si>
@@ -476,6 +536,9 @@
   </si>
   <si>
     <t>As a social media analyst, I want to use word embedding algorithms to measure the similarity between user queries and product descriptions on our social media platform, improving search relevance and user experience.</t>
+  </si>
+  <si>
+    <t>As a social worker, I want to use word embedding techniques to analyze case notes and identify recurring themes and patterns related to client needs and service utilization, guiding personalized service planning.</t>
   </si>
 </sst>
 </file>
@@ -508,7 +571,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,6 +623,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -668,7 +737,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -759,6 +828,15 @@
     <xf numFmtId="49" fontId="3" fillId="9" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,6 +864,7 @@
       <rgbColor rgb="ff16e6cf"/>
       <rgbColor rgb="ff00ab8e"/>
       <rgbColor rgb="ff006b65"/>
+      <rgbColor rgb="ff88f94e"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1844,7 +1923,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:F122"/>
+  <dimension ref="A2:F142"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2771,320 +2850,320 @@
       </c>
     </row>
     <row r="47" ht="19" customHeight="1">
-      <c r="A47" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B47" s="19">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s" s="20">
+      <c r="A47" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B47" s="31">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D47" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s" s="14">
+        <v>81</v>
+      </c>
+      <c r="F47" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" ht="19" customHeight="1">
+      <c r="A48" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B48" s="19">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D47" t="s" s="16">
-        <v>14</v>
-      </c>
-      <c r="E47" t="s" s="15">
-        <v>80</v>
-      </c>
-      <c r="F47" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" ht="19" customHeight="1">
-      <c r="A48" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B48" s="22">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s" s="23">
-        <v>74</v>
       </c>
       <c r="D48" t="s" s="16">
         <v>14</v>
       </c>
       <c r="E48" t="s" s="15">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F48" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="49" ht="19" customHeight="1">
-      <c r="A49" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B49" s="25">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s" s="26">
-        <v>76</v>
+      <c r="A49" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B49" s="22">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D49" t="s" s="16">
         <v>14</v>
       </c>
-      <c r="E49" t="s" s="14">
-        <v>82</v>
+      <c r="E49" t="s" s="15">
+        <v>83</v>
       </c>
       <c r="F49" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="50" ht="19" customHeight="1">
-      <c r="A50" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B50" s="28">
-        <v>7</v>
-      </c>
-      <c r="C50" t="s" s="29">
-        <v>78</v>
+      <c r="A50" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B50" s="25">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s" s="26">
+        <v>76</v>
       </c>
       <c r="D50" t="s" s="16">
         <v>14</v>
       </c>
       <c r="E50" t="s" s="14">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F50" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="51" ht="19" customHeight="1">
-      <c r="A51" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B51" s="19">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s" s="20">
+      <c r="A51" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B51" s="28">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D51" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E51" t="s" s="14">
+        <v>85</v>
+      </c>
+      <c r="F51" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" ht="19" customHeight="1">
+      <c r="A52" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B52" s="31">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D52" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E52" t="s" s="14">
+        <v>86</v>
+      </c>
+      <c r="F52" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" ht="19" customHeight="1">
+      <c r="A53" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B53" s="19">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D51" t="s" s="16">
-        <v>17</v>
-      </c>
-      <c r="E51" t="s" s="15">
-        <v>84</v>
-      </c>
-      <c r="F51" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" ht="19" customHeight="1">
-      <c r="A52" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B52" s="22">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D52" t="s" s="16">
-        <v>17</v>
-      </c>
-      <c r="E52" t="s" s="14">
-        <v>85</v>
-      </c>
-      <c r="F52" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" ht="19" customHeight="1">
-      <c r="A53" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B53" s="25">
-        <v>7</v>
-      </c>
-      <c r="C53" t="s" s="26">
-        <v>76</v>
       </c>
       <c r="D53" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="E53" t="s" s="14">
-        <v>86</v>
+      <c r="E53" t="s" s="15">
+        <v>87</v>
       </c>
       <c r="F53" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="54" ht="19" customHeight="1">
-      <c r="A54" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B54" s="28">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s" s="29">
-        <v>78</v>
+      <c r="A54" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B54" s="22">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D54" t="s" s="16">
         <v>17</v>
       </c>
       <c r="E54" t="s" s="14">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F54" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="55" ht="19" customHeight="1">
-      <c r="A55" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B55" s="19">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s" s="20">
+      <c r="A55" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B55" s="25">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D55" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E55" t="s" s="14">
+        <v>89</v>
+      </c>
+      <c r="F55" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" ht="19" customHeight="1">
+      <c r="A56" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B56" s="28">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D56" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E56" t="s" s="14">
+        <v>90</v>
+      </c>
+      <c r="F56" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" ht="19" customHeight="1">
+      <c r="A57" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B57" s="31">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D57" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E57" t="s" s="14">
+        <v>91</v>
+      </c>
+      <c r="F57" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" ht="19" customHeight="1">
+      <c r="A58" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B58" s="19">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D55" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E55" t="s" s="17">
-        <v>88</v>
-      </c>
-      <c r="F55" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" ht="19" customHeight="1">
-      <c r="A56" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B56" s="22">
-        <v>7</v>
-      </c>
-      <c r="C56" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D56" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E56" t="s" s="15">
-        <v>89</v>
-      </c>
-      <c r="F56" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" ht="19" customHeight="1">
-      <c r="A57" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B57" s="25">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D57" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E57" t="s" s="17">
-        <v>90</v>
-      </c>
-      <c r="F57" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" ht="19" customHeight="1">
-      <c r="A58" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B58" s="28">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s" s="29">
-        <v>78</v>
       </c>
       <c r="D58" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="E58" t="s" s="14">
-        <v>91</v>
+      <c r="E58" t="s" s="17">
+        <v>92</v>
       </c>
       <c r="F58" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="59" ht="19" customHeight="1">
-      <c r="A59" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B59" s="19">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s" s="20">
-        <v>72</v>
+      <c r="A59" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B59" s="22">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D59" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E59" t="s" s="14">
-        <v>92</v>
+        <v>20</v>
+      </c>
+      <c r="E59" t="s" s="15">
+        <v>93</v>
       </c>
       <c r="F59" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="60" ht="19" customHeight="1">
-      <c r="A60" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B60" s="22">
-        <v>7</v>
-      </c>
-      <c r="C60" t="s" s="23">
-        <v>74</v>
+      <c r="A60" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B60" s="25">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s" s="26">
+        <v>76</v>
       </c>
       <c r="D60" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E60" t="s" s="14">
-        <v>93</v>
+        <v>20</v>
+      </c>
+      <c r="E60" t="s" s="17">
+        <v>94</v>
       </c>
       <c r="F60" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="61" ht="19" customHeight="1">
-      <c r="A61" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B61" s="25">
-        <v>7</v>
-      </c>
-      <c r="C61" t="s" s="26">
-        <v>76</v>
+      <c r="A61" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B61" s="28">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s" s="29">
+        <v>78</v>
       </c>
       <c r="D61" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E61" t="s" s="17">
-        <v>94</v>
+        <v>20</v>
+      </c>
+      <c r="E61" t="s" s="14">
+        <v>95</v>
       </c>
       <c r="F61" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="62" ht="19" customHeight="1">
-      <c r="A62" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B62" s="28">
-        <v>7</v>
-      </c>
-      <c r="C62" t="s" s="29">
-        <v>78</v>
+      <c r="A62" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B62" s="31">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s" s="32">
+        <v>80</v>
       </c>
       <c r="D62" t="s" s="16">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E62" t="s" s="14">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F62" t="s" s="15">
         <v>11</v>
@@ -3101,10 +3180,10 @@
         <v>72</v>
       </c>
       <c r="D63" t="s" s="16">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E63" t="s" s="14">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F63" t="s" s="15">
         <v>11</v>
@@ -3121,10 +3200,10 @@
         <v>74</v>
       </c>
       <c r="D64" t="s" s="16">
-        <v>26</v>
-      </c>
-      <c r="E64" t="s" s="15">
-        <v>97</v>
+        <v>23</v>
+      </c>
+      <c r="E64" t="s" s="14">
+        <v>98</v>
       </c>
       <c r="F64" t="s" s="15">
         <v>11</v>
@@ -3141,10 +3220,10 @@
         <v>76</v>
       </c>
       <c r="D65" t="s" s="16">
-        <v>26</v>
-      </c>
-      <c r="E65" t="s" s="14">
-        <v>98</v>
+        <v>23</v>
+      </c>
+      <c r="E65" t="s" s="17">
+        <v>99</v>
       </c>
       <c r="F65" t="s" s="15">
         <v>11</v>
@@ -3161,330 +3240,330 @@
         <v>78</v>
       </c>
       <c r="D66" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="E66" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="F66" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" ht="19" customHeight="1">
+      <c r="A67" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B67" s="31">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D67" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="E67" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="F67" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" ht="19" customHeight="1">
+      <c r="A68" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B68" s="19">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D68" t="s" s="16">
         <v>26</v>
       </c>
-      <c r="E66" t="s" s="14">
-        <v>99</v>
-      </c>
-      <c r="F66" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" ht="19" customHeight="1">
-      <c r="A67" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B67" s="19">
-        <v>7</v>
-      </c>
-      <c r="C67" t="s" s="20">
+      <c r="E68" t="s" s="14">
+        <v>102</v>
+      </c>
+      <c r="F68" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" ht="19" customHeight="1">
+      <c r="A69" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B69" s="22">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D69" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E69" t="s" s="15">
+        <v>103</v>
+      </c>
+      <c r="F69" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" ht="19" customHeight="1">
+      <c r="A70" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B70" s="25">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D70" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E70" t="s" s="14">
+        <v>104</v>
+      </c>
+      <c r="F70" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" ht="19" customHeight="1">
+      <c r="A71" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B71" s="28">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D71" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E71" t="s" s="14">
+        <v>105</v>
+      </c>
+      <c r="F71" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" ht="19" customHeight="1">
+      <c r="A72" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B72" s="31">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D72" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E72" t="s" s="14">
+        <v>106</v>
+      </c>
+      <c r="F72" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" ht="19" customHeight="1">
+      <c r="A73" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B73" s="19">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D67" t="s" s="16">
+      <c r="D73" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="E67" t="s" s="15">
-        <v>100</v>
-      </c>
-      <c r="F67" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="68" ht="19" customHeight="1">
-      <c r="A68" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B68" s="22">
-        <v>7</v>
-      </c>
-      <c r="C68" t="s" s="23">
+      <c r="E73" t="s" s="15">
+        <v>107</v>
+      </c>
+      <c r="F73" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" ht="19" customHeight="1">
+      <c r="A74" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B74" s="22">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D68" t="s" s="16">
+      <c r="D74" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="E68" t="s" s="14">
-        <v>101</v>
-      </c>
-      <c r="F68" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" ht="19" customHeight="1">
-      <c r="A69" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B69" s="25">
-        <v>7</v>
-      </c>
-      <c r="C69" t="s" s="26">
+      <c r="E74" t="s" s="14">
+        <v>108</v>
+      </c>
+      <c r="F74" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" ht="19" customHeight="1">
+      <c r="A75" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B75" s="25">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D69" t="s" s="16">
+      <c r="D75" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="E69" t="s" s="14">
-        <v>102</v>
-      </c>
-      <c r="F69" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="70" ht="19" customHeight="1">
-      <c r="A70" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B70" s="28">
-        <v>7</v>
-      </c>
-      <c r="C70" t="s" s="29">
+      <c r="E75" t="s" s="14">
+        <v>109</v>
+      </c>
+      <c r="F75" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" ht="19" customHeight="1">
+      <c r="A76" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B76" s="28">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D70" t="s" s="16">
+      <c r="D76" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="E70" t="s" s="14">
-        <v>103</v>
-      </c>
-      <c r="F70" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="71" ht="19" customHeight="1">
-      <c r="A71" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B71" s="19">
-        <v>7</v>
-      </c>
-      <c r="C71" t="s" s="20">
+      <c r="E76" t="s" s="14">
+        <v>110</v>
+      </c>
+      <c r="F76" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" ht="19" customHeight="1">
+      <c r="A77" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B77" s="31">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D77" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E77" t="s" s="14">
+        <v>111</v>
+      </c>
+      <c r="F77" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" ht="19" customHeight="1">
+      <c r="A78" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B78" s="19">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D71" t="s" s="16">
+      <c r="D78" t="s" s="16">
         <v>32</v>
       </c>
-      <c r="E71" t="s" s="15">
-        <v>104</v>
-      </c>
-      <c r="F71" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="72" ht="19" customHeight="1">
-      <c r="A72" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B72" s="22">
-        <v>7</v>
-      </c>
-      <c r="C72" t="s" s="23">
+      <c r="E78" t="s" s="15">
+        <v>112</v>
+      </c>
+      <c r="F78" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" ht="19" customHeight="1">
+      <c r="A79" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B79" s="22">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D72" t="s" s="16">
+      <c r="D79" t="s" s="16">
         <v>32</v>
       </c>
-      <c r="E72" t="s" s="17">
-        <v>105</v>
-      </c>
-      <c r="F72" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="73" ht="19" customHeight="1">
-      <c r="A73" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B73" s="25">
-        <v>7</v>
-      </c>
-      <c r="C73" t="s" s="26">
+      <c r="E79" t="s" s="17">
+        <v>113</v>
+      </c>
+      <c r="F79" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" ht="19" customHeight="1">
+      <c r="A80" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B80" s="25">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D73" t="s" s="16">
+      <c r="D80" t="s" s="16">
         <v>32</v>
       </c>
-      <c r="E73" t="s" s="14">
-        <v>106</v>
-      </c>
-      <c r="F73" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="74" ht="19" customHeight="1">
-      <c r="A74" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B74" s="28">
-        <v>7</v>
-      </c>
-      <c r="C74" t="s" s="29">
+      <c r="E80" t="s" s="14">
+        <v>114</v>
+      </c>
+      <c r="F80" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" ht="19" customHeight="1">
+      <c r="A81" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B81" s="28">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D74" t="s" s="16">
+      <c r="D81" t="s" s="16">
         <v>32</v>
       </c>
-      <c r="E74" t="s" s="14">
-        <v>107</v>
-      </c>
-      <c r="F74" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="75" ht="19" customHeight="1">
-      <c r="A75" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B75" s="19">
-        <v>7</v>
-      </c>
-      <c r="C75" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D75" t="s" s="16">
-        <v>35</v>
-      </c>
-      <c r="E75" t="s" s="14">
-        <v>108</v>
-      </c>
-      <c r="F75" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="76" ht="19" customHeight="1">
-      <c r="A76" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B76" s="22">
-        <v>7</v>
-      </c>
-      <c r="C76" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D76" t="s" s="16">
-        <v>35</v>
-      </c>
-      <c r="E76" t="s" s="14">
-        <v>109</v>
-      </c>
-      <c r="F76" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="77" ht="19" customHeight="1">
-      <c r="A77" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B77" s="25">
-        <v>7</v>
-      </c>
-      <c r="C77" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D77" t="s" s="16">
-        <v>35</v>
-      </c>
-      <c r="E77" t="s" s="14">
-        <v>110</v>
-      </c>
-      <c r="F77" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="78" ht="19" customHeight="1">
-      <c r="A78" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B78" s="28">
-        <v>7</v>
-      </c>
-      <c r="C78" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D78" t="s" s="16">
-        <v>35</v>
-      </c>
-      <c r="E78" t="s" s="14">
-        <v>111</v>
-      </c>
-      <c r="F78" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="79" ht="19" customHeight="1">
-      <c r="A79" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B79" s="19">
-        <v>7</v>
-      </c>
-      <c r="C79" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D79" t="s" s="16">
-        <v>38</v>
-      </c>
-      <c r="E79" t="s" s="15">
-        <v>112</v>
-      </c>
-      <c r="F79" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="80" ht="19" customHeight="1">
-      <c r="A80" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B80" s="22">
-        <v>7</v>
-      </c>
-      <c r="C80" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D80" t="s" s="16">
-        <v>38</v>
-      </c>
-      <c r="E80" t="s" s="15">
-        <v>113</v>
-      </c>
-      <c r="F80" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="81" ht="19" customHeight="1">
-      <c r="A81" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B81" s="25">
-        <v>7</v>
-      </c>
-      <c r="C81" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D81" t="s" s="16">
-        <v>38</v>
-      </c>
       <c r="E81" t="s" s="14">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F81" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="82" ht="19" customHeight="1">
-      <c r="A82" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B82" s="28">
-        <v>7</v>
-      </c>
-      <c r="C82" t="s" s="29">
-        <v>78</v>
+      <c r="A82" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B82" s="31">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s" s="32">
+        <v>80</v>
       </c>
       <c r="D82" t="s" s="16">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E82" t="s" s="14">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F82" t="s" s="15">
         <v>11</v>
@@ -3501,10 +3580,10 @@
         <v>72</v>
       </c>
       <c r="D83" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="E83" t="s" s="15">
-        <v>116</v>
+        <v>35</v>
+      </c>
+      <c r="E83" t="s" s="14">
+        <v>117</v>
       </c>
       <c r="F83" t="s" s="15">
         <v>11</v>
@@ -3521,10 +3600,10 @@
         <v>74</v>
       </c>
       <c r="D84" t="s" s="16">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E84" t="s" s="14">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F84" t="s" s="15">
         <v>11</v>
@@ -3541,10 +3620,10 @@
         <v>76</v>
       </c>
       <c r="D85" t="s" s="16">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E85" t="s" s="14">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F85" t="s" s="15">
         <v>11</v>
@@ -3561,330 +3640,330 @@
         <v>78</v>
       </c>
       <c r="D86" t="s" s="16">
+        <v>35</v>
+      </c>
+      <c r="E86" t="s" s="14">
+        <v>120</v>
+      </c>
+      <c r="F86" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" ht="19" customHeight="1">
+      <c r="A87" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B87" s="31">
+        <v>7</v>
+      </c>
+      <c r="C87" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D87" t="s" s="16">
+        <v>35</v>
+      </c>
+      <c r="E87" t="s" s="14">
+        <v>121</v>
+      </c>
+      <c r="F87" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" ht="19" customHeight="1">
+      <c r="A88" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B88" s="19">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D88" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="E88" t="s" s="15">
+        <v>122</v>
+      </c>
+      <c r="F88" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" ht="19" customHeight="1">
+      <c r="A89" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B89" s="22">
+        <v>7</v>
+      </c>
+      <c r="C89" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D89" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="E89" t="s" s="15">
+        <v>123</v>
+      </c>
+      <c r="F89" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" ht="19" customHeight="1">
+      <c r="A90" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B90" s="25">
+        <v>7</v>
+      </c>
+      <c r="C90" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D90" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="E90" t="s" s="14">
+        <v>124</v>
+      </c>
+      <c r="F90" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" ht="19" customHeight="1">
+      <c r="A91" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B91" s="28">
+        <v>7</v>
+      </c>
+      <c r="C91" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D91" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="E91" t="s" s="14">
+        <v>125</v>
+      </c>
+      <c r="F91" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" ht="19" customHeight="1">
+      <c r="A92" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B92" s="31">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D92" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="E92" t="s" s="14">
+        <v>126</v>
+      </c>
+      <c r="F92" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" ht="19" customHeight="1">
+      <c r="A93" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B93" s="19">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D93" t="s" s="16">
         <v>41</v>
       </c>
-      <c r="E86" t="s" s="14">
-        <v>119</v>
-      </c>
-      <c r="F86" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="87" ht="19" customHeight="1">
-      <c r="A87" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B87" s="19">
-        <v>7</v>
-      </c>
-      <c r="C87" t="s" s="20">
+      <c r="E93" t="s" s="15">
+        <v>127</v>
+      </c>
+      <c r="F93" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" ht="19" customHeight="1">
+      <c r="A94" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B94" s="22">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D94" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E94" t="s" s="14">
+        <v>128</v>
+      </c>
+      <c r="F94" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" ht="19" customHeight="1">
+      <c r="A95" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B95" s="25">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D95" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E95" t="s" s="14">
+        <v>129</v>
+      </c>
+      <c r="F95" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" ht="19" customHeight="1">
+      <c r="A96" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B96" s="28">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D96" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E96" t="s" s="14">
+        <v>130</v>
+      </c>
+      <c r="F96" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" ht="19" customHeight="1">
+      <c r="A97" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B97" s="31">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D97" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E97" t="s" s="14">
+        <v>131</v>
+      </c>
+      <c r="F97" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" ht="19" customHeight="1">
+      <c r="A98" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B98" s="19">
+        <v>7</v>
+      </c>
+      <c r="C98" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D87" t="s" s="16">
+      <c r="D98" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E87" t="s" s="15">
-        <v>120</v>
-      </c>
-      <c r="F87" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="88" ht="19" customHeight="1">
-      <c r="A88" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B88" s="22">
-        <v>7</v>
-      </c>
-      <c r="C88" t="s" s="23">
+      <c r="E98" t="s" s="15">
+        <v>132</v>
+      </c>
+      <c r="F98" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" ht="19" customHeight="1">
+      <c r="A99" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B99" s="22">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D88" t="s" s="16">
+      <c r="D99" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E88" t="s" s="14">
-        <v>121</v>
-      </c>
-      <c r="F88" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="89" ht="19" customHeight="1">
-      <c r="A89" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B89" s="25">
-        <v>7</v>
-      </c>
-      <c r="C89" t="s" s="26">
+      <c r="E99" t="s" s="14">
+        <v>133</v>
+      </c>
+      <c r="F99" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" ht="19" customHeight="1">
+      <c r="A100" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B100" s="25">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D89" t="s" s="16">
+      <c r="D100" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E89" t="s" s="14">
-        <v>122</v>
-      </c>
-      <c r="F89" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="90" ht="19" customHeight="1">
-      <c r="A90" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B90" s="28">
-        <v>7</v>
-      </c>
-      <c r="C90" t="s" s="29">
+      <c r="E100" t="s" s="14">
+        <v>134</v>
+      </c>
+      <c r="F100" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" ht="19" customHeight="1">
+      <c r="A101" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B101" s="28">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D90" t="s" s="16">
+      <c r="D101" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E90" t="s" s="14">
-        <v>123</v>
-      </c>
-      <c r="F90" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="91" ht="19" customHeight="1">
-      <c r="A91" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B91" s="19">
-        <v>7</v>
-      </c>
-      <c r="C91" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D91" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E91" t="s" s="15">
-        <v>124</v>
-      </c>
-      <c r="F91" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="92" ht="19" customHeight="1">
-      <c r="A92" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B92" s="22">
-        <v>7</v>
-      </c>
-      <c r="C92" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D92" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E92" t="s" s="14">
-        <v>125</v>
-      </c>
-      <c r="F92" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="93" ht="19" customHeight="1">
-      <c r="A93" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B93" s="25">
-        <v>7</v>
-      </c>
-      <c r="C93" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D93" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E93" t="s" s="14">
-        <v>126</v>
-      </c>
-      <c r="F93" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="94" ht="19" customHeight="1">
-      <c r="A94" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B94" s="28">
-        <v>7</v>
-      </c>
-      <c r="C94" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D94" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E94" t="s" s="14">
-        <v>127</v>
-      </c>
-      <c r="F94" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="95" ht="19" customHeight="1">
-      <c r="A95" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B95" s="19">
-        <v>7</v>
-      </c>
-      <c r="C95" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D95" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E95" t="s" s="17">
-        <v>128</v>
-      </c>
-      <c r="F95" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="96" ht="19" customHeight="1">
-      <c r="A96" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B96" s="22">
-        <v>7</v>
-      </c>
-      <c r="C96" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D96" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E96" t="s" s="14">
-        <v>129</v>
-      </c>
-      <c r="F96" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="97" ht="19" customHeight="1">
-      <c r="A97" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B97" s="25">
-        <v>7</v>
-      </c>
-      <c r="C97" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D97" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E97" t="s" s="17">
-        <v>130</v>
-      </c>
-      <c r="F97" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="98" ht="19" customHeight="1">
-      <c r="A98" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B98" s="28">
-        <v>7</v>
-      </c>
-      <c r="C98" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D98" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E98" t="s" s="14">
-        <v>131</v>
-      </c>
-      <c r="F98" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="99" ht="19" customHeight="1">
-      <c r="A99" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B99" s="19">
-        <v>7</v>
-      </c>
-      <c r="C99" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D99" t="s" s="16">
-        <v>53</v>
-      </c>
-      <c r="E99" t="s" s="14">
-        <v>132</v>
-      </c>
-      <c r="F99" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="100" ht="19" customHeight="1">
-      <c r="A100" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B100" s="22">
-        <v>7</v>
-      </c>
-      <c r="C100" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D100" t="s" s="16">
-        <v>53</v>
-      </c>
-      <c r="E100" t="s" s="14">
-        <v>133</v>
-      </c>
-      <c r="F100" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="101" ht="19" customHeight="1">
-      <c r="A101" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B101" s="25">
-        <v>7</v>
-      </c>
-      <c r="C101" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D101" t="s" s="16">
-        <v>53</v>
-      </c>
       <c r="E101" t="s" s="14">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F101" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="102" ht="19" customHeight="1">
-      <c r="A102" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B102" s="28">
-        <v>7</v>
-      </c>
-      <c r="C102" t="s" s="29">
-        <v>78</v>
+      <c r="A102" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B102" s="31">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s" s="32">
+        <v>80</v>
       </c>
       <c r="D102" t="s" s="16">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E102" t="s" s="14">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F102" t="s" s="15">
         <v>11</v>
@@ -3901,10 +3980,10 @@
         <v>72</v>
       </c>
       <c r="D103" t="s" s="16">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E103" t="s" s="15">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F103" t="s" s="15">
         <v>11</v>
@@ -3921,10 +4000,10 @@
         <v>74</v>
       </c>
       <c r="D104" t="s" s="16">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E104" t="s" s="14">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F104" t="s" s="15">
         <v>11</v>
@@ -3941,10 +4020,10 @@
         <v>76</v>
       </c>
       <c r="D105" t="s" s="16">
-        <v>56</v>
-      </c>
-      <c r="E105" t="s" s="17">
-        <v>137</v>
+        <v>47</v>
+      </c>
+      <c r="E105" t="s" s="14">
+        <v>139</v>
       </c>
       <c r="F105" t="s" s="15">
         <v>11</v>
@@ -3961,332 +4040,732 @@
         <v>78</v>
       </c>
       <c r="D106" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E106" t="s" s="14">
+        <v>140</v>
+      </c>
+      <c r="F106" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" ht="19" customHeight="1">
+      <c r="A107" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B107" s="31">
+        <v>7</v>
+      </c>
+      <c r="C107" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D107" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E107" t="s" s="14">
+        <v>141</v>
+      </c>
+      <c r="F107" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" ht="19" customHeight="1">
+      <c r="A108" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B108" s="19">
+        <v>7</v>
+      </c>
+      <c r="C108" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D108" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E108" t="s" s="17">
+        <v>142</v>
+      </c>
+      <c r="F108" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" ht="19" customHeight="1">
+      <c r="A109" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B109" s="22">
+        <v>7</v>
+      </c>
+      <c r="C109" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D109" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E109" t="s" s="14">
+        <v>143</v>
+      </c>
+      <c r="F109" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" ht="19" customHeight="1">
+      <c r="A110" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B110" s="25">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D110" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E110" t="s" s="17">
+        <v>144</v>
+      </c>
+      <c r="F110" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="111" ht="19" customHeight="1">
+      <c r="A111" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B111" s="28">
+        <v>7</v>
+      </c>
+      <c r="C111" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D111" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E111" t="s" s="14">
+        <v>145</v>
+      </c>
+      <c r="F111" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" ht="19" customHeight="1">
+      <c r="A112" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B112" s="31">
+        <v>7</v>
+      </c>
+      <c r="C112" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D112" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E112" t="s" s="14">
+        <v>146</v>
+      </c>
+      <c r="F112" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" ht="19" customHeight="1">
+      <c r="A113" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B113" s="19">
+        <v>7</v>
+      </c>
+      <c r="C113" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D113" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E113" t="s" s="14">
+        <v>147</v>
+      </c>
+      <c r="F113" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" ht="19" customHeight="1">
+      <c r="A114" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B114" s="22">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D114" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E114" t="s" s="14">
+        <v>148</v>
+      </c>
+      <c r="F114" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" ht="19" customHeight="1">
+      <c r="A115" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B115" s="25">
+        <v>7</v>
+      </c>
+      <c r="C115" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D115" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E115" t="s" s="14">
+        <v>149</v>
+      </c>
+      <c r="F115" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" ht="19" customHeight="1">
+      <c r="A116" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B116" s="28">
+        <v>7</v>
+      </c>
+      <c r="C116" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D116" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E116" t="s" s="14">
+        <v>150</v>
+      </c>
+      <c r="F116" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" ht="19" customHeight="1">
+      <c r="A117" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B117" s="31">
+        <v>7</v>
+      </c>
+      <c r="C117" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D117" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E117" t="s" s="14">
+        <v>151</v>
+      </c>
+      <c r="F117" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" ht="19" customHeight="1">
+      <c r="A118" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B118" s="19">
+        <v>7</v>
+      </c>
+      <c r="C118" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D118" t="s" s="16">
         <v>56</v>
       </c>
-      <c r="E106" t="s" s="14">
-        <v>138</v>
-      </c>
-      <c r="F106" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="107" ht="19" customHeight="1">
-      <c r="A107" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B107" s="19">
-        <v>7</v>
-      </c>
-      <c r="C107" t="s" s="20">
+      <c r="E118" t="s" s="15">
+        <v>147</v>
+      </c>
+      <c r="F118" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" ht="19" customHeight="1">
+      <c r="A119" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B119" s="22">
+        <v>7</v>
+      </c>
+      <c r="C119" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D119" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E119" t="s" s="14">
+        <v>152</v>
+      </c>
+      <c r="F119" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120" ht="19" customHeight="1">
+      <c r="A120" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B120" s="25">
+        <v>7</v>
+      </c>
+      <c r="C120" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D120" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E120" t="s" s="17">
+        <v>153</v>
+      </c>
+      <c r="F120" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" ht="19" customHeight="1">
+      <c r="A121" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B121" s="28">
+        <v>7</v>
+      </c>
+      <c r="C121" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D121" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E121" t="s" s="14">
+        <v>154</v>
+      </c>
+      <c r="F121" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" ht="19" customHeight="1">
+      <c r="A122" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B122" s="31">
+        <v>7</v>
+      </c>
+      <c r="C122" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D122" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E122" t="s" s="14">
+        <v>155</v>
+      </c>
+      <c r="F122" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123" ht="19" customHeight="1">
+      <c r="A123" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B123" s="19">
+        <v>7</v>
+      </c>
+      <c r="C123" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D107" t="s" s="16">
+      <c r="D123" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E107" t="s" s="15">
-        <v>139</v>
-      </c>
-      <c r="F107" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="108" ht="19" customHeight="1">
-      <c r="A108" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B108" s="22">
-        <v>7</v>
-      </c>
-      <c r="C108" t="s" s="23">
+      <c r="E123" t="s" s="15">
+        <v>156</v>
+      </c>
+      <c r="F123" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" ht="19" customHeight="1">
+      <c r="A124" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B124" s="22">
+        <v>7</v>
+      </c>
+      <c r="C124" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D108" t="s" s="16">
+      <c r="D124" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E108" t="s" s="14">
-        <v>140</v>
-      </c>
-      <c r="F108" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="109" ht="19" customHeight="1">
-      <c r="A109" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B109" s="25">
-        <v>7</v>
-      </c>
-      <c r="C109" t="s" s="26">
+      <c r="E124" t="s" s="14">
+        <v>157</v>
+      </c>
+      <c r="F124" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" ht="19" customHeight="1">
+      <c r="A125" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B125" s="25">
+        <v>7</v>
+      </c>
+      <c r="C125" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D109" t="s" s="16">
+      <c r="D125" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E109" t="s" s="14">
-        <v>141</v>
-      </c>
-      <c r="F109" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="110" ht="19" customHeight="1">
-      <c r="A110" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B110" s="28">
-        <v>7</v>
-      </c>
-      <c r="C110" t="s" s="29">
+      <c r="E125" t="s" s="14">
+        <v>158</v>
+      </c>
+      <c r="F125" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126" ht="19" customHeight="1">
+      <c r="A126" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B126" s="28">
+        <v>7</v>
+      </c>
+      <c r="C126" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D110" t="s" s="16">
+      <c r="D126" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E110" t="s" s="14">
-        <v>142</v>
-      </c>
-      <c r="F110" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="111" ht="19" customHeight="1">
-      <c r="A111" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B111" s="19">
-        <v>7</v>
-      </c>
-      <c r="C111" t="s" s="20">
+      <c r="E126" t="s" s="14">
+        <v>159</v>
+      </c>
+      <c r="F126" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="127" ht="19" customHeight="1">
+      <c r="A127" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B127" s="31">
+        <v>7</v>
+      </c>
+      <c r="C127" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D127" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E127" t="s" s="14">
+        <v>160</v>
+      </c>
+      <c r="F127" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" ht="19" customHeight="1">
+      <c r="A128" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B128" s="19">
+        <v>7</v>
+      </c>
+      <c r="C128" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D111" t="s" s="16">
+      <c r="D128" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E111" t="s" s="15">
-        <v>143</v>
-      </c>
-      <c r="F111" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="112" ht="19" customHeight="1">
-      <c r="A112" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B112" s="22">
-        <v>7</v>
-      </c>
-      <c r="C112" t="s" s="23">
+      <c r="E128" t="s" s="15">
+        <v>161</v>
+      </c>
+      <c r="F128" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="129" ht="19" customHeight="1">
+      <c r="A129" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B129" s="22">
+        <v>7</v>
+      </c>
+      <c r="C129" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D112" t="s" s="16">
+      <c r="D129" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E112" t="s" s="14">
-        <v>144</v>
-      </c>
-      <c r="F112" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="113" ht="19" customHeight="1">
-      <c r="A113" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B113" s="25">
-        <v>7</v>
-      </c>
-      <c r="C113" t="s" s="26">
+      <c r="E129" t="s" s="14">
+        <v>162</v>
+      </c>
+      <c r="F129" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130" ht="19" customHeight="1">
+      <c r="A130" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B130" s="25">
+        <v>7</v>
+      </c>
+      <c r="C130" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D113" t="s" s="16">
+      <c r="D130" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E113" t="s" s="14">
-        <v>145</v>
-      </c>
-      <c r="F113" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="114" ht="19" customHeight="1">
-      <c r="A114" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B114" s="28">
-        <v>7</v>
-      </c>
-      <c r="C114" t="s" s="29">
+      <c r="E130" t="s" s="14">
+        <v>163</v>
+      </c>
+      <c r="F130" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" ht="19" customHeight="1">
+      <c r="A131" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B131" s="28">
+        <v>7</v>
+      </c>
+      <c r="C131" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D114" t="s" s="16">
+      <c r="D131" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E114" t="s" s="14">
-        <v>146</v>
-      </c>
-      <c r="F114" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="115" ht="19" customHeight="1">
-      <c r="A115" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B115" s="19">
-        <v>7</v>
-      </c>
-      <c r="C115" t="s" s="20">
+      <c r="E131" t="s" s="14">
+        <v>164</v>
+      </c>
+      <c r="F131" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="132" ht="19" customHeight="1">
+      <c r="A132" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B132" s="31">
+        <v>7</v>
+      </c>
+      <c r="C132" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D132" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E132" t="s" s="14">
+        <v>165</v>
+      </c>
+      <c r="F132" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133" ht="19" customHeight="1">
+      <c r="A133" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B133" s="19">
+        <v>7</v>
+      </c>
+      <c r="C133" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D115" t="s" s="16">
+      <c r="D133" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E115" t="s" s="15">
-        <v>147</v>
-      </c>
-      <c r="F115" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="116" ht="19" customHeight="1">
-      <c r="A116" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B116" s="22">
-        <v>7</v>
-      </c>
-      <c r="C116" t="s" s="23">
+      <c r="E133" t="s" s="15">
+        <v>166</v>
+      </c>
+      <c r="F133" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" ht="19" customHeight="1">
+      <c r="A134" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B134" s="22">
+        <v>7</v>
+      </c>
+      <c r="C134" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D116" t="s" s="16">
+      <c r="D134" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E116" t="s" s="14">
-        <v>148</v>
-      </c>
-      <c r="F116" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="117" ht="19" customHeight="1">
-      <c r="A117" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B117" s="25">
-        <v>7</v>
-      </c>
-      <c r="C117" t="s" s="26">
+      <c r="E134" t="s" s="14">
+        <v>167</v>
+      </c>
+      <c r="F134" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" ht="19" customHeight="1">
+      <c r="A135" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B135" s="25">
+        <v>7</v>
+      </c>
+      <c r="C135" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D117" t="s" s="16">
+      <c r="D135" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E117" t="s" s="14">
-        <v>149</v>
-      </c>
-      <c r="F117" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="118" ht="19" customHeight="1">
-      <c r="A118" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B118" s="28">
-        <v>7</v>
-      </c>
-      <c r="C118" t="s" s="29">
+      <c r="E135" t="s" s="14">
+        <v>168</v>
+      </c>
+      <c r="F135" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="136" ht="19" customHeight="1">
+      <c r="A136" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B136" s="28">
+        <v>7</v>
+      </c>
+      <c r="C136" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D118" t="s" s="16">
+      <c r="D136" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E118" t="s" s="14">
-        <v>150</v>
-      </c>
-      <c r="F118" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="119" ht="19" customHeight="1">
-      <c r="A119" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B119" s="19">
-        <v>7</v>
-      </c>
-      <c r="C119" t="s" s="20">
+      <c r="E136" t="s" s="14">
+        <v>169</v>
+      </c>
+      <c r="F136" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="137" ht="19" customHeight="1">
+      <c r="A137" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B137" s="31">
+        <v>7</v>
+      </c>
+      <c r="C137" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D137" t="s" s="16">
+        <v>65</v>
+      </c>
+      <c r="E137" t="s" s="14">
+        <v>170</v>
+      </c>
+      <c r="F137" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="138" ht="19" customHeight="1">
+      <c r="A138" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B138" s="19">
+        <v>7</v>
+      </c>
+      <c r="C138" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D119" t="s" s="16">
+      <c r="D138" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E119" t="s" s="15">
-        <v>151</v>
-      </c>
-      <c r="F119" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="120" ht="19" customHeight="1">
-      <c r="A120" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B120" s="22">
-        <v>7</v>
-      </c>
-      <c r="C120" t="s" s="23">
+      <c r="E138" t="s" s="15">
+        <v>171</v>
+      </c>
+      <c r="F138" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="139" ht="19" customHeight="1">
+      <c r="A139" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B139" s="22">
+        <v>7</v>
+      </c>
+      <c r="C139" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D120" t="s" s="16">
+      <c r="D139" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E120" t="s" s="14">
-        <v>152</v>
-      </c>
-      <c r="F120" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="121" ht="19" customHeight="1">
-      <c r="A121" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B121" s="25">
-        <v>7</v>
-      </c>
-      <c r="C121" t="s" s="26">
+      <c r="E139" t="s" s="14">
+        <v>172</v>
+      </c>
+      <c r="F139" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140" ht="19" customHeight="1">
+      <c r="A140" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B140" s="25">
+        <v>7</v>
+      </c>
+      <c r="C140" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D121" t="s" s="16">
+      <c r="D140" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E121" t="s" s="14">
-        <v>153</v>
-      </c>
-      <c r="F121" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="122" ht="19" customHeight="1">
-      <c r="A122" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B122" s="28">
-        <v>7</v>
-      </c>
-      <c r="C122" t="s" s="29">
+      <c r="E140" t="s" s="14">
+        <v>173</v>
+      </c>
+      <c r="F140" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="141" ht="19" customHeight="1">
+      <c r="A141" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B141" s="28">
+        <v>7</v>
+      </c>
+      <c r="C141" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D122" t="s" s="16">
+      <c r="D141" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E122" t="s" s="14">
-        <v>154</v>
-      </c>
-      <c r="F122" t="s" s="15">
+      <c r="E141" t="s" s="14">
+        <v>174</v>
+      </c>
+      <c r="F141" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="142" ht="19" customHeight="1">
+      <c r="A142" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B142" s="31">
+        <v>7</v>
+      </c>
+      <c r="C142" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D142" t="s" s="16">
+        <v>68</v>
+      </c>
+      <c r="E142" t="s" s="14">
+        <v>175</v>
+      </c>
+      <c r="F142" t="s" s="15">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add USs related to cluster domain "Social and Urban Studies" [Sociology]
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
+++ b/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="197">
   <si>
     <t>Tabella 1</t>
   </si>
@@ -259,6 +259,12 @@
     <t>As a social worker, I want to apply adversarial learning techniques to improve the privacy and security of confidential client data, ensuring that sensitive information remains protected while still allowing for effective analysis and decision-making.</t>
   </si>
   <si>
+    <t>Sociology</t>
+  </si>
+  <si>
+    <t>As a social scientist, I want to employ adversarial learning algorithms to explore the impact of media representation on public perception of political candidates, so that I can understand and mitigate the influence of biased media coverage on democratic processes.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply CNN models to analyze satellite imagery and identify changes in urban sprawl over time, helping me understand how demographic shifts affect city planning and development.</t>
   </si>
   <si>
@@ -274,6 +280,9 @@
     <t>As a child welfare advocate, I want to implement CNNs to analyze patterns in child behavior and environmental factors to predict the likelihood of neglect or abuse, facilitating early intervention and protection measures.</t>
   </si>
   <si>
+    <t>As a sociologist, I want to apply CNNs to analyze satellite imagery of urban areas, so that I can study spatial patterns of poverty and urban segregation and propose targeted interventions for social equity.</t>
+  </si>
+  <si>
     <t>As a government official, I want to deploy a conversational agent that can interactively guide citizens through demographic surveys, ensuring accurate data collection and enhancing public engagement in demographic studies.</t>
   </si>
   <si>
@@ -289,6 +298,9 @@
     <t>As a social worker, I want to develop a conversational agent powered by NLP to provide immediate crisis intervention and emotional support to individuals experiencing domestic violence, ensuring they have access to help 24/7.</t>
   </si>
   <si>
+    <t>As a social scientist, I want to deploy a conversational agent with NLP capabilities to conduct virtual focus groups across diverse geographical regions, so that I can explore regional variations in cultural practices and norms affecting social behaviors.</t>
+  </si>
+  <si>
     <t>As a demography data analyst, I want to employ a decision tree algorithm to evaluate the impact of educational attainment levels on population growth rates across various regions, providing insights into educational policies and workforce planning initiatives.</t>
   </si>
   <si>
@@ -304,6 +316,9 @@
     <t>As a child protection specialist, I want to utilize decision trees to prioritize cases of child neglect for investigation, ensuring that limited resources are allocated to the most critical situations where early intervention is crucial.</t>
   </si>
   <si>
+    <t>As a sociologist, I want to use decision trees to analyze survey data and identify key demographic factors influencing voting patterns, so that I can provide insights into political participation across different social groups.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a document classification model to automatically categorize research papers and reports into topics such as fertility rates, aging population trends, and migration patterns, facilitating literature review and data synthesis.</t>
   </si>
   <si>
@@ -319,6 +334,9 @@
     <t>As a social worker, I want to develop a document classification model to automatically categorize incoming client reports into different risk levels, facilitating prioritization of cases requiring urgent intervention.</t>
   </si>
   <si>
+    <t>As a social scientist investigating migration patterns, I want to use document classification to categorize policy documents and legislative texts related to immigration policies across different countries, so that I can compare regulatory approaches and their societal implications.</t>
+  </si>
+  <si>
     <t>As a demography consultant, I need an entity extraction tool to extract key demographic indicators such as birth rates, mortality rates, and migration flows from international demographic databases and reports, facilitating comparative analysis across countries.</t>
   </si>
   <si>
@@ -334,6 +352,9 @@
     <t>As a social worker, I want to develop an entity extraction system to automatically identify and extract key information from intake forms, such as names, addresses, and contact details, to streamline case management processes.</t>
   </si>
   <si>
+    <t>As a sociologist investigating cultural heritage, I want to develop an entity extraction model to identify and classify cultural artifacts mentioned in ethnographic studies and museum catalogs, so that I can preserve and document intangible cultural heritage more effectively.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a feature selection algorithm to identify the most influential demographic variables affecting population density changes in urban areas, helping me prioritize factors for detailed analysis and policy recommendations.</t>
   </si>
   <si>
@@ -349,6 +370,9 @@
     <t>As a social worker, I want to perform feature selection on demographic and socioeconomic variables to identify the most influential factors contributing to homelessness, enabling targeted interventions and resource allocation strategies.</t>
   </si>
   <si>
+    <t>As a sociologist studying healthcare disparities, I want to apply feature selection techniques to identify key socio-demographic factors influencing access to healthcare services among different demographic groups, so that I can recommend policies to enhance healthcare equity.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to address class imbalance in demographic datasets when analyzing rare population characteristics such as extreme age groups or minority ethnicities, ensuring accurate representation and interpretation of demographic trends.</t>
   </si>
   <si>
@@ -364,6 +388,9 @@
     <t>As a domestic violence advocate, I want to apply techniques for managing imbalanced datasets when analyzing police reports and victim statements, improving the accuracy of risk assessments and enhancing safety planning for survivors.</t>
   </si>
   <si>
+    <t>As a social scientist analyzing workforce diversity, I want to mitigate class imbalance in employment data to accurately assess representation of minority groups in corporate sectors, so that I can advocate for inclusive hiring practices and workplace policies.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply k-Nearest Neighbor (k-NN) algorithm to identify similar demographic clusters across different regions based on socio-economic indicators, facilitating comparative demographic analysis and regional policy recommendations.</t>
   </si>
   <si>
@@ -379,6 +406,9 @@
     <t>As a social worker, I want to use KNN to identify similarities in case histories and demographic profiles among clients to better understand common needs and tailor support services accordingly.</t>
   </si>
   <si>
+    <t>As a sociologist studying social media dynamics, I want to develop a keyword extraction model to analyze trending topics and hashtags in online discussions related to political movements, so that I can study digital activism and its impact on societal change.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a keyword extraction algorithm to automatically identify and extract key demographic terms from large volumes of census data and demographic surveys, enabling efficient data summarization and trend analysis.</t>
   </si>
   <si>
@@ -394,6 +424,9 @@
     <t>As a social worker, I want to develop a keyword extraction model to automatically identify key phrases related to domestic violence in client narratives, aiding in the identification of high-risk cases for immediate intervention.</t>
   </si>
   <si>
+    <t>As a sociologist investigating community dynamics, I want to apply k-NN algorithms to analyze demographic data and identify neighborhoods with similar socio-economic profiles, so that I can study residential segregation and its impact on social cohesion.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a multi-label classification model to classify demographic surveys into multiple categories such as age groups, income brackets, and educational levels simultaneously, enabling comprehensive analysis of socio-economic profiles within populations.</t>
   </si>
   <si>
@@ -409,6 +442,9 @@
     <t>As a healthcare coordinator in social work, I want to implement multi-label classification to categorize patient health records into different chronic conditions and mental health disorders, facilitating personalized care plans and treatment strategies.</t>
   </si>
   <si>
+    <t>As a sociologist studying urban communities, I want to apply multi-label classification to categorize demographic data into multiple labels representing socio-economic indicators, housing conditions, and access to public services, so that I can identify clusters of neighborhoods with similar socio-economic profiles.</t>
+  </si>
+  <si>
     <t>As a demographer, I aim to use a neural network to analyze complex demographic datasets and predict future population trends based on historical census data, enabling accurate forecasting for urban planning and policy-making.</t>
   </si>
   <si>
@@ -424,6 +460,9 @@
     <t>As a social worker, I want to develop a neural network model to analyze patterns in client behavior and demographic data to predict the likelihood of recidivism among individuals in correctional facilities, informing rehabilitation programs and support services.</t>
   </si>
   <si>
+    <t>As a social scientist studying public opinion, I want to develop a neural network-based sentiment analysis model to analyze social media content and identify nuanced attitudes towards socio-political issues, so that I can provide insights into public sentiment and policy preferences.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to apply random forest algorithms to analyze demographic survey data and predict household income levels based on demographic variables such as age, education, and employment status, aiding in socio-economic research and policy planning.</t>
   </si>
   <si>
@@ -439,6 +478,9 @@
     <t>As a social worker, I want to develop a random forest model to predict the risk of elderly isolation based on demographic data and living conditions, enabling targeted outreach and support services.</t>
   </si>
   <si>
+    <t>As a social scientist investigating urbanization, I want to apply random forest algorithms to analyze census data and classify neighborhoods into categories based on socio-economic status, housing conditions, and community resources, so that I can study patterns of urban inequality and gentrification.</t>
+  </si>
+  <si>
     <t>As a demography educator, I want to create a semantic similarity tool to compare demographic theories and methodologies from different historical periods and cultural contexts, facilitating comparative demographic studies and theoretical analysis.</t>
   </si>
   <si>
@@ -454,6 +496,9 @@
     <t>As a social worker, I want to develop a semantic similarity model to analyze client case notes and identify similarities in reported symptoms and behavior patterns, facilitating more accurate diagnosis and treatment planning.</t>
   </si>
   <si>
+    <t>As a social scientist studying language evolution, I want to develop a semantic similarity algorithm to compare texts from different historical periods and identify linguistic shifts and semantic changes over time, so that I can trace cultural transformations and societal shifts.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to perform sentiment analysis on social media data to understand public sentiment towards demographic policies and changes, helping to gauge public perception and support for policy initiatives.</t>
   </si>
   <si>
@@ -469,6 +514,9 @@
     <t>As a crisis counselor, I want to implement sentiment analysis on text messages and chat transcripts from crisis interventions to assess the emotional state of clients and tailor responses accordingly.</t>
   </si>
   <si>
+    <t>As a social scientist investigating media influence, I want to apply sentiment analysis to analyze news articles and editorial content to understand media framing of social issues and its impact on public perception and discourse.</t>
+  </si>
+  <si>
     <t>As a special education teacher, I want to utilize speech-to-text tools to convert spoken responses from students with speech disabilities into written text, so that I can facilitate their participation in classroom discussions and assessments.</t>
   </si>
   <si>
@@ -481,6 +529,9 @@
     <t>As a counselor, I want to implement speech to text for transcribing group therapy sessions to capture discussions and insights shared by participants, facilitating comprehensive session reviews and progress tracking.</t>
   </si>
   <si>
+    <t>As a sociologist investigating language use in educational settings, I want to use speech-to-text technology to transcribe classroom discussions and lectures, so that I can analyze teacher-student interactions and learning environments across different socio-economic contexts.</t>
+  </si>
+  <si>
     <t>As a demographer, I need a speech-to-text system to transcribe interviews and focus group discussions on demographic trends and population behaviors, facilitating qualitative data analysis and research insights.</t>
   </si>
   <si>
@@ -496,6 +547,9 @@
     <t>As a social worker, I want to develop a text categorization model to classify incoming client emails into different service categories (e.g., counseling, financial assistance, housing support), ensuring timely and efficient response to client needs.</t>
   </si>
   <si>
+    <t>As a sociologist studying urbanization, I want to apply text categorization techniques to classify policy documents related to urban development into categories such as housing policies, transportation strategies, and environmental sustainability measures, so that I can evaluate the impact of urban policies on community well-being.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply unsupervised clustering algorithms to analyze demographic survey data and identify distinct demographic segments within a population based on socio-economic characteristics, enabling targeted policy interventions and resource allocation strategies.</t>
   </si>
   <si>
@@ -511,6 +565,9 @@
     <t>As a social worker, I want to use unsupervised clustering to group client case notes based on similar behavioral patterns and risk factors, identifying common needs and informing personalized intervention plans.</t>
   </si>
   <si>
+    <t>As a sociologist studying community dynamics, I want to apply unsupervised clustering algorithms to analyze census data and identify clusters of neighborhoods with similar socio-economic profiles, so that I can study patterns of residential segregation and community resilience.</t>
+  </si>
+  <si>
     <t>As a demography educator, I want to utilize voice recognition capabilities to transcribe lectures and seminars on demographic theories and methodologies, providing accessible resources for students and researchers in demography.</t>
   </si>
   <si>
@@ -526,6 +583,9 @@
     <t>As a counselor, I want to develop a voice recognition system to detect emotional cues and distress signals in client speech during counseling sessions, aiding in real-time assessment and intervention.</t>
   </si>
   <si>
+    <t>As a researcher in sociology, I want to develop a voice recognition system to transcribe interviews and focus group discussions with community members, so that I can analyze qualitative data efficiently and uncover themes related to social identity and community dynamics.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to apply word embedding techniques to analyze text data from demographic surveys and reports, identifying semantic relationships between demographic terms and concepts, enhancing data interpretation and insight generation.</t>
   </si>
   <si>
@@ -539,6 +599,9 @@
   </si>
   <si>
     <t>As a social worker, I want to use word embedding techniques to analyze case notes and identify recurring themes and patterns related to client needs and service utilization, guiding personalized service planning.</t>
+  </si>
+  <si>
+    <t>As a social scientist studying public opinion, I want to apply word embedding techniques to analyze survey responses and identify clusters of words representing different attitudes and sentiments towards social issues such as climate change, immigration, and healthcare reform.</t>
   </si>
 </sst>
 </file>
@@ -571,7 +634,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -629,6 +692,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="19"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="20"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -737,7 +806,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -837,6 +906,15 @@
     <xf numFmtId="49" fontId="3" fillId="10" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="11" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,6 +943,7 @@
       <rgbColor rgb="ff00ab8e"/>
       <rgbColor rgb="ff006b65"/>
       <rgbColor rgb="ff88f94e"/>
+      <rgbColor rgb="ff60d836"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1923,7 +2002,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:F142"/>
+  <dimension ref="A2:F162"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1934,7 +2013,7 @@
     <col min="1" max="1" width="29.2422" style="1" customWidth="1"/>
     <col min="2" max="3" width="16.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="231.469" style="1" customWidth="1"/>
+    <col min="5" max="5" width="246.953" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.5781" style="1" customWidth="1"/>
     <col min="7" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
@@ -2870,500 +2949,500 @@
       </c>
     </row>
     <row r="48" ht="19" customHeight="1">
-      <c r="A48" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B48" s="19">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s" s="20">
+      <c r="A48" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B48" s="34">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D48" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="E48" t="s" s="14">
+        <v>83</v>
+      </c>
+      <c r="F48" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" ht="19" customHeight="1">
+      <c r="A49" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B49" s="19">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D48" t="s" s="16">
-        <v>14</v>
-      </c>
-      <c r="E48" t="s" s="15">
-        <v>82</v>
-      </c>
-      <c r="F48" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" ht="19" customHeight="1">
-      <c r="A49" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B49" s="22">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s" s="23">
-        <v>74</v>
       </c>
       <c r="D49" t="s" s="16">
         <v>14</v>
       </c>
       <c r="E49" t="s" s="15">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F49" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="50" ht="19" customHeight="1">
-      <c r="A50" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B50" s="25">
-        <v>7</v>
-      </c>
-      <c r="C50" t="s" s="26">
-        <v>76</v>
+      <c r="A50" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B50" s="22">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D50" t="s" s="16">
         <v>14</v>
       </c>
-      <c r="E50" t="s" s="14">
-        <v>84</v>
+      <c r="E50" t="s" s="15">
+        <v>85</v>
       </c>
       <c r="F50" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="51" ht="19" customHeight="1">
-      <c r="A51" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B51" s="28">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s" s="29">
-        <v>78</v>
+      <c r="A51" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B51" s="25">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s" s="26">
+        <v>76</v>
       </c>
       <c r="D51" t="s" s="16">
         <v>14</v>
       </c>
       <c r="E51" t="s" s="14">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F51" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="52" ht="19" customHeight="1">
-      <c r="A52" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B52" s="31">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s" s="32">
-        <v>80</v>
+      <c r="A52" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B52" s="28">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s" s="29">
+        <v>78</v>
       </c>
       <c r="D52" t="s" s="16">
         <v>14</v>
       </c>
       <c r="E52" t="s" s="14">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F52" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="53" ht="19" customHeight="1">
-      <c r="A53" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B53" s="19">
-        <v>7</v>
-      </c>
-      <c r="C53" t="s" s="20">
+      <c r="A53" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B53" s="31">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D53" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E53" t="s" s="14">
+        <v>88</v>
+      </c>
+      <c r="F53" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" ht="19" customHeight="1">
+      <c r="A54" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B54" s="34">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D54" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E54" t="s" s="14">
+        <v>89</v>
+      </c>
+      <c r="F54" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" ht="19" customHeight="1">
+      <c r="A55" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B55" s="19">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D53" t="s" s="16">
-        <v>17</v>
-      </c>
-      <c r="E53" t="s" s="15">
-        <v>87</v>
-      </c>
-      <c r="F53" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" ht="19" customHeight="1">
-      <c r="A54" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B54" s="22">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D54" t="s" s="16">
-        <v>17</v>
-      </c>
-      <c r="E54" t="s" s="14">
-        <v>88</v>
-      </c>
-      <c r="F54" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" ht="19" customHeight="1">
-      <c r="A55" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B55" s="25">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s" s="26">
-        <v>76</v>
       </c>
       <c r="D55" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="E55" t="s" s="14">
-        <v>89</v>
+      <c r="E55" t="s" s="15">
+        <v>90</v>
       </c>
       <c r="F55" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="56" ht="19" customHeight="1">
-      <c r="A56" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B56" s="28">
-        <v>7</v>
-      </c>
-      <c r="C56" t="s" s="29">
-        <v>78</v>
+      <c r="A56" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B56" s="22">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D56" t="s" s="16">
         <v>17</v>
       </c>
       <c r="E56" t="s" s="14">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F56" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="57" ht="19" customHeight="1">
-      <c r="A57" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B57" s="31">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s" s="32">
-        <v>80</v>
+      <c r="A57" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B57" s="25">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s" s="26">
+        <v>76</v>
       </c>
       <c r="D57" t="s" s="16">
         <v>17</v>
       </c>
       <c r="E57" t="s" s="14">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F57" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="58" ht="19" customHeight="1">
-      <c r="A58" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B58" s="19">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s" s="20">
+      <c r="A58" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B58" s="28">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D58" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E58" t="s" s="14">
+        <v>93</v>
+      </c>
+      <c r="F58" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" ht="19" customHeight="1">
+      <c r="A59" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B59" s="31">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D59" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E59" t="s" s="14">
+        <v>94</v>
+      </c>
+      <c r="F59" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" ht="19" customHeight="1">
+      <c r="A60" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B60" s="34">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D60" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E60" t="s" s="14">
+        <v>95</v>
+      </c>
+      <c r="F60" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" ht="19" customHeight="1">
+      <c r="A61" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B61" s="19">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D58" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E58" t="s" s="17">
-        <v>92</v>
-      </c>
-      <c r="F58" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" ht="19" customHeight="1">
-      <c r="A59" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B59" s="22">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D59" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E59" t="s" s="15">
-        <v>93</v>
-      </c>
-      <c r="F59" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" ht="19" customHeight="1">
-      <c r="A60" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B60" s="25">
-        <v>7</v>
-      </c>
-      <c r="C60" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D60" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E60" t="s" s="17">
-        <v>94</v>
-      </c>
-      <c r="F60" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" ht="19" customHeight="1">
-      <c r="A61" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B61" s="28">
-        <v>7</v>
-      </c>
-      <c r="C61" t="s" s="29">
-        <v>78</v>
       </c>
       <c r="D61" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="E61" t="s" s="14">
-        <v>95</v>
+      <c r="E61" t="s" s="17">
+        <v>96</v>
       </c>
       <c r="F61" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="62" ht="19" customHeight="1">
-      <c r="A62" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B62" s="31">
-        <v>7</v>
-      </c>
-      <c r="C62" t="s" s="32">
-        <v>80</v>
+      <c r="A62" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B62" s="22">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D62" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="E62" t="s" s="14">
-        <v>96</v>
+      <c r="E62" t="s" s="15">
+        <v>97</v>
       </c>
       <c r="F62" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="63" ht="19" customHeight="1">
-      <c r="A63" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B63" s="19">
-        <v>7</v>
-      </c>
-      <c r="C63" t="s" s="20">
+      <c r="A63" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B63" s="25">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D63" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="E63" t="s" s="17">
+        <v>98</v>
+      </c>
+      <c r="F63" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" ht="19" customHeight="1">
+      <c r="A64" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B64" s="28">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D64" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="E64" t="s" s="14">
+        <v>99</v>
+      </c>
+      <c r="F64" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" ht="19" customHeight="1">
+      <c r="A65" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B65" s="31">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D65" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="E65" t="s" s="14">
+        <v>100</v>
+      </c>
+      <c r="F65" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" ht="19" customHeight="1">
+      <c r="A66" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B66" s="34">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D66" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="E66" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="F66" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" ht="19" customHeight="1">
+      <c r="A67" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B67" s="19">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D63" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E63" t="s" s="14">
-        <v>97</v>
-      </c>
-      <c r="F63" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" ht="19" customHeight="1">
-      <c r="A64" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B64" s="22">
-        <v>7</v>
-      </c>
-      <c r="C64" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D64" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E64" t="s" s="14">
-        <v>98</v>
-      </c>
-      <c r="F64" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" ht="19" customHeight="1">
-      <c r="A65" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B65" s="25">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D65" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E65" t="s" s="17">
-        <v>99</v>
-      </c>
-      <c r="F65" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" ht="19" customHeight="1">
-      <c r="A66" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B66" s="28">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D66" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E66" t="s" s="14">
-        <v>100</v>
-      </c>
-      <c r="F66" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" ht="19" customHeight="1">
-      <c r="A67" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B67" s="31">
-        <v>7</v>
-      </c>
-      <c r="C67" t="s" s="32">
-        <v>80</v>
       </c>
       <c r="D67" t="s" s="16">
         <v>23</v>
       </c>
       <c r="E67" t="s" s="14">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F67" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="68" ht="19" customHeight="1">
-      <c r="A68" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B68" s="19">
-        <v>7</v>
-      </c>
-      <c r="C68" t="s" s="20">
-        <v>72</v>
+      <c r="A68" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B68" s="22">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D68" t="s" s="16">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E68" t="s" s="14">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F68" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="69" ht="19" customHeight="1">
-      <c r="A69" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B69" s="22">
-        <v>7</v>
-      </c>
-      <c r="C69" t="s" s="23">
-        <v>74</v>
+      <c r="A69" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B69" s="25">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s" s="26">
+        <v>76</v>
       </c>
       <c r="D69" t="s" s="16">
-        <v>26</v>
-      </c>
-      <c r="E69" t="s" s="15">
-        <v>103</v>
+        <v>23</v>
+      </c>
+      <c r="E69" t="s" s="17">
+        <v>104</v>
       </c>
       <c r="F69" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="70" ht="19" customHeight="1">
-      <c r="A70" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B70" s="25">
-        <v>7</v>
-      </c>
-      <c r="C70" t="s" s="26">
-        <v>76</v>
+      <c r="A70" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B70" s="28">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s" s="29">
+        <v>78</v>
       </c>
       <c r="D70" t="s" s="16">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E70" t="s" s="14">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F70" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="71" ht="19" customHeight="1">
-      <c r="A71" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B71" s="28">
-        <v>7</v>
-      </c>
-      <c r="C71" t="s" s="29">
-        <v>78</v>
+      <c r="A71" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B71" s="31">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s" s="32">
+        <v>80</v>
       </c>
       <c r="D71" t="s" s="16">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E71" t="s" s="14">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F71" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="72" ht="19" customHeight="1">
-      <c r="A72" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B72" s="31">
-        <v>7</v>
-      </c>
-      <c r="C72" t="s" s="32">
-        <v>80</v>
+      <c r="A72" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B72" s="34">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s" s="35">
+        <v>82</v>
       </c>
       <c r="D72" t="s" s="16">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E72" t="s" s="14">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F72" t="s" s="15">
         <v>11</v>
@@ -3380,10 +3459,10 @@
         <v>72</v>
       </c>
       <c r="D73" t="s" s="16">
-        <v>29</v>
-      </c>
-      <c r="E73" t="s" s="15">
-        <v>107</v>
+        <v>26</v>
+      </c>
+      <c r="E73" t="s" s="14">
+        <v>108</v>
       </c>
       <c r="F73" t="s" s="15">
         <v>11</v>
@@ -3400,10 +3479,10 @@
         <v>74</v>
       </c>
       <c r="D74" t="s" s="16">
-        <v>29</v>
-      </c>
-      <c r="E74" t="s" s="14">
-        <v>108</v>
+        <v>26</v>
+      </c>
+      <c r="E74" t="s" s="15">
+        <v>109</v>
       </c>
       <c r="F74" t="s" s="15">
         <v>11</v>
@@ -3420,10 +3499,10 @@
         <v>76</v>
       </c>
       <c r="D75" t="s" s="16">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E75" t="s" s="14">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F75" t="s" s="15">
         <v>11</v>
@@ -3440,10 +3519,10 @@
         <v>78</v>
       </c>
       <c r="D76" t="s" s="16">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E76" t="s" s="14">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F76" t="s" s="15">
         <v>11</v>
@@ -3460,510 +3539,510 @@
         <v>80</v>
       </c>
       <c r="D77" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E77" t="s" s="14">
+        <v>112</v>
+      </c>
+      <c r="F77" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" ht="19" customHeight="1">
+      <c r="A78" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B78" s="34">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D78" t="s" s="16">
+        <v>26</v>
+      </c>
+      <c r="E78" t="s" s="14">
+        <v>113</v>
+      </c>
+      <c r="F78" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" ht="19" customHeight="1">
+      <c r="A79" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B79" s="19">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D79" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="E77" t="s" s="14">
-        <v>111</v>
-      </c>
-      <c r="F77" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="78" ht="19" customHeight="1">
-      <c r="A78" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B78" s="19">
-        <v>7</v>
-      </c>
-      <c r="C78" t="s" s="20">
+      <c r="E79" t="s" s="15">
+        <v>114</v>
+      </c>
+      <c r="F79" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" ht="19" customHeight="1">
+      <c r="A80" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B80" s="22">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D80" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E80" t="s" s="14">
+        <v>115</v>
+      </c>
+      <c r="F80" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" ht="19" customHeight="1">
+      <c r="A81" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B81" s="25">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D81" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E81" t="s" s="14">
+        <v>116</v>
+      </c>
+      <c r="F81" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" ht="19" customHeight="1">
+      <c r="A82" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B82" s="28">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D82" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E82" t="s" s="14">
+        <v>117</v>
+      </c>
+      <c r="F82" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" ht="19" customHeight="1">
+      <c r="A83" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B83" s="31">
+        <v>7</v>
+      </c>
+      <c r="C83" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D83" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E83" t="s" s="14">
+        <v>118</v>
+      </c>
+      <c r="F83" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" ht="19" customHeight="1">
+      <c r="A84" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B84" s="34">
+        <v>7</v>
+      </c>
+      <c r="C84" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D84" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E84" t="s" s="14">
+        <v>119</v>
+      </c>
+      <c r="F84" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" ht="19" customHeight="1">
+      <c r="A85" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B85" s="19">
+        <v>7</v>
+      </c>
+      <c r="C85" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D78" t="s" s="16">
+      <c r="D85" t="s" s="16">
         <v>32</v>
       </c>
-      <c r="E78" t="s" s="15">
-        <v>112</v>
-      </c>
-      <c r="F78" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="79" ht="19" customHeight="1">
-      <c r="A79" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B79" s="22">
-        <v>7</v>
-      </c>
-      <c r="C79" t="s" s="23">
+      <c r="E85" t="s" s="15">
+        <v>120</v>
+      </c>
+      <c r="F85" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" ht="19" customHeight="1">
+      <c r="A86" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B86" s="22">
+        <v>7</v>
+      </c>
+      <c r="C86" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D79" t="s" s="16">
+      <c r="D86" t="s" s="16">
         <v>32</v>
       </c>
-      <c r="E79" t="s" s="17">
-        <v>113</v>
-      </c>
-      <c r="F79" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="80" ht="19" customHeight="1">
-      <c r="A80" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B80" s="25">
-        <v>7</v>
-      </c>
-      <c r="C80" t="s" s="26">
+      <c r="E86" t="s" s="17">
+        <v>121</v>
+      </c>
+      <c r="F86" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" ht="19" customHeight="1">
+      <c r="A87" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B87" s="25">
+        <v>7</v>
+      </c>
+      <c r="C87" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D80" t="s" s="16">
+      <c r="D87" t="s" s="16">
         <v>32</v>
       </c>
-      <c r="E80" t="s" s="14">
-        <v>114</v>
-      </c>
-      <c r="F80" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="81" ht="19" customHeight="1">
-      <c r="A81" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B81" s="28">
-        <v>7</v>
-      </c>
-      <c r="C81" t="s" s="29">
+      <c r="E87" t="s" s="14">
+        <v>122</v>
+      </c>
+      <c r="F87" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" ht="19" customHeight="1">
+      <c r="A88" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B88" s="28">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D81" t="s" s="16">
+      <c r="D88" t="s" s="16">
         <v>32</v>
       </c>
-      <c r="E81" t="s" s="14">
-        <v>115</v>
-      </c>
-      <c r="F81" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="82" ht="19" customHeight="1">
-      <c r="A82" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B82" s="31">
-        <v>7</v>
-      </c>
-      <c r="C82" t="s" s="32">
+      <c r="E88" t="s" s="14">
+        <v>123</v>
+      </c>
+      <c r="F88" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" ht="19" customHeight="1">
+      <c r="A89" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B89" s="31">
+        <v>7</v>
+      </c>
+      <c r="C89" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D82" t="s" s="16">
+      <c r="D89" t="s" s="16">
         <v>32</v>
       </c>
-      <c r="E82" t="s" s="14">
-        <v>116</v>
-      </c>
-      <c r="F82" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="83" ht="19" customHeight="1">
-      <c r="A83" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B83" s="19">
-        <v>7</v>
-      </c>
-      <c r="C83" t="s" s="20">
+      <c r="E89" t="s" s="14">
+        <v>124</v>
+      </c>
+      <c r="F89" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" ht="19" customHeight="1">
+      <c r="A90" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B90" s="34">
+        <v>7</v>
+      </c>
+      <c r="C90" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D90" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E90" t="s" s="14">
+        <v>125</v>
+      </c>
+      <c r="F90" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" ht="19" customHeight="1">
+      <c r="A91" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B91" s="19">
+        <v>7</v>
+      </c>
+      <c r="C91" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D83" t="s" s="16">
+      <c r="D91" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E83" t="s" s="14">
-        <v>117</v>
-      </c>
-      <c r="F83" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="84" ht="19" customHeight="1">
-      <c r="A84" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B84" s="22">
-        <v>7</v>
-      </c>
-      <c r="C84" t="s" s="23">
+      <c r="E91" t="s" s="14">
+        <v>126</v>
+      </c>
+      <c r="F91" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" ht="19" customHeight="1">
+      <c r="A92" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B92" s="22">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D84" t="s" s="16">
+      <c r="D92" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E84" t="s" s="14">
-        <v>118</v>
-      </c>
-      <c r="F84" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="85" ht="19" customHeight="1">
-      <c r="A85" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B85" s="25">
-        <v>7</v>
-      </c>
-      <c r="C85" t="s" s="26">
+      <c r="E92" t="s" s="14">
+        <v>127</v>
+      </c>
+      <c r="F92" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" ht="19" customHeight="1">
+      <c r="A93" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B93" s="25">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D85" t="s" s="16">
+      <c r="D93" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E85" t="s" s="14">
-        <v>119</v>
-      </c>
-      <c r="F85" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="86" ht="19" customHeight="1">
-      <c r="A86" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B86" s="28">
-        <v>7</v>
-      </c>
-      <c r="C86" t="s" s="29">
+      <c r="E93" t="s" s="14">
+        <v>128</v>
+      </c>
+      <c r="F93" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" ht="19" customHeight="1">
+      <c r="A94" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B94" s="28">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D86" t="s" s="16">
+      <c r="D94" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E86" t="s" s="14">
-        <v>120</v>
-      </c>
-      <c r="F86" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="87" ht="19" customHeight="1">
-      <c r="A87" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B87" s="31">
-        <v>7</v>
-      </c>
-      <c r="C87" t="s" s="32">
+      <c r="E94" t="s" s="14">
+        <v>129</v>
+      </c>
+      <c r="F94" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" ht="19" customHeight="1">
+      <c r="A95" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B95" s="31">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D87" t="s" s="16">
+      <c r="D95" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E87" t="s" s="14">
-        <v>121</v>
-      </c>
-      <c r="F87" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="88" ht="19" customHeight="1">
-      <c r="A88" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B88" s="19">
-        <v>7</v>
-      </c>
-      <c r="C88" t="s" s="20">
+      <c r="E95" t="s" s="14">
+        <v>130</v>
+      </c>
+      <c r="F95" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" ht="19" customHeight="1">
+      <c r="A96" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B96" s="34">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D96" t="s" s="16">
+        <v>35</v>
+      </c>
+      <c r="E96" t="s" s="14">
+        <v>131</v>
+      </c>
+      <c r="F96" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" ht="19" customHeight="1">
+      <c r="A97" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B97" s="19">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D88" t="s" s="16">
+      <c r="D97" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E88" t="s" s="15">
-        <v>122</v>
-      </c>
-      <c r="F88" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="89" ht="19" customHeight="1">
-      <c r="A89" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B89" s="22">
-        <v>7</v>
-      </c>
-      <c r="C89" t="s" s="23">
+      <c r="E97" t="s" s="15">
+        <v>132</v>
+      </c>
+      <c r="F97" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" ht="19" customHeight="1">
+      <c r="A98" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B98" s="22">
+        <v>7</v>
+      </c>
+      <c r="C98" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D89" t="s" s="16">
+      <c r="D98" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E89" t="s" s="15">
-        <v>123</v>
-      </c>
-      <c r="F89" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="90" ht="19" customHeight="1">
-      <c r="A90" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B90" s="25">
-        <v>7</v>
-      </c>
-      <c r="C90" t="s" s="26">
+      <c r="E98" t="s" s="15">
+        <v>133</v>
+      </c>
+      <c r="F98" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" ht="19" customHeight="1">
+      <c r="A99" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B99" s="25">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D90" t="s" s="16">
+      <c r="D99" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E90" t="s" s="14">
-        <v>124</v>
-      </c>
-      <c r="F90" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="91" ht="19" customHeight="1">
-      <c r="A91" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B91" s="28">
-        <v>7</v>
-      </c>
-      <c r="C91" t="s" s="29">
+      <c r="E99" t="s" s="14">
+        <v>134</v>
+      </c>
+      <c r="F99" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" ht="19" customHeight="1">
+      <c r="A100" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B100" s="28">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D91" t="s" s="16">
+      <c r="D100" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E91" t="s" s="14">
-        <v>125</v>
-      </c>
-      <c r="F91" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="92" ht="19" customHeight="1">
-      <c r="A92" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B92" s="31">
-        <v>7</v>
-      </c>
-      <c r="C92" t="s" s="32">
+      <c r="E100" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="F100" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" ht="19" customHeight="1">
+      <c r="A101" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B101" s="31">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D92" t="s" s="16">
+      <c r="D101" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E92" t="s" s="14">
-        <v>126</v>
-      </c>
-      <c r="F92" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="93" ht="19" customHeight="1">
-      <c r="A93" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B93" s="19">
-        <v>7</v>
-      </c>
-      <c r="C93" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D93" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="E93" t="s" s="15">
-        <v>127</v>
-      </c>
-      <c r="F93" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="94" ht="19" customHeight="1">
-      <c r="A94" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B94" s="22">
-        <v>7</v>
-      </c>
-      <c r="C94" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D94" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="E94" t="s" s="14">
-        <v>128</v>
-      </c>
-      <c r="F94" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="95" ht="19" customHeight="1">
-      <c r="A95" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B95" s="25">
-        <v>7</v>
-      </c>
-      <c r="C95" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D95" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="E95" t="s" s="14">
-        <v>129</v>
-      </c>
-      <c r="F95" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="96" ht="19" customHeight="1">
-      <c r="A96" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B96" s="28">
-        <v>7</v>
-      </c>
-      <c r="C96" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D96" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="E96" t="s" s="14">
-        <v>130</v>
-      </c>
-      <c r="F96" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="97" ht="19" customHeight="1">
-      <c r="A97" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B97" s="31">
-        <v>7</v>
-      </c>
-      <c r="C97" t="s" s="32">
-        <v>80</v>
-      </c>
-      <c r="D97" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="E97" t="s" s="14">
-        <v>131</v>
-      </c>
-      <c r="F97" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="98" ht="19" customHeight="1">
-      <c r="A98" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B98" s="19">
-        <v>7</v>
-      </c>
-      <c r="C98" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D98" t="s" s="16">
-        <v>44</v>
-      </c>
-      <c r="E98" t="s" s="15">
-        <v>132</v>
-      </c>
-      <c r="F98" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="99" ht="19" customHeight="1">
-      <c r="A99" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B99" s="22">
-        <v>7</v>
-      </c>
-      <c r="C99" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D99" t="s" s="16">
-        <v>44</v>
-      </c>
-      <c r="E99" t="s" s="14">
-        <v>133</v>
-      </c>
-      <c r="F99" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="100" ht="19" customHeight="1">
-      <c r="A100" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B100" s="25">
-        <v>7</v>
-      </c>
-      <c r="C100" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D100" t="s" s="16">
-        <v>44</v>
-      </c>
-      <c r="E100" t="s" s="14">
-        <v>134</v>
-      </c>
-      <c r="F100" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="101" ht="19" customHeight="1">
-      <c r="A101" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B101" s="28">
-        <v>7</v>
-      </c>
-      <c r="C101" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D101" t="s" s="16">
-        <v>44</v>
-      </c>
       <c r="E101" t="s" s="14">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F101" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="102" ht="19" customHeight="1">
-      <c r="A102" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B102" s="31">
-        <v>7</v>
-      </c>
-      <c r="C102" t="s" s="32">
-        <v>80</v>
+      <c r="A102" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B102" s="34">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s" s="35">
+        <v>82</v>
       </c>
       <c r="D102" t="s" s="16">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E102" t="s" s="14">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F102" t="s" s="15">
         <v>11</v>
@@ -3980,10 +4059,10 @@
         <v>72</v>
       </c>
       <c r="D103" t="s" s="16">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E103" t="s" s="15">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F103" t="s" s="15">
         <v>11</v>
@@ -4000,10 +4079,10 @@
         <v>74</v>
       </c>
       <c r="D104" t="s" s="16">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E104" t="s" s="14">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F104" t="s" s="15">
         <v>11</v>
@@ -4020,10 +4099,10 @@
         <v>76</v>
       </c>
       <c r="D105" t="s" s="16">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E105" t="s" s="14">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F105" t="s" s="15">
         <v>11</v>
@@ -4040,10 +4119,10 @@
         <v>78</v>
       </c>
       <c r="D106" t="s" s="16">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E106" t="s" s="14">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F106" t="s" s="15">
         <v>11</v>
@@ -4060,510 +4139,510 @@
         <v>80</v>
       </c>
       <c r="D107" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E107" t="s" s="14">
+        <v>142</v>
+      </c>
+      <c r="F107" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" ht="19" customHeight="1">
+      <c r="A108" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B108" s="34">
+        <v>7</v>
+      </c>
+      <c r="C108" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D108" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E108" t="s" s="14">
+        <v>143</v>
+      </c>
+      <c r="F108" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" ht="19" customHeight="1">
+      <c r="A109" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B109" s="19">
+        <v>7</v>
+      </c>
+      <c r="C109" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D109" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="E109" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="F109" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" ht="19" customHeight="1">
+      <c r="A110" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B110" s="22">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D110" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="E110" t="s" s="14">
+        <v>145</v>
+      </c>
+      <c r="F110" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="111" ht="19" customHeight="1">
+      <c r="A111" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B111" s="25">
+        <v>7</v>
+      </c>
+      <c r="C111" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D111" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="E111" t="s" s="14">
+        <v>146</v>
+      </c>
+      <c r="F111" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" ht="19" customHeight="1">
+      <c r="A112" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B112" s="28">
+        <v>7</v>
+      </c>
+      <c r="C112" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D112" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="E112" t="s" s="14">
+        <v>147</v>
+      </c>
+      <c r="F112" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" ht="19" customHeight="1">
+      <c r="A113" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B113" s="31">
+        <v>7</v>
+      </c>
+      <c r="C113" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D113" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="E113" t="s" s="14">
+        <v>148</v>
+      </c>
+      <c r="F113" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" ht="19" customHeight="1">
+      <c r="A114" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B114" s="34">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D114" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="E114" t="s" s="14">
+        <v>149</v>
+      </c>
+      <c r="F114" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" ht="19" customHeight="1">
+      <c r="A115" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B115" s="19">
+        <v>7</v>
+      </c>
+      <c r="C115" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D115" t="s" s="16">
         <v>47</v>
       </c>
-      <c r="E107" t="s" s="14">
-        <v>141</v>
-      </c>
-      <c r="F107" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="108" ht="19" customHeight="1">
-      <c r="A108" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B108" s="19">
-        <v>7</v>
-      </c>
-      <c r="C108" t="s" s="20">
+      <c r="E115" t="s" s="15">
+        <v>150</v>
+      </c>
+      <c r="F115" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" ht="19" customHeight="1">
+      <c r="A116" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B116" s="22">
+        <v>7</v>
+      </c>
+      <c r="C116" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D116" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E116" t="s" s="14">
+        <v>151</v>
+      </c>
+      <c r="F116" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" ht="19" customHeight="1">
+      <c r="A117" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B117" s="25">
+        <v>7</v>
+      </c>
+      <c r="C117" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D117" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E117" t="s" s="14">
+        <v>152</v>
+      </c>
+      <c r="F117" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" ht="19" customHeight="1">
+      <c r="A118" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B118" s="28">
+        <v>7</v>
+      </c>
+      <c r="C118" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D118" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E118" t="s" s="14">
+        <v>153</v>
+      </c>
+      <c r="F118" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" ht="19" customHeight="1">
+      <c r="A119" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B119" s="31">
+        <v>7</v>
+      </c>
+      <c r="C119" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D119" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E119" t="s" s="14">
+        <v>154</v>
+      </c>
+      <c r="F119" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120" ht="19" customHeight="1">
+      <c r="A120" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B120" s="34">
+        <v>7</v>
+      </c>
+      <c r="C120" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D120" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E120" t="s" s="14">
+        <v>155</v>
+      </c>
+      <c r="F120" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" ht="19" customHeight="1">
+      <c r="A121" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B121" s="19">
+        <v>7</v>
+      </c>
+      <c r="C121" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D108" t="s" s="16">
+      <c r="D121" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="E108" t="s" s="17">
-        <v>142</v>
-      </c>
-      <c r="F108" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="109" ht="19" customHeight="1">
-      <c r="A109" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B109" s="22">
-        <v>7</v>
-      </c>
-      <c r="C109" t="s" s="23">
+      <c r="E121" t="s" s="17">
+        <v>156</v>
+      </c>
+      <c r="F121" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" ht="19" customHeight="1">
+      <c r="A122" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B122" s="22">
+        <v>7</v>
+      </c>
+      <c r="C122" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D109" t="s" s="16">
+      <c r="D122" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="E109" t="s" s="14">
-        <v>143</v>
-      </c>
-      <c r="F109" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="110" ht="19" customHeight="1">
-      <c r="A110" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B110" s="25">
-        <v>7</v>
-      </c>
-      <c r="C110" t="s" s="26">
+      <c r="E122" t="s" s="14">
+        <v>157</v>
+      </c>
+      <c r="F122" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123" ht="19" customHeight="1">
+      <c r="A123" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B123" s="25">
+        <v>7</v>
+      </c>
+      <c r="C123" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D110" t="s" s="16">
+      <c r="D123" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="E110" t="s" s="17">
-        <v>144</v>
-      </c>
-      <c r="F110" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="111" ht="19" customHeight="1">
-      <c r="A111" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B111" s="28">
-        <v>7</v>
-      </c>
-      <c r="C111" t="s" s="29">
+      <c r="E123" t="s" s="17">
+        <v>158</v>
+      </c>
+      <c r="F123" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" ht="19" customHeight="1">
+      <c r="A124" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B124" s="28">
+        <v>7</v>
+      </c>
+      <c r="C124" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D111" t="s" s="16">
+      <c r="D124" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="E111" t="s" s="14">
-        <v>145</v>
-      </c>
-      <c r="F111" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="112" ht="19" customHeight="1">
-      <c r="A112" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B112" s="31">
-        <v>7</v>
-      </c>
-      <c r="C112" t="s" s="32">
+      <c r="E124" t="s" s="14">
+        <v>159</v>
+      </c>
+      <c r="F124" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" ht="19" customHeight="1">
+      <c r="A125" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B125" s="31">
+        <v>7</v>
+      </c>
+      <c r="C125" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D112" t="s" s="16">
+      <c r="D125" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="E112" t="s" s="14">
-        <v>146</v>
-      </c>
-      <c r="F112" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="113" ht="19" customHeight="1">
-      <c r="A113" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B113" s="19">
-        <v>7</v>
-      </c>
-      <c r="C113" t="s" s="20">
+      <c r="E125" t="s" s="14">
+        <v>160</v>
+      </c>
+      <c r="F125" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126" ht="19" customHeight="1">
+      <c r="A126" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B126" s="34">
+        <v>7</v>
+      </c>
+      <c r="C126" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D126" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E126" t="s" s="14">
+        <v>161</v>
+      </c>
+      <c r="F126" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="127" ht="19" customHeight="1">
+      <c r="A127" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B127" s="19">
+        <v>7</v>
+      </c>
+      <c r="C127" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D113" t="s" s="16">
+      <c r="D127" t="s" s="16">
         <v>53</v>
       </c>
-      <c r="E113" t="s" s="14">
-        <v>147</v>
-      </c>
-      <c r="F113" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="114" ht="19" customHeight="1">
-      <c r="A114" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B114" s="22">
-        <v>7</v>
-      </c>
-      <c r="C114" t="s" s="23">
+      <c r="E127" t="s" s="14">
+        <v>162</v>
+      </c>
+      <c r="F127" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" ht="19" customHeight="1">
+      <c r="A128" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B128" s="22">
+        <v>7</v>
+      </c>
+      <c r="C128" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D114" t="s" s="16">
+      <c r="D128" t="s" s="16">
         <v>53</v>
       </c>
-      <c r="E114" t="s" s="14">
-        <v>148</v>
-      </c>
-      <c r="F114" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="115" ht="19" customHeight="1">
-      <c r="A115" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B115" s="25">
-        <v>7</v>
-      </c>
-      <c r="C115" t="s" s="26">
+      <c r="E128" t="s" s="14">
+        <v>163</v>
+      </c>
+      <c r="F128" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="129" ht="19" customHeight="1">
+      <c r="A129" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B129" s="25">
+        <v>7</v>
+      </c>
+      <c r="C129" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D115" t="s" s="16">
+      <c r="D129" t="s" s="16">
         <v>53</v>
       </c>
-      <c r="E115" t="s" s="14">
-        <v>149</v>
-      </c>
-      <c r="F115" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="116" ht="19" customHeight="1">
-      <c r="A116" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B116" s="28">
-        <v>7</v>
-      </c>
-      <c r="C116" t="s" s="29">
+      <c r="E129" t="s" s="14">
+        <v>164</v>
+      </c>
+      <c r="F129" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130" ht="19" customHeight="1">
+      <c r="A130" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B130" s="28">
+        <v>7</v>
+      </c>
+      <c r="C130" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D116" t="s" s="16">
+      <c r="D130" t="s" s="16">
         <v>53</v>
       </c>
-      <c r="E116" t="s" s="14">
-        <v>150</v>
-      </c>
-      <c r="F116" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="117" ht="19" customHeight="1">
-      <c r="A117" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B117" s="31">
-        <v>7</v>
-      </c>
-      <c r="C117" t="s" s="32">
+      <c r="E130" t="s" s="14">
+        <v>165</v>
+      </c>
+      <c r="F130" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" ht="19" customHeight="1">
+      <c r="A131" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B131" s="31">
+        <v>7</v>
+      </c>
+      <c r="C131" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D117" t="s" s="16">
+      <c r="D131" t="s" s="16">
         <v>53</v>
       </c>
-      <c r="E117" t="s" s="14">
-        <v>151</v>
-      </c>
-      <c r="F117" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="118" ht="19" customHeight="1">
-      <c r="A118" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B118" s="19">
-        <v>7</v>
-      </c>
-      <c r="C118" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D118" t="s" s="16">
-        <v>56</v>
-      </c>
-      <c r="E118" t="s" s="15">
-        <v>147</v>
-      </c>
-      <c r="F118" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="119" ht="19" customHeight="1">
-      <c r="A119" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B119" s="22">
-        <v>7</v>
-      </c>
-      <c r="C119" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D119" t="s" s="16">
-        <v>56</v>
-      </c>
-      <c r="E119" t="s" s="14">
-        <v>152</v>
-      </c>
-      <c r="F119" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="120" ht="19" customHeight="1">
-      <c r="A120" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B120" s="25">
-        <v>7</v>
-      </c>
-      <c r="C120" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D120" t="s" s="16">
-        <v>56</v>
-      </c>
-      <c r="E120" t="s" s="17">
-        <v>153</v>
-      </c>
-      <c r="F120" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="121" ht="19" customHeight="1">
-      <c r="A121" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B121" s="28">
-        <v>7</v>
-      </c>
-      <c r="C121" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D121" t="s" s="16">
-        <v>56</v>
-      </c>
-      <c r="E121" t="s" s="14">
-        <v>154</v>
-      </c>
-      <c r="F121" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="122" ht="19" customHeight="1">
-      <c r="A122" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B122" s="31">
-        <v>7</v>
-      </c>
-      <c r="C122" t="s" s="32">
-        <v>80</v>
-      </c>
-      <c r="D122" t="s" s="16">
-        <v>56</v>
-      </c>
-      <c r="E122" t="s" s="14">
-        <v>155</v>
-      </c>
-      <c r="F122" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="123" ht="19" customHeight="1">
-      <c r="A123" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B123" s="19">
-        <v>7</v>
-      </c>
-      <c r="C123" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D123" t="s" s="16">
-        <v>59</v>
-      </c>
-      <c r="E123" t="s" s="15">
-        <v>156</v>
-      </c>
-      <c r="F123" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="124" ht="19" customHeight="1">
-      <c r="A124" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B124" s="22">
-        <v>7</v>
-      </c>
-      <c r="C124" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D124" t="s" s="16">
-        <v>59</v>
-      </c>
-      <c r="E124" t="s" s="14">
-        <v>157</v>
-      </c>
-      <c r="F124" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="125" ht="19" customHeight="1">
-      <c r="A125" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B125" s="25">
-        <v>7</v>
-      </c>
-      <c r="C125" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D125" t="s" s="16">
-        <v>59</v>
-      </c>
-      <c r="E125" t="s" s="14">
-        <v>158</v>
-      </c>
-      <c r="F125" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="126" ht="19" customHeight="1">
-      <c r="A126" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B126" s="28">
-        <v>7</v>
-      </c>
-      <c r="C126" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D126" t="s" s="16">
-        <v>59</v>
-      </c>
-      <c r="E126" t="s" s="14">
-        <v>159</v>
-      </c>
-      <c r="F126" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="127" ht="19" customHeight="1">
-      <c r="A127" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B127" s="31">
-        <v>7</v>
-      </c>
-      <c r="C127" t="s" s="32">
-        <v>80</v>
-      </c>
-      <c r="D127" t="s" s="16">
-        <v>59</v>
-      </c>
-      <c r="E127" t="s" s="14">
-        <v>160</v>
-      </c>
-      <c r="F127" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="128" ht="19" customHeight="1">
-      <c r="A128" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B128" s="19">
-        <v>7</v>
-      </c>
-      <c r="C128" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D128" t="s" s="16">
-        <v>62</v>
-      </c>
-      <c r="E128" t="s" s="15">
-        <v>161</v>
-      </c>
-      <c r="F128" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="129" ht="19" customHeight="1">
-      <c r="A129" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B129" s="22">
-        <v>7</v>
-      </c>
-      <c r="C129" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D129" t="s" s="16">
-        <v>62</v>
-      </c>
-      <c r="E129" t="s" s="14">
-        <v>162</v>
-      </c>
-      <c r="F129" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="130" ht="19" customHeight="1">
-      <c r="A130" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B130" s="25">
-        <v>7</v>
-      </c>
-      <c r="C130" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D130" t="s" s="16">
-        <v>62</v>
-      </c>
-      <c r="E130" t="s" s="14">
-        <v>163</v>
-      </c>
-      <c r="F130" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="131" ht="19" customHeight="1">
-      <c r="A131" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B131" s="28">
-        <v>7</v>
-      </c>
-      <c r="C131" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D131" t="s" s="16">
-        <v>62</v>
-      </c>
       <c r="E131" t="s" s="14">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F131" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="132" ht="19" customHeight="1">
-      <c r="A132" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B132" s="31">
-        <v>7</v>
-      </c>
-      <c r="C132" t="s" s="32">
-        <v>80</v>
+      <c r="A132" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B132" s="34">
+        <v>7</v>
+      </c>
+      <c r="C132" t="s" s="35">
+        <v>82</v>
       </c>
       <c r="D132" t="s" s="16">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E132" t="s" s="14">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F132" t="s" s="15">
         <v>11</v>
@@ -4580,10 +4659,10 @@
         <v>72</v>
       </c>
       <c r="D133" t="s" s="16">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E133" t="s" s="15">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F133" t="s" s="15">
         <v>11</v>
@@ -4600,10 +4679,10 @@
         <v>74</v>
       </c>
       <c r="D134" t="s" s="16">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E134" t="s" s="14">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F134" t="s" s="15">
         <v>11</v>
@@ -4620,10 +4699,10 @@
         <v>76</v>
       </c>
       <c r="D135" t="s" s="16">
-        <v>65</v>
-      </c>
-      <c r="E135" t="s" s="14">
-        <v>168</v>
+        <v>56</v>
+      </c>
+      <c r="E135" t="s" s="17">
+        <v>169</v>
       </c>
       <c r="F135" t="s" s="15">
         <v>11</v>
@@ -4640,10 +4719,10 @@
         <v>78</v>
       </c>
       <c r="D136" t="s" s="16">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E136" t="s" s="14">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F136" t="s" s="15">
         <v>11</v>
@@ -4660,112 +4739,512 @@
         <v>80</v>
       </c>
       <c r="D137" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E137" t="s" s="14">
+        <v>171</v>
+      </c>
+      <c r="F137" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="138" ht="19" customHeight="1">
+      <c r="A138" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B138" s="34">
+        <v>7</v>
+      </c>
+      <c r="C138" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D138" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E138" t="s" s="14">
+        <v>172</v>
+      </c>
+      <c r="F138" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="139" ht="19" customHeight="1">
+      <c r="A139" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B139" s="19">
+        <v>7</v>
+      </c>
+      <c r="C139" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D139" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E139" t="s" s="15">
+        <v>173</v>
+      </c>
+      <c r="F139" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140" ht="19" customHeight="1">
+      <c r="A140" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B140" s="22">
+        <v>7</v>
+      </c>
+      <c r="C140" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D140" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E140" t="s" s="14">
+        <v>174</v>
+      </c>
+      <c r="F140" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="141" ht="19" customHeight="1">
+      <c r="A141" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B141" s="25">
+        <v>7</v>
+      </c>
+      <c r="C141" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D141" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E141" t="s" s="14">
+        <v>175</v>
+      </c>
+      <c r="F141" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="142" ht="19" customHeight="1">
+      <c r="A142" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B142" s="28">
+        <v>7</v>
+      </c>
+      <c r="C142" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D142" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E142" t="s" s="14">
+        <v>176</v>
+      </c>
+      <c r="F142" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="143" ht="19" customHeight="1">
+      <c r="A143" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B143" s="31">
+        <v>7</v>
+      </c>
+      <c r="C143" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D143" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E143" t="s" s="14">
+        <v>177</v>
+      </c>
+      <c r="F143" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="144" ht="19" customHeight="1">
+      <c r="A144" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B144" s="34">
+        <v>7</v>
+      </c>
+      <c r="C144" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D144" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E144" t="s" s="14">
+        <v>178</v>
+      </c>
+      <c r="F144" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" ht="19" customHeight="1">
+      <c r="A145" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B145" s="19">
+        <v>7</v>
+      </c>
+      <c r="C145" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D145" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E145" t="s" s="15">
+        <v>179</v>
+      </c>
+      <c r="F145" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="146" ht="19" customHeight="1">
+      <c r="A146" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B146" s="22">
+        <v>7</v>
+      </c>
+      <c r="C146" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D146" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E146" t="s" s="14">
+        <v>180</v>
+      </c>
+      <c r="F146" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="147" ht="19" customHeight="1">
+      <c r="A147" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B147" s="25">
+        <v>7</v>
+      </c>
+      <c r="C147" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D147" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E147" t="s" s="14">
+        <v>181</v>
+      </c>
+      <c r="F147" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="148" ht="19" customHeight="1">
+      <c r="A148" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B148" s="28">
+        <v>7</v>
+      </c>
+      <c r="C148" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D148" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E148" t="s" s="14">
+        <v>182</v>
+      </c>
+      <c r="F148" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="149" ht="19" customHeight="1">
+      <c r="A149" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B149" s="31">
+        <v>7</v>
+      </c>
+      <c r="C149" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D149" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E149" t="s" s="14">
+        <v>183</v>
+      </c>
+      <c r="F149" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="150" ht="19" customHeight="1">
+      <c r="A150" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B150" s="34">
+        <v>7</v>
+      </c>
+      <c r="C150" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D150" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E150" t="s" s="14">
+        <v>184</v>
+      </c>
+      <c r="F150" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="151" ht="19" customHeight="1">
+      <c r="A151" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B151" s="19">
+        <v>7</v>
+      </c>
+      <c r="C151" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D151" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E137" t="s" s="14">
-        <v>170</v>
-      </c>
-      <c r="F137" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="138" ht="19" customHeight="1">
-      <c r="A138" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B138" s="19">
-        <v>7</v>
-      </c>
-      <c r="C138" t="s" s="20">
+      <c r="E151" t="s" s="15">
+        <v>185</v>
+      </c>
+      <c r="F151" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="152" ht="19" customHeight="1">
+      <c r="A152" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B152" s="22">
+        <v>7</v>
+      </c>
+      <c r="C152" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D152" t="s" s="16">
+        <v>65</v>
+      </c>
+      <c r="E152" t="s" s="14">
+        <v>186</v>
+      </c>
+      <c r="F152" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="153" ht="19" customHeight="1">
+      <c r="A153" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B153" s="25">
+        <v>7</v>
+      </c>
+      <c r="C153" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D153" t="s" s="16">
+        <v>65</v>
+      </c>
+      <c r="E153" t="s" s="14">
+        <v>187</v>
+      </c>
+      <c r="F153" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="154" ht="19" customHeight="1">
+      <c r="A154" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B154" s="28">
+        <v>7</v>
+      </c>
+      <c r="C154" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D154" t="s" s="16">
+        <v>65</v>
+      </c>
+      <c r="E154" t="s" s="14">
+        <v>188</v>
+      </c>
+      <c r="F154" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="155" ht="19" customHeight="1">
+      <c r="A155" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B155" s="31">
+        <v>7</v>
+      </c>
+      <c r="C155" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D155" t="s" s="16">
+        <v>65</v>
+      </c>
+      <c r="E155" t="s" s="14">
+        <v>189</v>
+      </c>
+      <c r="F155" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="156" ht="19" customHeight="1">
+      <c r="A156" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B156" s="34">
+        <v>7</v>
+      </c>
+      <c r="C156" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D156" t="s" s="16">
+        <v>65</v>
+      </c>
+      <c r="E156" t="s" s="14">
+        <v>190</v>
+      </c>
+      <c r="F156" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="157" ht="19" customHeight="1">
+      <c r="A157" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B157" s="19">
+        <v>7</v>
+      </c>
+      <c r="C157" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D138" t="s" s="16">
+      <c r="D157" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E138" t="s" s="15">
-        <v>171</v>
-      </c>
-      <c r="F138" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="139" ht="19" customHeight="1">
-      <c r="A139" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B139" s="22">
-        <v>7</v>
-      </c>
-      <c r="C139" t="s" s="23">
+      <c r="E157" t="s" s="15">
+        <v>191</v>
+      </c>
+      <c r="F157" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="158" ht="19" customHeight="1">
+      <c r="A158" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B158" s="22">
+        <v>7</v>
+      </c>
+      <c r="C158" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D139" t="s" s="16">
+      <c r="D158" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E139" t="s" s="14">
-        <v>172</v>
-      </c>
-      <c r="F139" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="140" ht="19" customHeight="1">
-      <c r="A140" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B140" s="25">
-        <v>7</v>
-      </c>
-      <c r="C140" t="s" s="26">
+      <c r="E158" t="s" s="14">
+        <v>192</v>
+      </c>
+      <c r="F158" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" ht="19" customHeight="1">
+      <c r="A159" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B159" s="25">
+        <v>7</v>
+      </c>
+      <c r="C159" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D140" t="s" s="16">
+      <c r="D159" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E140" t="s" s="14">
-        <v>173</v>
-      </c>
-      <c r="F140" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="141" ht="19" customHeight="1">
-      <c r="A141" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B141" s="28">
-        <v>7</v>
-      </c>
-      <c r="C141" t="s" s="29">
+      <c r="E159" t="s" s="14">
+        <v>193</v>
+      </c>
+      <c r="F159" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="160" ht="19" customHeight="1">
+      <c r="A160" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B160" s="28">
+        <v>7</v>
+      </c>
+      <c r="C160" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D141" t="s" s="16">
+      <c r="D160" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E141" t="s" s="14">
-        <v>174</v>
-      </c>
-      <c r="F141" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="142" ht="19" customHeight="1">
-      <c r="A142" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B142" s="31">
-        <v>7</v>
-      </c>
-      <c r="C142" t="s" s="32">
+      <c r="E160" t="s" s="14">
+        <v>194</v>
+      </c>
+      <c r="F160" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="161" ht="19" customHeight="1">
+      <c r="A161" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B161" s="31">
+        <v>7</v>
+      </c>
+      <c r="C161" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D142" t="s" s="16">
+      <c r="D161" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E142" t="s" s="14">
-        <v>175</v>
-      </c>
-      <c r="F142" t="s" s="15">
+      <c r="E161" t="s" s="14">
+        <v>195</v>
+      </c>
+      <c r="F161" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="162" ht="19" customHeight="1">
+      <c r="A162" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B162" s="34">
+        <v>7</v>
+      </c>
+      <c r="C162" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D162" t="s" s="16">
+        <v>68</v>
+      </c>
+      <c r="E162" t="s" s="14">
+        <v>196</v>
+      </c>
+      <c r="F162" t="s" s="15">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add USs related to cluster domain "Social and Urban Studies" [Transportation]
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
+++ b/refair-server/datasets/Chain-of-Thought Dataset/CoTDataset-2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="218">
   <si>
     <t>Tabella 1</t>
   </si>
@@ -265,6 +265,12 @@
     <t>As a social scientist, I want to employ adversarial learning algorithms to explore the impact of media representation on public perception of political candidates, so that I can understand and mitigate the influence of biased media coverage on democratic processes.</t>
   </si>
   <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>As a traffic management specialist, I want to use adversarial learning models to detect and mitigate adversarial attacks on traffic signal control systems, ensuring reliable and secure traffic flow in smart cities.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply CNN models to analyze satellite imagery and identify changes in urban sprawl over time, helping me understand how demographic shifts affect city planning and development.</t>
   </si>
   <si>
@@ -283,6 +289,9 @@
     <t>As a sociologist, I want to apply CNNs to analyze satellite imagery of urban areas, so that I can study spatial patterns of poverty and urban segregation and propose targeted interventions for social equity.</t>
   </si>
   <si>
+    <t>As a traffic analyst, I want to implement CNN architectures to accurately count and classify vehicles from surveillance camera footage, facilitating better traffic flow management and optimizing infrastructure planning.</t>
+  </si>
+  <si>
     <t>As a government official, I want to deploy a conversational agent that can interactively guide citizens through demographic surveys, ensuring accurate data collection and enhancing public engagement in demographic studies.</t>
   </si>
   <si>
@@ -301,6 +310,9 @@
     <t>As a social scientist, I want to deploy a conversational agent with NLP capabilities to conduct virtual focus groups across diverse geographical regions, so that I can explore regional variations in cultural practices and norms affecting social behaviors.</t>
   </si>
   <si>
+    <t>As a commuter, I want a conversational agent integrated into the transportation app to provide real-time updates on bus schedules and delays, so that I can plan my journey more effectively.</t>
+  </si>
+  <si>
     <t>As a demography data analyst, I want to employ a decision tree algorithm to evaluate the impact of educational attainment levels on population growth rates across various regions, providing insights into educational policies and workforce planning initiatives.</t>
   </si>
   <si>
@@ -319,6 +331,9 @@
     <t>As a sociologist, I want to use decision trees to analyze survey data and identify key demographic factors influencing voting patterns, so that I can provide insights into political participation across different social groups.</t>
   </si>
   <si>
+    <t>As a traffic engineer, I want to develop a decision tree model to classify different types of traffic incidents based on historical data, aiding in quick response and effective management of emergency services.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a document classification model to automatically categorize research papers and reports into topics such as fertility rates, aging population trends, and migration patterns, facilitating literature review and data synthesis.</t>
   </si>
   <si>
@@ -337,6 +352,9 @@
     <t>As a social scientist investigating migration patterns, I want to use document classification to categorize policy documents and legislative texts related to immigration policies across different countries, so that I can compare regulatory approaches and their societal implications.</t>
   </si>
   <si>
+    <t>As a logistics coordinator, I want to develop a document classification system using machine learning to automatically categorize shipping manifests into different freight categories, streamlining customs clearance processes.</t>
+  </si>
+  <si>
     <t>As a demography consultant, I need an entity extraction tool to extract key demographic indicators such as birth rates, mortality rates, and migration flows from international demographic databases and reports, facilitating comparative analysis across countries.</t>
   </si>
   <si>
@@ -355,6 +373,9 @@
     <t>As a sociologist investigating cultural heritage, I want to develop an entity extraction model to identify and classify cultural artifacts mentioned in ethnographic studies and museum catalogs, so that I can preserve and document intangible cultural heritage more effectively.</t>
   </si>
   <si>
+    <t>As a maintenance supervisor for railway systems, I want to employ entity extraction models to automatically identify and categorize components and maintenance activities mentioned in maintenance reports, facilitating efficient maintenance scheduling.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a feature selection algorithm to identify the most influential demographic variables affecting population density changes in urban areas, helping me prioritize factors for detailed analysis and policy recommendations.</t>
   </si>
   <si>
@@ -373,6 +394,9 @@
     <t>As a sociologist studying healthcare disparities, I want to apply feature selection techniques to identify key socio-demographic factors influencing access to healthcare services among different demographic groups, so that I can recommend policies to enhance healthcare equity.</t>
   </si>
   <si>
+    <t>As a traffic engineer, I want to perform feature selection on traffic sensor data to identify the most relevant factors influencing traffic flow, enabling more accurate predictive models for congestion management.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to address class imbalance in demographic datasets when analyzing rare population characteristics such as extreme age groups or minority ethnicities, ensuring accurate representation and interpretation of demographic trends.</t>
   </si>
   <si>
@@ -391,6 +415,9 @@
     <t>As a social scientist analyzing workforce diversity, I want to mitigate class imbalance in employment data to accurately assess representation of minority groups in corporate sectors, so that I can advocate for inclusive hiring practices and workplace policies.</t>
   </si>
   <si>
+    <t>As a logistics coordinator, I want to manage imbalanced data in freight delay incidents to prioritize corrective actions and optimize supply chain resilience, ensuring timely delivery and customer satisfaction.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply k-Nearest Neighbor (k-NN) algorithm to identify similar demographic clusters across different regions based on socio-economic indicators, facilitating comparative demographic analysis and regional policy recommendations.</t>
   </si>
   <si>
@@ -409,6 +436,9 @@
     <t>As a sociologist studying social media dynamics, I want to develop a keyword extraction model to analyze trending topics and hashtags in online discussions related to political movements, so that I can study digital activism and its impact on societal change.</t>
   </si>
   <si>
+    <t>As a transportation planner, I want to implement keyword extraction techniques on public feedback surveys to extract key concerns related to public transport services, guiding improvements in service quality and customer satisfaction.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a keyword extraction algorithm to automatically identify and extract key demographic terms from large volumes of census data and demographic surveys, enabling efficient data summarization and trend analysis.</t>
   </si>
   <si>
@@ -427,6 +457,9 @@
     <t>As a sociologist investigating community dynamics, I want to apply k-NN algorithms to analyze demographic data and identify neighborhoods with similar socio-economic profiles, so that I can study residential segregation and its impact on social cohesion.</t>
   </si>
   <si>
+    <t>As a logistics manager, I want to implement a k-Nearest Neighbor approach to optimize vehicle routing by recommending nearest distribution centers based on real-time delivery demands and traffic conditions.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need a multi-label classification model to classify demographic surveys into multiple categories such as age groups, income brackets, and educational levels simultaneously, enabling comprehensive analysis of socio-economic profiles within populations.</t>
   </si>
   <si>
@@ -445,6 +478,9 @@
     <t>As a sociologist studying urban communities, I want to apply multi-label classification to categorize demographic data into multiple labels representing socio-economic indicators, housing conditions, and access to public services, so that I can identify clusters of neighborhoods with similar socio-economic profiles.</t>
   </si>
   <si>
+    <t>As a public transport operator, I want to develop a multi-label classification system to classify public transport routes based on service types (express, local, shuttle) and peak hour usage patterns (morning rush, evening peak), optimizing route planning and resource allocation.</t>
+  </si>
+  <si>
     <t>As a demographer, I aim to use a neural network to analyze complex demographic datasets and predict future population trends based on historical census data, enabling accurate forecasting for urban planning and policy-making.</t>
   </si>
   <si>
@@ -463,6 +499,9 @@
     <t>As a social scientist studying public opinion, I want to develop a neural network-based sentiment analysis model to analyze social media content and identify nuanced attitudes towards socio-political issues, so that I can provide insights into public sentiment and policy preferences.</t>
   </si>
   <si>
+    <t>As a transportation engineer, I want to design a neural network model to predict traffic flow dynamics at intersections based on real-time sensor data, improving traffic signal timing and reducing congestion.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to apply random forest algorithms to analyze demographic survey data and predict household income levels based on demographic variables such as age, education, and employment status, aiding in socio-economic research and policy planning.</t>
   </si>
   <si>
@@ -481,6 +520,9 @@
     <t>As a social scientist investigating urbanization, I want to apply random forest algorithms to analyze census data and classify neighborhoods into categories based on socio-economic status, housing conditions, and community resources, so that I can study patterns of urban inequality and gentrification.</t>
   </si>
   <si>
+    <t>As a public transport planner, I want to develop a random forest model to predict ridership levels for bus and subway services based on factors such as day of the week, weather conditions, and local events, optimizing service frequencies and resource allocation.</t>
+  </si>
+  <si>
     <t>As a demography educator, I want to create a semantic similarity tool to compare demographic theories and methodologies from different historical periods and cultural contexts, facilitating comparative demographic studies and theoretical analysis.</t>
   </si>
   <si>
@@ -499,6 +541,9 @@
     <t>As a social scientist studying language evolution, I want to develop a semantic similarity algorithm to compare texts from different historical periods and identify linguistic shifts and semantic changes over time, so that I can trace cultural transformations and societal shifts.</t>
   </si>
   <si>
+    <t>As a logistics coordinator, I want to apply semantic similarity models to analyze similarities in delivery routes and optimize truck dispatching schedules, reducing transportation costs and improving delivery efficiency.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to perform sentiment analysis on social media data to understand public sentiment towards demographic policies and changes, helping to gauge public perception and support for policy initiatives.</t>
   </si>
   <si>
@@ -517,6 +562,9 @@
     <t>As a social scientist investigating media influence, I want to apply sentiment analysis to analyze news articles and editorial content to understand media framing of social issues and its impact on public perception and discourse.</t>
   </si>
   <si>
+    <t>As a public transport operator, I want to use sentiment analysis on passenger reviews and complaints to identify recurring issues and prioritize service improvements on specific routes or modes of transport.</t>
+  </si>
+  <si>
     <t>As a special education teacher, I want to utilize speech-to-text tools to convert spoken responses from students with speech disabilities into written text, so that I can facilitate their participation in classroom discussions and assessments.</t>
   </si>
   <si>
@@ -532,6 +580,9 @@
     <t>As a sociologist investigating language use in educational settings, I want to use speech-to-text technology to transcribe classroom discussions and lectures, so that I can analyze teacher-student interactions and learning environments across different socio-economic contexts.</t>
   </si>
   <si>
+    <t>As a logistics manager, I want to integrate speech to text functionality into warehouse operations to transcribe verbal inventory updates and shipment instructions, reducing manual data entry errors and improving efficiency.</t>
+  </si>
+  <si>
     <t>As a demographer, I need a speech-to-text system to transcribe interviews and focus group discussions on demographic trends and population behaviors, facilitating qualitative data analysis and research insights.</t>
   </si>
   <si>
@@ -550,6 +601,9 @@
     <t>As a sociologist studying urbanization, I want to apply text categorization techniques to classify policy documents related to urban development into categories such as housing policies, transportation strategies, and environmental sustainability measures, so that I can evaluate the impact of urban policies on community well-being.</t>
   </si>
   <si>
+    <t>As a logistics coordinator, I want to develop a text categorization model to classify customer service emails into different categories such as complaints, inquiries, and feedback, improving response times and customer satisfaction in freight transportation services.</t>
+  </si>
+  <si>
     <t>As a demographer, I need to apply unsupervised clustering algorithms to analyze demographic survey data and identify distinct demographic segments within a population based on socio-economic characteristics, enabling targeted policy interventions and resource allocation strategies.</t>
   </si>
   <si>
@@ -568,6 +622,9 @@
     <t>As a sociologist studying community dynamics, I want to apply unsupervised clustering algorithms to analyze census data and identify clusters of neighborhoods with similar socio-economic profiles, so that I can study patterns of residential segregation and community resilience.</t>
   </si>
   <si>
+    <t>As a logistics coordinator, I want to implement unsupervised clustering to group shipping routes based on geographical proximity, traffic conditions, and delivery deadlines, optimizing route planning and reducing transportation costs.</t>
+  </si>
+  <si>
     <t>As a demography educator, I want to utilize voice recognition capabilities to transcribe lectures and seminars on demographic theories and methodologies, providing accessible resources for students and researchers in demography.</t>
   </si>
   <si>
@@ -586,6 +643,9 @@
     <t>As a researcher in sociology, I want to develop a voice recognition system to transcribe interviews and focus group discussions with community members, so that I can analyze qualitative data efficiently and uncover themes related to social identity and community dynamics.</t>
   </si>
   <si>
+    <t>As a public transport dispatcher, I want to implement voice recognition technology to accurately interpret driver communications from onboard radios, facilitating real-time updates and coordination of bus routes and schedules.</t>
+  </si>
+  <si>
     <t>As a demography researcher, I need to apply word embedding techniques to analyze text data from demographic surveys and reports, identifying semantic relationships between demographic terms and concepts, enhancing data interpretation and insight generation.</t>
   </si>
   <si>
@@ -602,6 +662,9 @@
   </si>
   <si>
     <t>As a social scientist studying public opinion, I want to apply word embedding techniques to analyze survey responses and identify clusters of words representing different attitudes and sentiments towards social issues such as climate change, immigration, and healthcare reform.</t>
+  </si>
+  <si>
+    <t>As a city planner, I want to leverage word embedding algorithms to analyze textual descriptions of urban transport infrastructure projects and stakeholder feedback, identifying key themes and sentiments to inform project prioritization and community engagement strategies.</t>
   </si>
 </sst>
 </file>
@@ -634,7 +697,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -698,6 +761,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="20"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="21"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -806,7 +875,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -915,6 +984,15 @@
     <xf numFmtId="49" fontId="3" fillId="11" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="12" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -944,6 +1022,7 @@
       <rgbColor rgb="ff006b65"/>
       <rgbColor rgb="ff88f94e"/>
       <rgbColor rgb="ff60d836"/>
+      <rgbColor rgb="ff1cb000"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2002,7 +2081,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:F162"/>
+  <dimension ref="A2:F182"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2969,720 +3048,720 @@
       </c>
     </row>
     <row r="49" ht="19" customHeight="1">
-      <c r="A49" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B49" s="19">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s" s="20">
+      <c r="A49" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B49" s="37">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D49" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s" s="14">
+        <v>85</v>
+      </c>
+      <c r="F49" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" ht="19" customHeight="1">
+      <c r="A50" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B50" s="19">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D49" t="s" s="16">
-        <v>14</v>
-      </c>
-      <c r="E49" t="s" s="15">
-        <v>84</v>
-      </c>
-      <c r="F49" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" ht="19" customHeight="1">
-      <c r="A50" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B50" s="22">
-        <v>7</v>
-      </c>
-      <c r="C50" t="s" s="23">
-        <v>74</v>
       </c>
       <c r="D50" t="s" s="16">
         <v>14</v>
       </c>
       <c r="E50" t="s" s="15">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F50" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="51" ht="19" customHeight="1">
-      <c r="A51" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B51" s="25">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s" s="26">
-        <v>76</v>
+      <c r="A51" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B51" s="22">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D51" t="s" s="16">
         <v>14</v>
       </c>
-      <c r="E51" t="s" s="14">
-        <v>86</v>
+      <c r="E51" t="s" s="15">
+        <v>87</v>
       </c>
       <c r="F51" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="52" ht="19" customHeight="1">
-      <c r="A52" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B52" s="28">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s" s="29">
-        <v>78</v>
+      <c r="A52" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B52" s="25">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s" s="26">
+        <v>76</v>
       </c>
       <c r="D52" t="s" s="16">
         <v>14</v>
       </c>
       <c r="E52" t="s" s="14">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F52" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="53" ht="19" customHeight="1">
-      <c r="A53" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B53" s="31">
-        <v>7</v>
-      </c>
-      <c r="C53" t="s" s="32">
-        <v>80</v>
+      <c r="A53" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B53" s="28">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s" s="29">
+        <v>78</v>
       </c>
       <c r="D53" t="s" s="16">
         <v>14</v>
       </c>
       <c r="E53" t="s" s="14">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F53" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="54" ht="19" customHeight="1">
-      <c r="A54" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B54" s="34">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s" s="35">
-        <v>82</v>
+      <c r="A54" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B54" s="31">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s" s="32">
+        <v>80</v>
       </c>
       <c r="D54" t="s" s="16">
         <v>14</v>
       </c>
       <c r="E54" t="s" s="14">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F54" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="55" ht="19" customHeight="1">
-      <c r="A55" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B55" s="19">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s" s="20">
+      <c r="A55" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B55" s="34">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D55" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E55" t="s" s="14">
+        <v>91</v>
+      </c>
+      <c r="F55" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" ht="19" customHeight="1">
+      <c r="A56" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B56" s="37">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D56" t="s" s="16">
+        <v>14</v>
+      </c>
+      <c r="E56" t="s" s="14">
+        <v>92</v>
+      </c>
+      <c r="F56" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" ht="19" customHeight="1">
+      <c r="A57" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B57" s="19">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D55" t="s" s="16">
-        <v>17</v>
-      </c>
-      <c r="E55" t="s" s="15">
-        <v>90</v>
-      </c>
-      <c r="F55" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" ht="19" customHeight="1">
-      <c r="A56" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B56" s="22">
-        <v>7</v>
-      </c>
-      <c r="C56" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D56" t="s" s="16">
-        <v>17</v>
-      </c>
-      <c r="E56" t="s" s="14">
-        <v>91</v>
-      </c>
-      <c r="F56" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" ht="19" customHeight="1">
-      <c r="A57" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B57" s="25">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s" s="26">
-        <v>76</v>
       </c>
       <c r="D57" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="E57" t="s" s="14">
-        <v>92</v>
+      <c r="E57" t="s" s="15">
+        <v>93</v>
       </c>
       <c r="F57" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="58" ht="19" customHeight="1">
-      <c r="A58" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B58" s="28">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s" s="29">
-        <v>78</v>
+      <c r="A58" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B58" s="22">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D58" t="s" s="16">
         <v>17</v>
       </c>
       <c r="E58" t="s" s="14">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F58" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="59" ht="19" customHeight="1">
-      <c r="A59" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B59" s="31">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s" s="32">
-        <v>80</v>
+      <c r="A59" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B59" s="25">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s" s="26">
+        <v>76</v>
       </c>
       <c r="D59" t="s" s="16">
         <v>17</v>
       </c>
       <c r="E59" t="s" s="14">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F59" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="60" ht="19" customHeight="1">
-      <c r="A60" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B60" s="34">
-        <v>7</v>
-      </c>
-      <c r="C60" t="s" s="35">
-        <v>82</v>
+      <c r="A60" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B60" s="28">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s" s="29">
+        <v>78</v>
       </c>
       <c r="D60" t="s" s="16">
         <v>17</v>
       </c>
       <c r="E60" t="s" s="14">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F60" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="61" ht="19" customHeight="1">
-      <c r="A61" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B61" s="19">
-        <v>7</v>
-      </c>
-      <c r="C61" t="s" s="20">
+      <c r="A61" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B61" s="31">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D61" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E61" t="s" s="14">
+        <v>97</v>
+      </c>
+      <c r="F61" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" ht="19" customHeight="1">
+      <c r="A62" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B62" s="34">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D62" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E62" t="s" s="14">
+        <v>98</v>
+      </c>
+      <c r="F62" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" ht="19" customHeight="1">
+      <c r="A63" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B63" s="37">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D63" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="E63" t="s" s="14">
+        <v>99</v>
+      </c>
+      <c r="F63" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" ht="19" customHeight="1">
+      <c r="A64" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B64" s="19">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D61" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E61" t="s" s="17">
-        <v>96</v>
-      </c>
-      <c r="F61" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" ht="19" customHeight="1">
-      <c r="A62" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B62" s="22">
-        <v>7</v>
-      </c>
-      <c r="C62" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D62" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E62" t="s" s="15">
-        <v>97</v>
-      </c>
-      <c r="F62" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" ht="19" customHeight="1">
-      <c r="A63" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B63" s="25">
-        <v>7</v>
-      </c>
-      <c r="C63" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D63" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="E63" t="s" s="17">
-        <v>98</v>
-      </c>
-      <c r="F63" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" ht="19" customHeight="1">
-      <c r="A64" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B64" s="28">
-        <v>7</v>
-      </c>
-      <c r="C64" t="s" s="29">
-        <v>78</v>
       </c>
       <c r="D64" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="E64" t="s" s="14">
-        <v>99</v>
+      <c r="E64" t="s" s="17">
+        <v>100</v>
       </c>
       <c r="F64" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="65" ht="19" customHeight="1">
-      <c r="A65" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B65" s="31">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s" s="32">
-        <v>80</v>
+      <c r="A65" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B65" s="22">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D65" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="E65" t="s" s="14">
-        <v>100</v>
+      <c r="E65" t="s" s="15">
+        <v>101</v>
       </c>
       <c r="F65" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="66" ht="19" customHeight="1">
-      <c r="A66" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B66" s="34">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s" s="35">
-        <v>82</v>
+      <c r="A66" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B66" s="25">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s" s="26">
+        <v>76</v>
       </c>
       <c r="D66" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="E66" t="s" s="14">
-        <v>101</v>
+      <c r="E66" t="s" s="17">
+        <v>102</v>
       </c>
       <c r="F66" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="67" ht="19" customHeight="1">
-      <c r="A67" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B67" s="19">
-        <v>7</v>
-      </c>
-      <c r="C67" t="s" s="20">
+      <c r="A67" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B67" s="28">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D67" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="E67" t="s" s="14">
+        <v>103</v>
+      </c>
+      <c r="F67" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" ht="19" customHeight="1">
+      <c r="A68" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B68" s="31">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D68" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="E68" t="s" s="14">
+        <v>104</v>
+      </c>
+      <c r="F68" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" ht="19" customHeight="1">
+      <c r="A69" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B69" s="34">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D69" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="E69" t="s" s="14">
+        <v>105</v>
+      </c>
+      <c r="F69" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" ht="19" customHeight="1">
+      <c r="A70" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B70" s="37">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D70" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="E70" t="s" s="14">
+        <v>106</v>
+      </c>
+      <c r="F70" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" ht="19" customHeight="1">
+      <c r="A71" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B71" s="19">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D67" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E67" t="s" s="14">
-        <v>102</v>
-      </c>
-      <c r="F67" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="68" ht="19" customHeight="1">
-      <c r="A68" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B68" s="22">
-        <v>7</v>
-      </c>
-      <c r="C68" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D68" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E68" t="s" s="14">
-        <v>103</v>
-      </c>
-      <c r="F68" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" ht="19" customHeight="1">
-      <c r="A69" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B69" s="25">
-        <v>7</v>
-      </c>
-      <c r="C69" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D69" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E69" t="s" s="17">
-        <v>104</v>
-      </c>
-      <c r="F69" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="70" ht="19" customHeight="1">
-      <c r="A70" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B70" s="28">
-        <v>7</v>
-      </c>
-      <c r="C70" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D70" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="E70" t="s" s="14">
-        <v>105</v>
-      </c>
-      <c r="F70" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="71" ht="19" customHeight="1">
-      <c r="A71" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B71" s="31">
-        <v>7</v>
-      </c>
-      <c r="C71" t="s" s="32">
-        <v>80</v>
       </c>
       <c r="D71" t="s" s="16">
         <v>23</v>
       </c>
       <c r="E71" t="s" s="14">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F71" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="72" ht="19" customHeight="1">
-      <c r="A72" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B72" s="34">
-        <v>7</v>
-      </c>
-      <c r="C72" t="s" s="35">
-        <v>82</v>
+      <c r="A72" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B72" s="22">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D72" t="s" s="16">
         <v>23</v>
       </c>
       <c r="E72" t="s" s="14">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F72" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="73" ht="19" customHeight="1">
-      <c r="A73" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B73" s="19">
-        <v>7</v>
-      </c>
-      <c r="C73" t="s" s="20">
+      <c r="A73" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B73" s="25">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D73" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="E73" t="s" s="17">
+        <v>109</v>
+      </c>
+      <c r="F73" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" ht="19" customHeight="1">
+      <c r="A74" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B74" s="28">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D74" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="E74" t="s" s="14">
+        <v>110</v>
+      </c>
+      <c r="F74" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" ht="19" customHeight="1">
+      <c r="A75" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B75" s="31">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D75" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="E75" t="s" s="14">
+        <v>111</v>
+      </c>
+      <c r="F75" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" ht="19" customHeight="1">
+      <c r="A76" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B76" s="34">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D76" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="E76" t="s" s="14">
+        <v>112</v>
+      </c>
+      <c r="F76" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" ht="19" customHeight="1">
+      <c r="A77" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B77" s="37">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D77" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="E77" t="s" s="14">
+        <v>113</v>
+      </c>
+      <c r="F77" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" ht="19" customHeight="1">
+      <c r="A78" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B78" s="19">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s" s="20">
         <v>72</v>
-      </c>
-      <c r="D73" t="s" s="16">
-        <v>26</v>
-      </c>
-      <c r="E73" t="s" s="14">
-        <v>108</v>
-      </c>
-      <c r="F73" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="74" ht="19" customHeight="1">
-      <c r="A74" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B74" s="22">
-        <v>7</v>
-      </c>
-      <c r="C74" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D74" t="s" s="16">
-        <v>26</v>
-      </c>
-      <c r="E74" t="s" s="15">
-        <v>109</v>
-      </c>
-      <c r="F74" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="75" ht="19" customHeight="1">
-      <c r="A75" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B75" s="25">
-        <v>7</v>
-      </c>
-      <c r="C75" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D75" t="s" s="16">
-        <v>26</v>
-      </c>
-      <c r="E75" t="s" s="14">
-        <v>110</v>
-      </c>
-      <c r="F75" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="76" ht="19" customHeight="1">
-      <c r="A76" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B76" s="28">
-        <v>7</v>
-      </c>
-      <c r="C76" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D76" t="s" s="16">
-        <v>26</v>
-      </c>
-      <c r="E76" t="s" s="14">
-        <v>111</v>
-      </c>
-      <c r="F76" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="77" ht="19" customHeight="1">
-      <c r="A77" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B77" s="31">
-        <v>7</v>
-      </c>
-      <c r="C77" t="s" s="32">
-        <v>80</v>
-      </c>
-      <c r="D77" t="s" s="16">
-        <v>26</v>
-      </c>
-      <c r="E77" t="s" s="14">
-        <v>112</v>
-      </c>
-      <c r="F77" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="78" ht="19" customHeight="1">
-      <c r="A78" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B78" s="34">
-        <v>7</v>
-      </c>
-      <c r="C78" t="s" s="35">
-        <v>82</v>
       </c>
       <c r="D78" t="s" s="16">
         <v>26</v>
       </c>
       <c r="E78" t="s" s="14">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F78" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="79" ht="19" customHeight="1">
-      <c r="A79" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B79" s="19">
-        <v>7</v>
-      </c>
-      <c r="C79" t="s" s="20">
-        <v>72</v>
+      <c r="A79" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B79" s="22">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s" s="23">
+        <v>74</v>
       </c>
       <c r="D79" t="s" s="16">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E79" t="s" s="15">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F79" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="80" ht="19" customHeight="1">
-      <c r="A80" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B80" s="22">
-        <v>7</v>
-      </c>
-      <c r="C80" t="s" s="23">
-        <v>74</v>
+      <c r="A80" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B80" s="25">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s" s="26">
+        <v>76</v>
       </c>
       <c r="D80" t="s" s="16">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E80" t="s" s="14">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F80" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="81" ht="19" customHeight="1">
-      <c r="A81" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B81" s="25">
-        <v>7</v>
-      </c>
-      <c r="C81" t="s" s="26">
-        <v>76</v>
+      <c r="A81" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B81" s="28">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s" s="29">
+        <v>78</v>
       </c>
       <c r="D81" t="s" s="16">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E81" t="s" s="14">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F81" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="82" ht="19" customHeight="1">
-      <c r="A82" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B82" s="28">
-        <v>7</v>
-      </c>
-      <c r="C82" t="s" s="29">
-        <v>78</v>
+      <c r="A82" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B82" s="31">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s" s="32">
+        <v>80</v>
       </c>
       <c r="D82" t="s" s="16">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E82" t="s" s="14">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F82" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="83" ht="19" customHeight="1">
-      <c r="A83" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B83" s="31">
-        <v>7</v>
-      </c>
-      <c r="C83" t="s" s="32">
-        <v>80</v>
+      <c r="A83" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B83" s="34">
+        <v>7</v>
+      </c>
+      <c r="C83" t="s" s="35">
+        <v>82</v>
       </c>
       <c r="D83" t="s" s="16">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E83" t="s" s="14">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F83" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="84" ht="19" customHeight="1">
-      <c r="A84" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B84" s="34">
-        <v>7</v>
-      </c>
-      <c r="C84" t="s" s="35">
-        <v>82</v>
+      <c r="A84" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B84" s="37">
+        <v>7</v>
+      </c>
+      <c r="C84" t="s" s="38">
+        <v>84</v>
       </c>
       <c r="D84" t="s" s="16">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E84" t="s" s="14">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F84" t="s" s="15">
         <v>11</v>
@@ -3699,10 +3778,10 @@
         <v>72</v>
       </c>
       <c r="D85" t="s" s="16">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E85" t="s" s="15">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F85" t="s" s="15">
         <v>11</v>
@@ -3719,10 +3798,10 @@
         <v>74</v>
       </c>
       <c r="D86" t="s" s="16">
-        <v>32</v>
-      </c>
-      <c r="E86" t="s" s="17">
-        <v>121</v>
+        <v>29</v>
+      </c>
+      <c r="E86" t="s" s="14">
+        <v>122</v>
       </c>
       <c r="F86" t="s" s="15">
         <v>11</v>
@@ -3739,10 +3818,10 @@
         <v>76</v>
       </c>
       <c r="D87" t="s" s="16">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E87" t="s" s="14">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F87" t="s" s="15">
         <v>11</v>
@@ -3759,10 +3838,10 @@
         <v>78</v>
       </c>
       <c r="D88" t="s" s="16">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E88" t="s" s="14">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F88" t="s" s="15">
         <v>11</v>
@@ -3779,10 +3858,10 @@
         <v>80</v>
       </c>
       <c r="D89" t="s" s="16">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E89" t="s" s="14">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F89" t="s" s="15">
         <v>11</v>
@@ -3799,730 +3878,730 @@
         <v>82</v>
       </c>
       <c r="D90" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E90" t="s" s="14">
+        <v>126</v>
+      </c>
+      <c r="F90" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" ht="19" customHeight="1">
+      <c r="A91" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B91" s="37">
+        <v>7</v>
+      </c>
+      <c r="C91" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D91" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E91" t="s" s="14">
+        <v>127</v>
+      </c>
+      <c r="F91" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" ht="19" customHeight="1">
+      <c r="A92" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B92" s="19">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D92" t="s" s="16">
         <v>32</v>
       </c>
-      <c r="E90" t="s" s="14">
-        <v>125</v>
-      </c>
-      <c r="F90" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="91" ht="19" customHeight="1">
-      <c r="A91" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B91" s="19">
-        <v>7</v>
-      </c>
-      <c r="C91" t="s" s="20">
+      <c r="E92" t="s" s="15">
+        <v>128</v>
+      </c>
+      <c r="F92" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" ht="19" customHeight="1">
+      <c r="A93" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B93" s="22">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D93" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E93" t="s" s="17">
+        <v>129</v>
+      </c>
+      <c r="F93" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" ht="19" customHeight="1">
+      <c r="A94" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B94" s="25">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D94" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E94" t="s" s="14">
+        <v>130</v>
+      </c>
+      <c r="F94" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" ht="19" customHeight="1">
+      <c r="A95" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B95" s="28">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D95" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E95" t="s" s="14">
+        <v>131</v>
+      </c>
+      <c r="F95" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" ht="19" customHeight="1">
+      <c r="A96" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B96" s="31">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D96" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E96" t="s" s="14">
+        <v>132</v>
+      </c>
+      <c r="F96" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" ht="19" customHeight="1">
+      <c r="A97" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B97" s="34">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D97" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E97" t="s" s="14">
+        <v>133</v>
+      </c>
+      <c r="F97" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" ht="19" customHeight="1">
+      <c r="A98" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B98" s="37">
+        <v>7</v>
+      </c>
+      <c r="C98" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D98" t="s" s="16">
+        <v>32</v>
+      </c>
+      <c r="E98" t="s" s="14">
+        <v>134</v>
+      </c>
+      <c r="F98" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" ht="19" customHeight="1">
+      <c r="A99" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B99" s="19">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D91" t="s" s="16">
+      <c r="D99" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E91" t="s" s="14">
-        <v>126</v>
-      </c>
-      <c r="F91" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="92" ht="19" customHeight="1">
-      <c r="A92" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B92" s="22">
-        <v>7</v>
-      </c>
-      <c r="C92" t="s" s="23">
+      <c r="E99" t="s" s="14">
+        <v>135</v>
+      </c>
+      <c r="F99" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" ht="19" customHeight="1">
+      <c r="A100" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B100" s="22">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D92" t="s" s="16">
+      <c r="D100" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E92" t="s" s="14">
-        <v>127</v>
-      </c>
-      <c r="F92" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="93" ht="19" customHeight="1">
-      <c r="A93" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B93" s="25">
-        <v>7</v>
-      </c>
-      <c r="C93" t="s" s="26">
+      <c r="E100" t="s" s="14">
+        <v>136</v>
+      </c>
+      <c r="F100" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" ht="19" customHeight="1">
+      <c r="A101" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B101" s="25">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D93" t="s" s="16">
+      <c r="D101" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E93" t="s" s="14">
-        <v>128</v>
-      </c>
-      <c r="F93" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="94" ht="19" customHeight="1">
-      <c r="A94" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B94" s="28">
-        <v>7</v>
-      </c>
-      <c r="C94" t="s" s="29">
+      <c r="E101" t="s" s="14">
+        <v>137</v>
+      </c>
+      <c r="F101" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" ht="19" customHeight="1">
+      <c r="A102" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B102" s="28">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D94" t="s" s="16">
+      <c r="D102" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E94" t="s" s="14">
-        <v>129</v>
-      </c>
-      <c r="F94" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="95" ht="19" customHeight="1">
-      <c r="A95" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B95" s="31">
-        <v>7</v>
-      </c>
-      <c r="C95" t="s" s="32">
+      <c r="E102" t="s" s="14">
+        <v>138</v>
+      </c>
+      <c r="F102" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" ht="19" customHeight="1">
+      <c r="A103" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B103" s="31">
+        <v>7</v>
+      </c>
+      <c r="C103" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D95" t="s" s="16">
+      <c r="D103" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E95" t="s" s="14">
-        <v>130</v>
-      </c>
-      <c r="F95" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="96" ht="19" customHeight="1">
-      <c r="A96" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B96" s="34">
-        <v>7</v>
-      </c>
-      <c r="C96" t="s" s="35">
+      <c r="E103" t="s" s="14">
+        <v>139</v>
+      </c>
+      <c r="F103" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104" ht="19" customHeight="1">
+      <c r="A104" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B104" s="34">
+        <v>7</v>
+      </c>
+      <c r="C104" t="s" s="35">
         <v>82</v>
       </c>
-      <c r="D96" t="s" s="16">
+      <c r="D104" t="s" s="16">
         <v>35</v>
       </c>
-      <c r="E96" t="s" s="14">
-        <v>131</v>
-      </c>
-      <c r="F96" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="97" ht="19" customHeight="1">
-      <c r="A97" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B97" s="19">
-        <v>7</v>
-      </c>
-      <c r="C97" t="s" s="20">
+      <c r="E104" t="s" s="14">
+        <v>140</v>
+      </c>
+      <c r="F104" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" ht="19" customHeight="1">
+      <c r="A105" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B105" s="37">
+        <v>7</v>
+      </c>
+      <c r="C105" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D105" t="s" s="16">
+        <v>35</v>
+      </c>
+      <c r="E105" t="s" s="14">
+        <v>141</v>
+      </c>
+      <c r="F105" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" ht="19" customHeight="1">
+      <c r="A106" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B106" s="19">
+        <v>7</v>
+      </c>
+      <c r="C106" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D97" t="s" s="16">
+      <c r="D106" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E97" t="s" s="15">
-        <v>132</v>
-      </c>
-      <c r="F97" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="98" ht="19" customHeight="1">
-      <c r="A98" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B98" s="22">
-        <v>7</v>
-      </c>
-      <c r="C98" t="s" s="23">
+      <c r="E106" t="s" s="15">
+        <v>142</v>
+      </c>
+      <c r="F106" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" ht="19" customHeight="1">
+      <c r="A107" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B107" s="22">
+        <v>7</v>
+      </c>
+      <c r="C107" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D98" t="s" s="16">
+      <c r="D107" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E98" t="s" s="15">
-        <v>133</v>
-      </c>
-      <c r="F98" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="99" ht="19" customHeight="1">
-      <c r="A99" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B99" s="25">
-        <v>7</v>
-      </c>
-      <c r="C99" t="s" s="26">
+      <c r="E107" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="F107" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" ht="19" customHeight="1">
+      <c r="A108" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B108" s="25">
+        <v>7</v>
+      </c>
+      <c r="C108" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D99" t="s" s="16">
+      <c r="D108" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E99" t="s" s="14">
-        <v>134</v>
-      </c>
-      <c r="F99" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="100" ht="19" customHeight="1">
-      <c r="A100" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B100" s="28">
-        <v>7</v>
-      </c>
-      <c r="C100" t="s" s="29">
+      <c r="E108" t="s" s="14">
+        <v>144</v>
+      </c>
+      <c r="F108" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" ht="19" customHeight="1">
+      <c r="A109" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B109" s="28">
+        <v>7</v>
+      </c>
+      <c r="C109" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D100" t="s" s="16">
+      <c r="D109" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E100" t="s" s="14">
-        <v>135</v>
-      </c>
-      <c r="F100" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="101" ht="19" customHeight="1">
-      <c r="A101" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B101" s="31">
-        <v>7</v>
-      </c>
-      <c r="C101" t="s" s="32">
+      <c r="E109" t="s" s="14">
+        <v>145</v>
+      </c>
+      <c r="F109" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" ht="19" customHeight="1">
+      <c r="A110" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B110" s="31">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D101" t="s" s="16">
+      <c r="D110" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E101" t="s" s="14">
-        <v>136</v>
-      </c>
-      <c r="F101" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="102" ht="19" customHeight="1">
-      <c r="A102" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B102" s="34">
-        <v>7</v>
-      </c>
-      <c r="C102" t="s" s="35">
+      <c r="E110" t="s" s="14">
+        <v>146</v>
+      </c>
+      <c r="F110" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="111" ht="19" customHeight="1">
+      <c r="A111" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B111" s="34">
+        <v>7</v>
+      </c>
+      <c r="C111" t="s" s="35">
         <v>82</v>
       </c>
-      <c r="D102" t="s" s="16">
+      <c r="D111" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="E102" t="s" s="14">
-        <v>137</v>
-      </c>
-      <c r="F102" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="103" ht="19" customHeight="1">
-      <c r="A103" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B103" s="19">
-        <v>7</v>
-      </c>
-      <c r="C103" t="s" s="20">
+      <c r="E111" t="s" s="14">
+        <v>147</v>
+      </c>
+      <c r="F111" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" ht="19" customHeight="1">
+      <c r="A112" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B112" s="37">
+        <v>7</v>
+      </c>
+      <c r="C112" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D112" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="E112" t="s" s="14">
+        <v>148</v>
+      </c>
+      <c r="F112" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" ht="19" customHeight="1">
+      <c r="A113" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B113" s="19">
+        <v>7</v>
+      </c>
+      <c r="C113" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D103" t="s" s="16">
+      <c r="D113" t="s" s="16">
         <v>41</v>
       </c>
-      <c r="E103" t="s" s="15">
-        <v>138</v>
-      </c>
-      <c r="F103" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="104" ht="19" customHeight="1">
-      <c r="A104" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B104" s="22">
-        <v>7</v>
-      </c>
-      <c r="C104" t="s" s="23">
+      <c r="E113" t="s" s="15">
+        <v>149</v>
+      </c>
+      <c r="F113" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" ht="19" customHeight="1">
+      <c r="A114" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B114" s="22">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D104" t="s" s="16">
+      <c r="D114" t="s" s="16">
         <v>41</v>
       </c>
-      <c r="E104" t="s" s="14">
-        <v>139</v>
-      </c>
-      <c r="F104" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="105" ht="19" customHeight="1">
-      <c r="A105" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B105" s="25">
-        <v>7</v>
-      </c>
-      <c r="C105" t="s" s="26">
+      <c r="E114" t="s" s="14">
+        <v>150</v>
+      </c>
+      <c r="F114" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" ht="19" customHeight="1">
+      <c r="A115" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B115" s="25">
+        <v>7</v>
+      </c>
+      <c r="C115" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D105" t="s" s="16">
+      <c r="D115" t="s" s="16">
         <v>41</v>
       </c>
-      <c r="E105" t="s" s="14">
-        <v>140</v>
-      </c>
-      <c r="F105" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="106" ht="19" customHeight="1">
-      <c r="A106" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B106" s="28">
-        <v>7</v>
-      </c>
-      <c r="C106" t="s" s="29">
+      <c r="E115" t="s" s="14">
+        <v>151</v>
+      </c>
+      <c r="F115" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" ht="19" customHeight="1">
+      <c r="A116" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B116" s="28">
+        <v>7</v>
+      </c>
+      <c r="C116" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D106" t="s" s="16">
+      <c r="D116" t="s" s="16">
         <v>41</v>
       </c>
-      <c r="E106" t="s" s="14">
-        <v>141</v>
-      </c>
-      <c r="F106" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="107" ht="19" customHeight="1">
-      <c r="A107" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B107" s="31">
-        <v>7</v>
-      </c>
-      <c r="C107" t="s" s="32">
+      <c r="E116" t="s" s="14">
+        <v>152</v>
+      </c>
+      <c r="F116" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" ht="19" customHeight="1">
+      <c r="A117" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B117" s="31">
+        <v>7</v>
+      </c>
+      <c r="C117" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D107" t="s" s="16">
+      <c r="D117" t="s" s="16">
         <v>41</v>
       </c>
-      <c r="E107" t="s" s="14">
-        <v>142</v>
-      </c>
-      <c r="F107" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="108" ht="19" customHeight="1">
-      <c r="A108" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B108" s="34">
-        <v>7</v>
-      </c>
-      <c r="C108" t="s" s="35">
+      <c r="E117" t="s" s="14">
+        <v>153</v>
+      </c>
+      <c r="F117" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" ht="19" customHeight="1">
+      <c r="A118" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B118" s="34">
+        <v>7</v>
+      </c>
+      <c r="C118" t="s" s="35">
         <v>82</v>
       </c>
-      <c r="D108" t="s" s="16">
+      <c r="D118" t="s" s="16">
         <v>41</v>
       </c>
-      <c r="E108" t="s" s="14">
-        <v>143</v>
-      </c>
-      <c r="F108" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="109" ht="19" customHeight="1">
-      <c r="A109" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B109" s="19">
-        <v>7</v>
-      </c>
-      <c r="C109" t="s" s="20">
+      <c r="E118" t="s" s="14">
+        <v>154</v>
+      </c>
+      <c r="F118" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" ht="19" customHeight="1">
+      <c r="A119" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B119" s="37">
+        <v>7</v>
+      </c>
+      <c r="C119" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D119" t="s" s="16">
+        <v>41</v>
+      </c>
+      <c r="E119" t="s" s="14">
+        <v>155</v>
+      </c>
+      <c r="F119" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120" ht="19" customHeight="1">
+      <c r="A120" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B120" s="19">
+        <v>7</v>
+      </c>
+      <c r="C120" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D109" t="s" s="16">
+      <c r="D120" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E109" t="s" s="15">
-        <v>144</v>
-      </c>
-      <c r="F109" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="110" ht="19" customHeight="1">
-      <c r="A110" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B110" s="22">
-        <v>7</v>
-      </c>
-      <c r="C110" t="s" s="23">
+      <c r="E120" t="s" s="15">
+        <v>156</v>
+      </c>
+      <c r="F120" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" ht="19" customHeight="1">
+      <c r="A121" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B121" s="22">
+        <v>7</v>
+      </c>
+      <c r="C121" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D110" t="s" s="16">
+      <c r="D121" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E110" t="s" s="14">
-        <v>145</v>
-      </c>
-      <c r="F110" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="111" ht="19" customHeight="1">
-      <c r="A111" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B111" s="25">
-        <v>7</v>
-      </c>
-      <c r="C111" t="s" s="26">
+      <c r="E121" t="s" s="14">
+        <v>157</v>
+      </c>
+      <c r="F121" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" ht="19" customHeight="1">
+      <c r="A122" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B122" s="25">
+        <v>7</v>
+      </c>
+      <c r="C122" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D111" t="s" s="16">
+      <c r="D122" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E111" t="s" s="14">
-        <v>146</v>
-      </c>
-      <c r="F111" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="112" ht="19" customHeight="1">
-      <c r="A112" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B112" s="28">
-        <v>7</v>
-      </c>
-      <c r="C112" t="s" s="29">
+      <c r="E122" t="s" s="14">
+        <v>158</v>
+      </c>
+      <c r="F122" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123" ht="19" customHeight="1">
+      <c r="A123" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B123" s="28">
+        <v>7</v>
+      </c>
+      <c r="C123" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D112" t="s" s="16">
+      <c r="D123" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E112" t="s" s="14">
-        <v>147</v>
-      </c>
-      <c r="F112" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="113" ht="19" customHeight="1">
-      <c r="A113" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B113" s="31">
-        <v>7</v>
-      </c>
-      <c r="C113" t="s" s="32">
+      <c r="E123" t="s" s="14">
+        <v>159</v>
+      </c>
+      <c r="F123" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" ht="19" customHeight="1">
+      <c r="A124" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B124" s="31">
+        <v>7</v>
+      </c>
+      <c r="C124" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D113" t="s" s="16">
+      <c r="D124" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E113" t="s" s="14">
-        <v>148</v>
-      </c>
-      <c r="F113" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="114" ht="19" customHeight="1">
-      <c r="A114" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B114" s="34">
-        <v>7</v>
-      </c>
-      <c r="C114" t="s" s="35">
+      <c r="E124" t="s" s="14">
+        <v>160</v>
+      </c>
+      <c r="F124" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" ht="19" customHeight="1">
+      <c r="A125" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B125" s="34">
+        <v>7</v>
+      </c>
+      <c r="C125" t="s" s="35">
         <v>82</v>
       </c>
-      <c r="D114" t="s" s="16">
+      <c r="D125" t="s" s="16">
         <v>44</v>
       </c>
-      <c r="E114" t="s" s="14">
-        <v>149</v>
-      </c>
-      <c r="F114" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="115" ht="19" customHeight="1">
-      <c r="A115" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B115" s="19">
-        <v>7</v>
-      </c>
-      <c r="C115" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D115" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E115" t="s" s="15">
-        <v>150</v>
-      </c>
-      <c r="F115" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="116" ht="19" customHeight="1">
-      <c r="A116" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B116" s="22">
-        <v>7</v>
-      </c>
-      <c r="C116" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D116" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E116" t="s" s="14">
-        <v>151</v>
-      </c>
-      <c r="F116" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="117" ht="19" customHeight="1">
-      <c r="A117" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B117" s="25">
-        <v>7</v>
-      </c>
-      <c r="C117" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D117" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E117" t="s" s="14">
-        <v>152</v>
-      </c>
-      <c r="F117" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="118" ht="19" customHeight="1">
-      <c r="A118" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B118" s="28">
-        <v>7</v>
-      </c>
-      <c r="C118" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D118" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E118" t="s" s="14">
-        <v>153</v>
-      </c>
-      <c r="F118" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="119" ht="19" customHeight="1">
-      <c r="A119" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B119" s="31">
-        <v>7</v>
-      </c>
-      <c r="C119" t="s" s="32">
-        <v>80</v>
-      </c>
-      <c r="D119" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E119" t="s" s="14">
-        <v>154</v>
-      </c>
-      <c r="F119" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="120" ht="19" customHeight="1">
-      <c r="A120" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B120" s="34">
-        <v>7</v>
-      </c>
-      <c r="C120" t="s" s="35">
-        <v>82</v>
-      </c>
-      <c r="D120" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E120" t="s" s="14">
-        <v>155</v>
-      </c>
-      <c r="F120" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="121" ht="19" customHeight="1">
-      <c r="A121" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B121" s="19">
-        <v>7</v>
-      </c>
-      <c r="C121" t="s" s="20">
-        <v>72</v>
-      </c>
-      <c r="D121" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E121" t="s" s="17">
-        <v>156</v>
-      </c>
-      <c r="F121" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="122" ht="19" customHeight="1">
-      <c r="A122" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B122" s="22">
-        <v>7</v>
-      </c>
-      <c r="C122" t="s" s="23">
-        <v>74</v>
-      </c>
-      <c r="D122" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E122" t="s" s="14">
-        <v>157</v>
-      </c>
-      <c r="F122" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="123" ht="19" customHeight="1">
-      <c r="A123" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B123" s="25">
-        <v>7</v>
-      </c>
-      <c r="C123" t="s" s="26">
-        <v>76</v>
-      </c>
-      <c r="D123" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E123" t="s" s="17">
-        <v>158</v>
-      </c>
-      <c r="F123" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="124" ht="19" customHeight="1">
-      <c r="A124" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B124" s="28">
-        <v>7</v>
-      </c>
-      <c r="C124" t="s" s="29">
-        <v>78</v>
-      </c>
-      <c r="D124" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="E124" t="s" s="14">
-        <v>159</v>
-      </c>
-      <c r="F124" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="125" ht="19" customHeight="1">
-      <c r="A125" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B125" s="31">
-        <v>7</v>
-      </c>
-      <c r="C125" t="s" s="32">
-        <v>80</v>
-      </c>
-      <c r="D125" t="s" s="16">
-        <v>50</v>
-      </c>
       <c r="E125" t="s" s="14">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F125" t="s" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="126" ht="19" customHeight="1">
-      <c r="A126" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B126" s="34">
-        <v>7</v>
-      </c>
-      <c r="C126" t="s" s="35">
-        <v>82</v>
+      <c r="A126" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B126" s="37">
+        <v>7</v>
+      </c>
+      <c r="C126" t="s" s="38">
+        <v>84</v>
       </c>
       <c r="D126" t="s" s="16">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E126" t="s" s="14">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F126" t="s" s="15">
         <v>11</v>
@@ -4539,10 +4618,10 @@
         <v>72</v>
       </c>
       <c r="D127" t="s" s="16">
-        <v>53</v>
-      </c>
-      <c r="E127" t="s" s="14">
-        <v>162</v>
+        <v>47</v>
+      </c>
+      <c r="E127" t="s" s="15">
+        <v>163</v>
       </c>
       <c r="F127" t="s" s="15">
         <v>11</v>
@@ -4559,10 +4638,10 @@
         <v>74</v>
       </c>
       <c r="D128" t="s" s="16">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E128" t="s" s="14">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F128" t="s" s="15">
         <v>11</v>
@@ -4579,10 +4658,10 @@
         <v>76</v>
       </c>
       <c r="D129" t="s" s="16">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E129" t="s" s="14">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F129" t="s" s="15">
         <v>11</v>
@@ -4599,10 +4678,10 @@
         <v>78</v>
       </c>
       <c r="D130" t="s" s="16">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E130" t="s" s="14">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F130" t="s" s="15">
         <v>11</v>
@@ -4619,10 +4698,10 @@
         <v>80</v>
       </c>
       <c r="D131" t="s" s="16">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E131" t="s" s="14">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F131" t="s" s="15">
         <v>11</v>
@@ -4639,612 +4718,1012 @@
         <v>82</v>
       </c>
       <c r="D132" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E132" t="s" s="14">
+        <v>168</v>
+      </c>
+      <c r="F132" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133" ht="19" customHeight="1">
+      <c r="A133" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B133" s="37">
+        <v>7</v>
+      </c>
+      <c r="C133" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D133" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E133" t="s" s="14">
+        <v>169</v>
+      </c>
+      <c r="F133" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" ht="19" customHeight="1">
+      <c r="A134" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B134" s="19">
+        <v>7</v>
+      </c>
+      <c r="C134" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D134" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E134" t="s" s="17">
+        <v>170</v>
+      </c>
+      <c r="F134" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" ht="19" customHeight="1">
+      <c r="A135" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B135" s="22">
+        <v>7</v>
+      </c>
+      <c r="C135" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D135" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E135" t="s" s="14">
+        <v>171</v>
+      </c>
+      <c r="F135" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="136" ht="19" customHeight="1">
+      <c r="A136" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B136" s="25">
+        <v>7</v>
+      </c>
+      <c r="C136" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D136" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E136" t="s" s="17">
+        <v>172</v>
+      </c>
+      <c r="F136" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="137" ht="19" customHeight="1">
+      <c r="A137" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B137" s="28">
+        <v>7</v>
+      </c>
+      <c r="C137" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D137" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E137" t="s" s="14">
+        <v>173</v>
+      </c>
+      <c r="F137" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="138" ht="19" customHeight="1">
+      <c r="A138" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B138" s="31">
+        <v>7</v>
+      </c>
+      <c r="C138" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D138" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E138" t="s" s="14">
+        <v>174</v>
+      </c>
+      <c r="F138" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="139" ht="19" customHeight="1">
+      <c r="A139" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B139" s="34">
+        <v>7</v>
+      </c>
+      <c r="C139" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D139" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E139" t="s" s="14">
+        <v>175</v>
+      </c>
+      <c r="F139" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140" ht="19" customHeight="1">
+      <c r="A140" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B140" s="37">
+        <v>7</v>
+      </c>
+      <c r="C140" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D140" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E140" t="s" s="14">
+        <v>176</v>
+      </c>
+      <c r="F140" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="141" ht="19" customHeight="1">
+      <c r="A141" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B141" s="19">
+        <v>7</v>
+      </c>
+      <c r="C141" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="D141" t="s" s="16">
         <v>53</v>
       </c>
-      <c r="E132" t="s" s="14">
-        <v>167</v>
-      </c>
-      <c r="F132" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="133" ht="19" customHeight="1">
-      <c r="A133" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B133" s="19">
-        <v>7</v>
-      </c>
-      <c r="C133" t="s" s="20">
+      <c r="E141" t="s" s="14">
+        <v>177</v>
+      </c>
+      <c r="F141" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="142" ht="19" customHeight="1">
+      <c r="A142" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B142" s="22">
+        <v>7</v>
+      </c>
+      <c r="C142" t="s" s="23">
+        <v>74</v>
+      </c>
+      <c r="D142" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E142" t="s" s="14">
+        <v>178</v>
+      </c>
+      <c r="F142" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="143" ht="19" customHeight="1">
+      <c r="A143" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B143" s="25">
+        <v>7</v>
+      </c>
+      <c r="C143" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="D143" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E143" t="s" s="14">
+        <v>179</v>
+      </c>
+      <c r="F143" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="144" ht="19" customHeight="1">
+      <c r="A144" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B144" s="28">
+        <v>7</v>
+      </c>
+      <c r="C144" t="s" s="29">
+        <v>78</v>
+      </c>
+      <c r="D144" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E144" t="s" s="14">
+        <v>180</v>
+      </c>
+      <c r="F144" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" ht="19" customHeight="1">
+      <c r="A145" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B145" s="31">
+        <v>7</v>
+      </c>
+      <c r="C145" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="D145" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E145" t="s" s="14">
+        <v>181</v>
+      </c>
+      <c r="F145" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="146" ht="19" customHeight="1">
+      <c r="A146" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B146" s="34">
+        <v>7</v>
+      </c>
+      <c r="C146" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D146" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E146" t="s" s="14">
+        <v>182</v>
+      </c>
+      <c r="F146" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="147" ht="19" customHeight="1">
+      <c r="A147" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B147" s="37">
+        <v>7</v>
+      </c>
+      <c r="C147" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D147" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E147" t="s" s="14">
+        <v>183</v>
+      </c>
+      <c r="F147" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="148" ht="19" customHeight="1">
+      <c r="A148" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B148" s="19">
+        <v>7</v>
+      </c>
+      <c r="C148" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D133" t="s" s="16">
+      <c r="D148" t="s" s="16">
         <v>56</v>
       </c>
-      <c r="E133" t="s" s="15">
-        <v>162</v>
-      </c>
-      <c r="F133" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="134" ht="19" customHeight="1">
-      <c r="A134" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B134" s="22">
-        <v>7</v>
-      </c>
-      <c r="C134" t="s" s="23">
+      <c r="E148" t="s" s="15">
+        <v>177</v>
+      </c>
+      <c r="F148" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="149" ht="19" customHeight="1">
+      <c r="A149" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B149" s="22">
+        <v>7</v>
+      </c>
+      <c r="C149" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D134" t="s" s="16">
+      <c r="D149" t="s" s="16">
         <v>56</v>
       </c>
-      <c r="E134" t="s" s="14">
-        <v>168</v>
-      </c>
-      <c r="F134" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="135" ht="19" customHeight="1">
-      <c r="A135" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B135" s="25">
-        <v>7</v>
-      </c>
-      <c r="C135" t="s" s="26">
+      <c r="E149" t="s" s="14">
+        <v>184</v>
+      </c>
+      <c r="F149" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="150" ht="19" customHeight="1">
+      <c r="A150" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B150" s="25">
+        <v>7</v>
+      </c>
+      <c r="C150" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D135" t="s" s="16">
+      <c r="D150" t="s" s="16">
         <v>56</v>
       </c>
-      <c r="E135" t="s" s="17">
-        <v>169</v>
-      </c>
-      <c r="F135" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="136" ht="19" customHeight="1">
-      <c r="A136" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B136" s="28">
-        <v>7</v>
-      </c>
-      <c r="C136" t="s" s="29">
+      <c r="E150" t="s" s="17">
+        <v>185</v>
+      </c>
+      <c r="F150" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="151" ht="19" customHeight="1">
+      <c r="A151" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B151" s="28">
+        <v>7</v>
+      </c>
+      <c r="C151" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D136" t="s" s="16">
+      <c r="D151" t="s" s="16">
         <v>56</v>
       </c>
-      <c r="E136" t="s" s="14">
-        <v>170</v>
-      </c>
-      <c r="F136" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="137" ht="19" customHeight="1">
-      <c r="A137" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B137" s="31">
-        <v>7</v>
-      </c>
-      <c r="C137" t="s" s="32">
+      <c r="E151" t="s" s="14">
+        <v>186</v>
+      </c>
+      <c r="F151" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="152" ht="19" customHeight="1">
+      <c r="A152" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B152" s="31">
+        <v>7</v>
+      </c>
+      <c r="C152" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D137" t="s" s="16">
+      <c r="D152" t="s" s="16">
         <v>56</v>
       </c>
-      <c r="E137" t="s" s="14">
-        <v>171</v>
-      </c>
-      <c r="F137" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="138" ht="19" customHeight="1">
-      <c r="A138" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B138" s="34">
-        <v>7</v>
-      </c>
-      <c r="C138" t="s" s="35">
+      <c r="E152" t="s" s="14">
+        <v>187</v>
+      </c>
+      <c r="F152" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="153" ht="19" customHeight="1">
+      <c r="A153" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B153" s="34">
+        <v>7</v>
+      </c>
+      <c r="C153" t="s" s="35">
         <v>82</v>
       </c>
-      <c r="D138" t="s" s="16">
+      <c r="D153" t="s" s="16">
         <v>56</v>
       </c>
-      <c r="E138" t="s" s="14">
-        <v>172</v>
-      </c>
-      <c r="F138" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="139" ht="19" customHeight="1">
-      <c r="A139" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B139" s="19">
-        <v>7</v>
-      </c>
-      <c r="C139" t="s" s="20">
+      <c r="E153" t="s" s="14">
+        <v>188</v>
+      </c>
+      <c r="F153" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="154" ht="19" customHeight="1">
+      <c r="A154" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B154" s="37">
+        <v>7</v>
+      </c>
+      <c r="C154" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D154" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E154" t="s" s="14">
+        <v>189</v>
+      </c>
+      <c r="F154" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="155" ht="19" customHeight="1">
+      <c r="A155" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B155" s="19">
+        <v>7</v>
+      </c>
+      <c r="C155" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D139" t="s" s="16">
+      <c r="D155" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E139" t="s" s="15">
-        <v>173</v>
-      </c>
-      <c r="F139" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="140" ht="19" customHeight="1">
-      <c r="A140" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B140" s="22">
-        <v>7</v>
-      </c>
-      <c r="C140" t="s" s="23">
+      <c r="E155" t="s" s="15">
+        <v>190</v>
+      </c>
+      <c r="F155" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="156" ht="19" customHeight="1">
+      <c r="A156" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B156" s="22">
+        <v>7</v>
+      </c>
+      <c r="C156" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D140" t="s" s="16">
+      <c r="D156" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E140" t="s" s="14">
-        <v>174</v>
-      </c>
-      <c r="F140" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="141" ht="19" customHeight="1">
-      <c r="A141" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B141" s="25">
-        <v>7</v>
-      </c>
-      <c r="C141" t="s" s="26">
+      <c r="E156" t="s" s="14">
+        <v>191</v>
+      </c>
+      <c r="F156" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="157" ht="19" customHeight="1">
+      <c r="A157" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B157" s="25">
+        <v>7</v>
+      </c>
+      <c r="C157" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D141" t="s" s="16">
+      <c r="D157" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E141" t="s" s="14">
-        <v>175</v>
-      </c>
-      <c r="F141" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="142" ht="19" customHeight="1">
-      <c r="A142" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B142" s="28">
-        <v>7</v>
-      </c>
-      <c r="C142" t="s" s="29">
+      <c r="E157" t="s" s="14">
+        <v>192</v>
+      </c>
+      <c r="F157" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="158" ht="19" customHeight="1">
+      <c r="A158" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B158" s="28">
+        <v>7</v>
+      </c>
+      <c r="C158" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D142" t="s" s="16">
+      <c r="D158" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E142" t="s" s="14">
-        <v>176</v>
-      </c>
-      <c r="F142" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="143" ht="19" customHeight="1">
-      <c r="A143" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B143" s="31">
-        <v>7</v>
-      </c>
-      <c r="C143" t="s" s="32">
+      <c r="E158" t="s" s="14">
+        <v>193</v>
+      </c>
+      <c r="F158" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" ht="19" customHeight="1">
+      <c r="A159" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B159" s="31">
+        <v>7</v>
+      </c>
+      <c r="C159" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D143" t="s" s="16">
+      <c r="D159" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E143" t="s" s="14">
-        <v>177</v>
-      </c>
-      <c r="F143" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="144" ht="19" customHeight="1">
-      <c r="A144" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B144" s="34">
-        <v>7</v>
-      </c>
-      <c r="C144" t="s" s="35">
+      <c r="E159" t="s" s="14">
+        <v>194</v>
+      </c>
+      <c r="F159" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="160" ht="19" customHeight="1">
+      <c r="A160" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B160" s="34">
+        <v>7</v>
+      </c>
+      <c r="C160" t="s" s="35">
         <v>82</v>
       </c>
-      <c r="D144" t="s" s="16">
+      <c r="D160" t="s" s="16">
         <v>59</v>
       </c>
-      <c r="E144" t="s" s="14">
-        <v>178</v>
-      </c>
-      <c r="F144" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="145" ht="19" customHeight="1">
-      <c r="A145" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B145" s="19">
-        <v>7</v>
-      </c>
-      <c r="C145" t="s" s="20">
+      <c r="E160" t="s" s="14">
+        <v>195</v>
+      </c>
+      <c r="F160" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="161" ht="19" customHeight="1">
+      <c r="A161" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B161" s="37">
+        <v>7</v>
+      </c>
+      <c r="C161" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D161" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E161" t="s" s="14">
+        <v>196</v>
+      </c>
+      <c r="F161" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="162" ht="19" customHeight="1">
+      <c r="A162" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B162" s="19">
+        <v>7</v>
+      </c>
+      <c r="C162" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D145" t="s" s="16">
+      <c r="D162" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E145" t="s" s="15">
-        <v>179</v>
-      </c>
-      <c r="F145" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="146" ht="19" customHeight="1">
-      <c r="A146" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B146" s="22">
-        <v>7</v>
-      </c>
-      <c r="C146" t="s" s="23">
+      <c r="E162" t="s" s="15">
+        <v>197</v>
+      </c>
+      <c r="F162" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" ht="19" customHeight="1">
+      <c r="A163" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B163" s="22">
+        <v>7</v>
+      </c>
+      <c r="C163" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D146" t="s" s="16">
+      <c r="D163" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E146" t="s" s="14">
-        <v>180</v>
-      </c>
-      <c r="F146" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="147" ht="19" customHeight="1">
-      <c r="A147" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B147" s="25">
-        <v>7</v>
-      </c>
-      <c r="C147" t="s" s="26">
+      <c r="E163" t="s" s="14">
+        <v>198</v>
+      </c>
+      <c r="F163" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="164" ht="19" customHeight="1">
+      <c r="A164" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B164" s="25">
+        <v>7</v>
+      </c>
+      <c r="C164" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D147" t="s" s="16">
+      <c r="D164" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E147" t="s" s="14">
-        <v>181</v>
-      </c>
-      <c r="F147" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="148" ht="19" customHeight="1">
-      <c r="A148" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B148" s="28">
-        <v>7</v>
-      </c>
-      <c r="C148" t="s" s="29">
+      <c r="E164" t="s" s="14">
+        <v>199</v>
+      </c>
+      <c r="F164" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="165" ht="19" customHeight="1">
+      <c r="A165" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B165" s="28">
+        <v>7</v>
+      </c>
+      <c r="C165" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D148" t="s" s="16">
+      <c r="D165" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E148" t="s" s="14">
-        <v>182</v>
-      </c>
-      <c r="F148" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="149" ht="19" customHeight="1">
-      <c r="A149" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B149" s="31">
-        <v>7</v>
-      </c>
-      <c r="C149" t="s" s="32">
+      <c r="E165" t="s" s="14">
+        <v>200</v>
+      </c>
+      <c r="F165" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="166" ht="19" customHeight="1">
+      <c r="A166" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B166" s="31">
+        <v>7</v>
+      </c>
+      <c r="C166" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D149" t="s" s="16">
+      <c r="D166" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E149" t="s" s="14">
-        <v>183</v>
-      </c>
-      <c r="F149" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="150" ht="19" customHeight="1">
-      <c r="A150" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B150" s="34">
-        <v>7</v>
-      </c>
-      <c r="C150" t="s" s="35">
+      <c r="E166" t="s" s="14">
+        <v>201</v>
+      </c>
+      <c r="F166" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="167" ht="19" customHeight="1">
+      <c r="A167" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B167" s="34">
+        <v>7</v>
+      </c>
+      <c r="C167" t="s" s="35">
         <v>82</v>
       </c>
-      <c r="D150" t="s" s="16">
+      <c r="D167" t="s" s="16">
         <v>62</v>
       </c>
-      <c r="E150" t="s" s="14">
-        <v>184</v>
-      </c>
-      <c r="F150" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="151" ht="19" customHeight="1">
-      <c r="A151" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B151" s="19">
-        <v>7</v>
-      </c>
-      <c r="C151" t="s" s="20">
+      <c r="E167" t="s" s="14">
+        <v>202</v>
+      </c>
+      <c r="F167" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" ht="19" customHeight="1">
+      <c r="A168" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B168" s="37">
+        <v>7</v>
+      </c>
+      <c r="C168" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D168" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="E168" t="s" s="14">
+        <v>203</v>
+      </c>
+      <c r="F168" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="169" ht="19" customHeight="1">
+      <c r="A169" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B169" s="19">
+        <v>7</v>
+      </c>
+      <c r="C169" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D151" t="s" s="16">
+      <c r="D169" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E151" t="s" s="15">
-        <v>185</v>
-      </c>
-      <c r="F151" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="152" ht="19" customHeight="1">
-      <c r="A152" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B152" s="22">
-        <v>7</v>
-      </c>
-      <c r="C152" t="s" s="23">
+      <c r="E169" t="s" s="15">
+        <v>204</v>
+      </c>
+      <c r="F169" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="170" ht="19" customHeight="1">
+      <c r="A170" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B170" s="22">
+        <v>7</v>
+      </c>
+      <c r="C170" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D152" t="s" s="16">
+      <c r="D170" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E152" t="s" s="14">
-        <v>186</v>
-      </c>
-      <c r="F152" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="153" ht="19" customHeight="1">
-      <c r="A153" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B153" s="25">
-        <v>7</v>
-      </c>
-      <c r="C153" t="s" s="26">
+      <c r="E170" t="s" s="14">
+        <v>205</v>
+      </c>
+      <c r="F170" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="171" ht="19" customHeight="1">
+      <c r="A171" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B171" s="25">
+        <v>7</v>
+      </c>
+      <c r="C171" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D153" t="s" s="16">
+      <c r="D171" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E153" t="s" s="14">
-        <v>187</v>
-      </c>
-      <c r="F153" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="154" ht="19" customHeight="1">
-      <c r="A154" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B154" s="28">
-        <v>7</v>
-      </c>
-      <c r="C154" t="s" s="29">
+      <c r="E171" t="s" s="14">
+        <v>206</v>
+      </c>
+      <c r="F171" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="172" ht="19" customHeight="1">
+      <c r="A172" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B172" s="28">
+        <v>7</v>
+      </c>
+      <c r="C172" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D154" t="s" s="16">
+      <c r="D172" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E154" t="s" s="14">
-        <v>188</v>
-      </c>
-      <c r="F154" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="155" ht="19" customHeight="1">
-      <c r="A155" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B155" s="31">
-        <v>7</v>
-      </c>
-      <c r="C155" t="s" s="32">
+      <c r="E172" t="s" s="14">
+        <v>207</v>
+      </c>
+      <c r="F172" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="173" ht="19" customHeight="1">
+      <c r="A173" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B173" s="31">
+        <v>7</v>
+      </c>
+      <c r="C173" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D155" t="s" s="16">
+      <c r="D173" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E155" t="s" s="14">
-        <v>189</v>
-      </c>
-      <c r="F155" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="156" ht="19" customHeight="1">
-      <c r="A156" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B156" s="34">
-        <v>7</v>
-      </c>
-      <c r="C156" t="s" s="35">
+      <c r="E173" t="s" s="14">
+        <v>208</v>
+      </c>
+      <c r="F173" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="174" ht="19" customHeight="1">
+      <c r="A174" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B174" s="34">
+        <v>7</v>
+      </c>
+      <c r="C174" t="s" s="35">
         <v>82</v>
       </c>
-      <c r="D156" t="s" s="16">
+      <c r="D174" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="E156" t="s" s="14">
-        <v>190</v>
-      </c>
-      <c r="F156" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="157" ht="19" customHeight="1">
-      <c r="A157" t="s" s="18">
-        <v>71</v>
-      </c>
-      <c r="B157" s="19">
-        <v>7</v>
-      </c>
-      <c r="C157" t="s" s="20">
+      <c r="E174" t="s" s="14">
+        <v>209</v>
+      </c>
+      <c r="F174" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="175" ht="19" customHeight="1">
+      <c r="A175" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B175" s="37">
+        <v>7</v>
+      </c>
+      <c r="C175" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D175" t="s" s="16">
+        <v>65</v>
+      </c>
+      <c r="E175" t="s" s="14">
+        <v>210</v>
+      </c>
+      <c r="F175" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="176" ht="19" customHeight="1">
+      <c r="A176" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B176" s="19">
+        <v>7</v>
+      </c>
+      <c r="C176" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="D157" t="s" s="16">
+      <c r="D176" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E157" t="s" s="15">
-        <v>191</v>
-      </c>
-      <c r="F157" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="158" ht="19" customHeight="1">
-      <c r="A158" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B158" s="22">
-        <v>7</v>
-      </c>
-      <c r="C158" t="s" s="23">
+      <c r="E176" t="s" s="15">
+        <v>211</v>
+      </c>
+      <c r="F176" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="177" ht="19" customHeight="1">
+      <c r="A177" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="B177" s="22">
+        <v>7</v>
+      </c>
+      <c r="C177" t="s" s="23">
         <v>74</v>
       </c>
-      <c r="D158" t="s" s="16">
+      <c r="D177" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E158" t="s" s="14">
-        <v>192</v>
-      </c>
-      <c r="F158" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="159" ht="19" customHeight="1">
-      <c r="A159" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="B159" s="25">
-        <v>7</v>
-      </c>
-      <c r="C159" t="s" s="26">
+      <c r="E177" t="s" s="14">
+        <v>212</v>
+      </c>
+      <c r="F177" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="178" ht="19" customHeight="1">
+      <c r="A178" t="s" s="24">
+        <v>71</v>
+      </c>
+      <c r="B178" s="25">
+        <v>7</v>
+      </c>
+      <c r="C178" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="D159" t="s" s="16">
+      <c r="D178" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E159" t="s" s="14">
-        <v>193</v>
-      </c>
-      <c r="F159" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="160" ht="19" customHeight="1">
-      <c r="A160" t="s" s="27">
-        <v>71</v>
-      </c>
-      <c r="B160" s="28">
-        <v>7</v>
-      </c>
-      <c r="C160" t="s" s="29">
+      <c r="E178" t="s" s="14">
+        <v>213</v>
+      </c>
+      <c r="F178" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="179" ht="19" customHeight="1">
+      <c r="A179" t="s" s="27">
+        <v>71</v>
+      </c>
+      <c r="B179" s="28">
+        <v>7</v>
+      </c>
+      <c r="C179" t="s" s="29">
         <v>78</v>
       </c>
-      <c r="D160" t="s" s="16">
+      <c r="D179" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E160" t="s" s="14">
-        <v>194</v>
-      </c>
-      <c r="F160" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="161" ht="19" customHeight="1">
-      <c r="A161" t="s" s="30">
-        <v>71</v>
-      </c>
-      <c r="B161" s="31">
-        <v>7</v>
-      </c>
-      <c r="C161" t="s" s="32">
+      <c r="E179" t="s" s="14">
+        <v>214</v>
+      </c>
+      <c r="F179" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="180" ht="19" customHeight="1">
+      <c r="A180" t="s" s="30">
+        <v>71</v>
+      </c>
+      <c r="B180" s="31">
+        <v>7</v>
+      </c>
+      <c r="C180" t="s" s="32">
         <v>80</v>
       </c>
-      <c r="D161" t="s" s="16">
+      <c r="D180" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E161" t="s" s="14">
-        <v>195</v>
-      </c>
-      <c r="F161" t="s" s="15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="162" ht="19" customHeight="1">
-      <c r="A162" t="s" s="33">
-        <v>71</v>
-      </c>
-      <c r="B162" s="34">
-        <v>7</v>
-      </c>
-      <c r="C162" t="s" s="35">
+      <c r="E180" t="s" s="14">
+        <v>215</v>
+      </c>
+      <c r="F180" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="181" ht="19" customHeight="1">
+      <c r="A181" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="B181" s="34">
+        <v>7</v>
+      </c>
+      <c r="C181" t="s" s="35">
         <v>82</v>
       </c>
-      <c r="D162" t="s" s="16">
+      <c r="D181" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="E162" t="s" s="14">
-        <v>196</v>
-      </c>
-      <c r="F162" t="s" s="15">
+      <c r="E181" t="s" s="14">
+        <v>216</v>
+      </c>
+      <c r="F181" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="182" ht="19" customHeight="1">
+      <c r="A182" t="s" s="36">
+        <v>71</v>
+      </c>
+      <c r="B182" s="37">
+        <v>7</v>
+      </c>
+      <c r="C182" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="D182" t="s" s="16">
+        <v>68</v>
+      </c>
+      <c r="E182" t="s" s="14">
+        <v>217</v>
+      </c>
+      <c r="F182" t="s" s="15">
         <v>11</v>
       </c>
     </row>

</xml_diff>